<commit_message>
1.add expect value to selected.xlsx
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>code</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>remain</t>
+  </si>
+  <si>
+    <t>expval</t>
   </si>
   <si>
     <t>sz123160</t>
@@ -1627,14 +1630,15 @@
   <sheetPr/>
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C102"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="11.3727272727273" customWidth="1"/>
+    <col min="4" max="4" width="10.5454545454545" customWidth="1"/>
     <col min="9" max="9" width="11.6272727272727" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1648,7 +1652,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1658,1152 +1664,1455 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>3.35</v>
       </c>
+      <c r="D2" s="2">
+        <v>121.989910896765</v>
+      </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>3.4</v>
       </c>
+      <c r="D3" s="2">
+        <v>129.697793924965</v>
+      </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>5.84</v>
       </c>
+      <c r="D4" s="2">
+        <v>120.230719344356</v>
+      </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
         <v>2.94</v>
       </c>
+      <c r="D5" s="2">
+        <v>119.665806146018</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>2.485</v>
       </c>
+      <c r="D6" s="2">
+        <v>129.235977741638</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>3.2</v>
       </c>
+      <c r="D7" s="2">
+        <v>125.382118497519</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>2.217</v>
       </c>
+      <c r="D8" s="2">
+        <v>120.459292128776</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>3.912</v>
       </c>
+      <c r="D9" s="2">
+        <v>123.156114267543</v>
+      </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>4.993</v>
       </c>
+      <c r="D10" s="2">
+        <v>121.439957713431</v>
+      </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>6.346</v>
       </c>
+      <c r="D11" s="2">
+        <v>125.645147056752</v>
+      </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2">
         <v>5.496</v>
       </c>
+      <c r="D12" s="2">
+        <v>124.305054076071</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>4.596</v>
       </c>
+      <c r="D13" s="2">
+        <v>120.804903848194</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2">
         <v>3.746</v>
       </c>
+      <c r="D14" s="2">
+        <v>123.107727170317</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2">
         <v>2.188</v>
       </c>
+      <c r="D15" s="2">
+        <v>120.393953132973</v>
+      </c>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2">
         <v>2.496</v>
       </c>
+      <c r="D16" s="2">
+        <v>123.623554782845</v>
+      </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2">
         <v>3.781</v>
       </c>
+      <c r="D17" s="2">
+        <v>121.177221026604</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="2">
         <v>5.98</v>
       </c>
+      <c r="D18" s="2">
+        <v>114.364051053301</v>
+      </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>6</v>
       </c>
+      <c r="D19" s="2">
+        <v>117.96345785723</v>
+      </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2">
         <v>4.189</v>
       </c>
+      <c r="D20" s="2">
+        <v>120.912302756424</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2">
         <v>6.698</v>
       </c>
+      <c r="D21" s="2">
+        <v>114.878884940992</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2">
         <v>3.798</v>
       </c>
+      <c r="D22" s="2">
+        <v>117.199262416777</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2">
         <v>2.073</v>
       </c>
+      <c r="D23" s="2">
+        <v>120.508083398791</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2">
         <v>3.011</v>
       </c>
+      <c r="D24" s="2">
+        <v>121.162716989449</v>
+      </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2">
         <v>5.806</v>
       </c>
+      <c r="D25" s="2">
+        <v>120.081189000763</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2">
         <v>3.6</v>
       </c>
+      <c r="D26" s="2">
+        <v>121.66792732966</v>
+      </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2">
         <v>5.996</v>
       </c>
+      <c r="D27" s="2">
+        <v>115.123180283228</v>
+      </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2">
         <v>6.35</v>
       </c>
+      <c r="D28" s="2">
+        <v>121.82054305199</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2">
         <v>3.212</v>
       </c>
+      <c r="D29" s="2">
+        <v>121.855256265948</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2">
         <v>7</v>
       </c>
+      <c r="D30" s="2">
+        <v>121.801264282139</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2">
         <v>3.199</v>
       </c>
+      <c r="D31" s="2">
+        <v>121.250966284914</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C32" s="2">
         <v>4.946</v>
       </c>
+      <c r="D32" s="2">
+        <v>120.439026342324</v>
+      </c>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2">
         <v>2.4</v>
       </c>
+      <c r="D33" s="2">
+        <v>121.823233207769</v>
+      </c>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" s="2">
         <v>3.4</v>
       </c>
+      <c r="D34" s="2">
+        <v>121.625487586061</v>
+      </c>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C35" s="2">
         <v>4</v>
       </c>
+      <c r="D35" s="2">
+        <v>116.239442104632</v>
+      </c>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2">
         <v>5.228</v>
       </c>
+      <c r="D36" s="2">
+        <v>110.993718510803</v>
+      </c>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2">
         <v>4.596</v>
       </c>
+      <c r="D37" s="2">
+        <v>120.784281215055</v>
+      </c>
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2">
         <v>5.29</v>
       </c>
+      <c r="D38" s="2">
+        <v>120.398164905531</v>
+      </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2">
         <v>3.97</v>
       </c>
+      <c r="D39" s="2">
+        <v>121.395095285333</v>
+      </c>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C40" s="2">
         <v>4.199</v>
       </c>
+      <c r="D40" s="2">
+        <v>136.561881387139</v>
+      </c>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="2">
         <v>6.293</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="2">
+        <v>126.256827797916</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="2">
         <v>6.825</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="2">
+        <v>118.420485667135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="2">
         <v>2.996</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="2">
+        <v>121.29156295359</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2">
         <v>4.498</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="2">
+        <v>117.656972745387</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="2">
         <v>6.573</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="2">
+        <v>108.806196223492</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="2">
         <v>5.999</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="2">
+        <v>118.388170912385</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2">
         <v>3.631</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="2">
+        <v>113.524140591099</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="2">
+        <v>117.410954622583</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="2">
         <v>6.492</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="2">
+        <v>114.548452373091</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2">
         <v>2.993</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="2">
+        <v>118.342393709361</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2">
         <v>2.999</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="2">
+        <v>113.350002529279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C52" s="2">
         <v>3.018</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" s="2">
+        <v>113.55141763046</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C53" s="2">
         <v>4.611</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="2">
+        <v>115.503839879336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C54" s="2">
         <v>5.259</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="2">
+        <v>121.333868445679</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2">
         <v>3.199</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="2">
+        <v>115.054630258146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" s="2">
         <v>5.769</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" s="2">
+        <v>120.472067984248</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C57" s="2">
         <v>2.441</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" s="2">
+        <v>121.260528503978</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C58" s="2">
         <v>3.963</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" s="2">
+        <v>120.614418054437</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C59" s="2">
         <v>5.136</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="2">
+        <v>117.172571155337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60" s="2">
         <v>5.996</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60" s="2">
+        <v>114.635352739791</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C61" s="2">
         <v>5.156</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61" s="2">
+        <v>119.815745223765</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C62" s="2">
         <v>3.838</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62" s="2">
+        <v>117.569883216862</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C63" s="2">
         <v>5.426</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63" s="2">
+        <v>120.240051719881</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C64" s="2">
         <v>6.297</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64" s="2">
+        <v>120.121775493153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C65" s="2">
         <v>6.398</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65" s="2">
+        <v>117.190221183311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C66" s="2">
         <v>2.862</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66" s="2">
+        <v>118.600633960811</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C67" s="2">
         <v>6.449</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67" s="2">
+        <v>114.491392538292</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C68" s="2">
         <v>2.698</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68" s="2">
+        <v>123.727479773656</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C69" s="2">
         <v>4.996</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69" s="2">
+        <v>111.50802726058</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C70" s="2">
         <v>4.049</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70" s="2">
+        <v>121.447300012887</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C71" s="2">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71" s="2">
+        <v>121.404109754235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C72" s="2">
         <v>5.999</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72" s="2">
+        <v>120.984608342506</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C73" s="2">
         <v>6.961</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73" s="2">
+        <v>118.332516098165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C74" s="2">
         <v>3.998</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74" s="2">
+        <v>120.781330384156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C75" s="2">
         <v>4.579</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75" s="2">
+        <v>120.938110164478</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C76" s="2">
         <v>4.15</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76" s="2">
+        <v>121.474216090883</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C77" s="2">
         <v>6.027</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77" s="2">
+        <v>113.343905012089</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C78" s="2">
         <v>5.1</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78" s="2">
+        <v>115.359720949917</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C79" s="2">
         <v>2.983</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79" s="2">
+        <v>123.426274049671</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C80" s="2">
         <v>1.613</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="D80" s="2">
+        <v>123.304715164726</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C81" s="2">
         <v>2.997</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="D81" s="2">
+        <v>120.33641442544</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C82" s="2">
         <v>5.825</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82" s="2">
+        <v>123.815473958624</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C83" s="2">
         <v>2.297</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="D83" s="2">
+        <v>119.823463989325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C84" s="2">
         <v>2.089</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="D84" s="2">
+        <v>115.266340194479</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C85" s="2">
         <v>2.249</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="D85" s="2">
+        <v>117.030703376507</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C86" s="2">
         <v>2.171</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86" s="2">
+        <v>116.700977382144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C87" s="2">
         <v>4.775</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87" s="2">
+        <v>121.049724109707</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C88" s="2">
         <v>5.499</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88" s="2">
+        <v>113.327545443232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="D89" s="2">
+        <v>120.399448200669</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C90" s="2">
         <v>5.699</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="D90" s="2">
+        <v>112.557325807964</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C91" s="2">
         <v>5.999</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="D91" s="2">
+        <v>117.190911231469</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C92" s="2">
         <v>6.42</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92" s="2">
+        <v>129.094540919188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C93" s="2">
         <v>4.85</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="D93" s="2">
+        <v>118.625249125071</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C94" s="2">
         <v>4.65</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94" s="2">
+        <v>121.233484609976</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C95" s="2">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95" s="2">
+        <v>121.842307787216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C96" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96" s="2">
+        <v>121.520163542405</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C97" s="2">
         <v>4.1</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97" s="2">
+        <v>121.635998526793</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C98" s="2">
         <v>2.674</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="D98" s="2">
+        <v>120.680103700345</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C99" s="2">
         <v>3.874</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99" s="2">
+        <v>121.653164044284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C100" s="2">
         <v>4.4</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100" s="2">
+        <v>115.127671719834</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C101" s="2">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101" s="2">
+        <v>114.559256285896</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C102" s="2">
         <v>3.6</v>
+      </c>
+      <c r="D102" s="2">
+        <v>121.138096580978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add tab of revise
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>code</t>
   </si>
@@ -28,22 +28,190 @@
     <t>expval</t>
   </si>
   <si>
+    <t>sz123162</t>
+  </si>
+  <si>
+    <t>东杰转债</t>
+  </si>
+  <si>
+    <t>sz123163</t>
+  </si>
+  <si>
+    <t>金沃转债</t>
+  </si>
+  <si>
+    <t>sz123164</t>
+  </si>
+  <si>
+    <t>法本转债</t>
+  </si>
+  <si>
+    <t>sz123126</t>
+  </si>
+  <si>
+    <t>瑞丰转债</t>
+  </si>
+  <si>
+    <t>sz123056</t>
+  </si>
+  <si>
+    <t>雪榕转债</t>
+  </si>
+  <si>
+    <t>sz123039</t>
+  </si>
+  <si>
+    <t>开润转债</t>
+  </si>
+  <si>
+    <t>sz123106</t>
+  </si>
+  <si>
+    <t>正丹转债</t>
+  </si>
+  <si>
+    <t>sz123093</t>
+  </si>
+  <si>
+    <t>金陵转债</t>
+  </si>
+  <si>
+    <t>sz123063</t>
+  </si>
+  <si>
+    <t>大禹转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
+    <t>sz123050</t>
+  </si>
+  <si>
+    <t>聚飞转债</t>
+  </si>
+  <si>
+    <t>sz123065</t>
+  </si>
+  <si>
+    <t>宝莱转债</t>
+  </si>
+  <si>
+    <t>sz123129</t>
+  </si>
+  <si>
+    <t>锦鸡转债</t>
+  </si>
+  <si>
+    <t>sz123100</t>
+  </si>
+  <si>
+    <t>朗科转债</t>
+  </si>
+  <si>
+    <t>sz123116</t>
+  </si>
+  <si>
+    <t>万兴转债</t>
+  </si>
+  <si>
+    <t>sz123122</t>
+  </si>
+  <si>
+    <t>富瀚转债</t>
+  </si>
+  <si>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
+  </si>
+  <si>
+    <t>sz123088</t>
+  </si>
+  <si>
+    <t>威唐转债</t>
+  </si>
+  <si>
+    <t>sz123064</t>
+  </si>
+  <si>
+    <t>万孚转债</t>
+  </si>
+  <si>
+    <t>sz123131</t>
+  </si>
+  <si>
+    <t>奥飞转债</t>
+  </si>
+  <si>
+    <t>sz123154</t>
+  </si>
+  <si>
+    <t>火星转债</t>
+  </si>
+  <si>
+    <t>sz123101</t>
+  </si>
+  <si>
+    <t>拓斯转债</t>
+  </si>
+  <si>
+    <t>sz123136</t>
+  </si>
+  <si>
+    <t>城市转债</t>
+  </si>
+  <si>
+    <t>sz123153</t>
+  </si>
+  <si>
+    <t>英力转债</t>
+  </si>
+  <si>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>中陆转债</t>
+  </si>
+  <si>
+    <t>sz123138</t>
+  </si>
+  <si>
+    <t>丝路转债</t>
+  </si>
+  <si>
+    <t>sz123124</t>
+  </si>
+  <si>
+    <t>晶瑞转2</t>
+  </si>
+  <si>
+    <t>sz123132</t>
+  </si>
+  <si>
+    <t>回盛转债</t>
+  </si>
+  <si>
+    <t>sz123127</t>
+  </si>
+  <si>
+    <t>耐普转债</t>
+  </si>
+  <si>
     <t>sz123160</t>
   </si>
   <si>
     <t>泰福转债</t>
   </si>
   <si>
-    <t>sz123126</t>
-  </si>
-  <si>
-    <t>瑞丰转债</t>
-  </si>
-  <si>
-    <t>sz123056</t>
-  </si>
-  <si>
-    <t>雪榕转债</t>
+    <t>sz123144</t>
+  </si>
+  <si>
+    <t>裕兴转债</t>
   </si>
   <si>
     <t>sz123159</t>
@@ -52,210 +220,6 @@
     <t>崧盛转债</t>
   </si>
   <si>
-    <t>sz123093</t>
-  </si>
-  <si>
-    <t>金陵转债</t>
-  </si>
-  <si>
-    <t>sz123106</t>
-  </si>
-  <si>
-    <t>正丹转债</t>
-  </si>
-  <si>
-    <t>sz123039</t>
-  </si>
-  <si>
-    <t>开润转债</t>
-  </si>
-  <si>
-    <t>sz123059</t>
-  </si>
-  <si>
-    <t>银信转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
-  </si>
-  <si>
-    <t>sz123063</t>
-  </si>
-  <si>
-    <t>大禹转债</t>
-  </si>
-  <si>
-    <t>sz123044</t>
-  </si>
-  <si>
-    <t>红相转债</t>
-  </si>
-  <si>
-    <t>sz123109</t>
-  </si>
-  <si>
-    <t>昌红转债</t>
-  </si>
-  <si>
-    <t>sz123050</t>
-  </si>
-  <si>
-    <t>聚飞转债</t>
-  </si>
-  <si>
-    <t>sz123065</t>
-  </si>
-  <si>
-    <t>宝莱转债</t>
-  </si>
-  <si>
-    <t>sz123061</t>
-  </si>
-  <si>
-    <t>航新转债</t>
-  </si>
-  <si>
-    <t>sz123116</t>
-  </si>
-  <si>
-    <t>万兴转债</t>
-  </si>
-  <si>
-    <t>sz123064</t>
-  </si>
-  <si>
-    <t>万孚转债</t>
-  </si>
-  <si>
-    <t>sz123129</t>
-  </si>
-  <si>
-    <t>锦鸡转债</t>
-  </si>
-  <si>
-    <t>sz123087</t>
-  </si>
-  <si>
-    <t>明电转债</t>
-  </si>
-  <si>
-    <t>sz123101</t>
-  </si>
-  <si>
-    <t>拓斯转债</t>
-  </si>
-  <si>
-    <t>sz123100</t>
-  </si>
-  <si>
-    <t>朗科转债</t>
-  </si>
-  <si>
-    <t>sz123054</t>
-  </si>
-  <si>
-    <t>思特转债</t>
-  </si>
-  <si>
-    <t>sz123088</t>
-  </si>
-  <si>
-    <t>威唐转债</t>
-  </si>
-  <si>
-    <t>sz123122</t>
-  </si>
-  <si>
-    <t>富瀚转债</t>
-  </si>
-  <si>
-    <t>sz123155</t>
-  </si>
-  <si>
-    <t>中陆转债</t>
-  </si>
-  <si>
-    <t>sz123075</t>
-  </si>
-  <si>
-    <t>贝斯转债</t>
-  </si>
-  <si>
-    <t>sz123131</t>
-  </si>
-  <si>
-    <t>奥飞转债</t>
-  </si>
-  <si>
-    <t>sz123141</t>
-  </si>
-  <si>
-    <t>宏丰转债</t>
-  </si>
-  <si>
-    <t>sz123151</t>
-  </si>
-  <si>
-    <t>康医转债</t>
-  </si>
-  <si>
-    <t>sz123118</t>
-  </si>
-  <si>
-    <t>惠城转债</t>
-  </si>
-  <si>
-    <t>sz123157</t>
-  </si>
-  <si>
-    <t>科蓝转债</t>
-  </si>
-  <si>
-    <t>sz123138</t>
-  </si>
-  <si>
-    <t>丝路转债</t>
-  </si>
-  <si>
-    <t>sz123153</t>
-  </si>
-  <si>
-    <t>英力转债</t>
-  </si>
-  <si>
-    <t>sz123127</t>
-  </si>
-  <si>
-    <t>耐普转债</t>
-  </si>
-  <si>
-    <t>sz123124</t>
-  </si>
-  <si>
-    <t>晶瑞转2</t>
-  </si>
-  <si>
-    <t>sz123136</t>
-  </si>
-  <si>
-    <t>城市转债</t>
-  </si>
-  <si>
-    <t>sz123154</t>
-  </si>
-  <si>
-    <t>火星转债</t>
-  </si>
-  <si>
-    <t>sz123156</t>
-  </si>
-  <si>
-    <t>博汇转债</t>
-  </si>
-  <si>
     <t>sz128138</t>
   </si>
   <si>
@@ -280,16 +244,28 @@
     <t>瀛通转债</t>
   </si>
   <si>
+    <t>sz128044</t>
+  </si>
+  <si>
+    <t>岭南转债</t>
+  </si>
+  <si>
     <t>sz128125</t>
   </si>
   <si>
     <t>华阳转债</t>
   </si>
   <si>
-    <t>sz128044</t>
-  </si>
-  <si>
-    <t>岭南转债</t>
+    <t>sz128072</t>
+  </si>
+  <si>
+    <t>翔鹭转债</t>
+  </si>
+  <si>
+    <t>sz127072</t>
+  </si>
+  <si>
+    <t>博实转债</t>
   </si>
   <si>
     <t>sz127041</t>
@@ -298,28 +274,22 @@
     <t>弘亚转债</t>
   </si>
   <si>
+    <t>sz128116</t>
+  </si>
+  <si>
+    <t>瑞达转债</t>
+  </si>
+  <si>
     <t>sz128049</t>
   </si>
   <si>
     <t>华源转债</t>
   </si>
   <si>
-    <t>sz127072</t>
-  </si>
-  <si>
-    <t>博实转债</t>
-  </si>
-  <si>
-    <t>sz128116</t>
-  </si>
-  <si>
-    <t>瑞达转债</t>
-  </si>
-  <si>
-    <t>sz128069</t>
-  </si>
-  <si>
-    <t>华森转债</t>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
   </si>
   <si>
     <t>sz128071</t>
@@ -328,34 +298,28 @@
     <t>合兴转债</t>
   </si>
   <si>
-    <t>sz128072</t>
-  </si>
-  <si>
-    <t>翔鹭转债</t>
-  </si>
-  <si>
-    <t>sz128066</t>
-  </si>
-  <si>
-    <t>亚泰转债</t>
-  </si>
-  <si>
     <t>sz127051</t>
   </si>
   <si>
     <t>博杰转债</t>
   </si>
   <si>
+    <t>sz127055</t>
+  </si>
+  <si>
+    <t>精装转债</t>
+  </si>
+  <si>
     <t>sz128123</t>
   </si>
   <si>
     <t>国光转债</t>
   </si>
   <si>
-    <t>sz127055</t>
-  </si>
-  <si>
-    <t>精装转债</t>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>奥佳转债</t>
   </si>
   <si>
     <t>sz128143</t>
@@ -400,60 +364,54 @@
     <t>塞力转债</t>
   </si>
   <si>
+    <t>sh113584</t>
+  </si>
+  <si>
+    <t>家悦转债</t>
+  </si>
+  <si>
     <t>sh113530</t>
   </si>
   <si>
     <t>大丰转债</t>
   </si>
   <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <t>纵横转债</t>
+  </si>
+  <si>
+    <t>sh113606</t>
+  </si>
+  <si>
+    <t>荣泰转债</t>
+  </si>
+  <si>
     <t>sh113604</t>
   </si>
   <si>
     <t>多伦转债</t>
   </si>
   <si>
+    <t>sh113624</t>
+  </si>
+  <si>
+    <t>正川转债</t>
+  </si>
+  <si>
     <t>sh113527</t>
   </si>
   <si>
     <t>维格转债</t>
   </si>
   <si>
-    <t>sh113584</t>
-  </si>
-  <si>
-    <t>家悦转债</t>
-  </si>
-  <si>
-    <t>sh113573</t>
-  </si>
-  <si>
-    <t>纵横转债</t>
-  </si>
-  <si>
-    <t>sh113535</t>
-  </si>
-  <si>
-    <t>大业转债</t>
-  </si>
-  <si>
-    <t>sh113624</t>
-  </si>
-  <si>
-    <t>正川转债</t>
-  </si>
-  <si>
-    <t>sh113608</t>
-  </si>
-  <si>
-    <t>威派转债</t>
-  </si>
-  <si>
-    <t>sh113606</t>
-  </si>
-  <si>
-    <t>荣泰转债</t>
-  </si>
-  <si>
     <t>sh113519</t>
   </si>
   <si>
@@ -466,12 +424,30 @@
     <t>沪工转债</t>
   </si>
   <si>
+    <t>sh113625</t>
+  </si>
+  <si>
+    <t>江山转债</t>
+  </si>
+  <si>
+    <t>sh113524</t>
+  </si>
+  <si>
+    <t>奇精转债</t>
+  </si>
+  <si>
     <t>sh113610</t>
   </si>
   <si>
     <t>灵康转债</t>
   </si>
   <si>
+    <t>sh113566</t>
+  </si>
+  <si>
+    <t>翔港转债</t>
+  </si>
+  <si>
     <t>sh113628</t>
   </si>
   <si>
@@ -484,36 +460,18 @@
     <t>好客转债</t>
   </si>
   <si>
-    <t>sh113657</t>
-  </si>
-  <si>
-    <t>再22转债</t>
-  </si>
-  <si>
     <t>sh113597</t>
   </si>
   <si>
     <t>佳力转债</t>
   </si>
   <si>
-    <t>sh113566</t>
-  </si>
-  <si>
-    <t>翔港转债</t>
-  </si>
-  <si>
     <t>sh113594</t>
   </si>
   <si>
     <t>淳中转债</t>
   </si>
   <si>
-    <t>sh113625</t>
-  </si>
-  <si>
-    <t>江山转债</t>
-  </si>
-  <si>
     <t>sh113546</t>
   </si>
   <si>
@@ -526,30 +484,12 @@
     <t>华体转债</t>
   </si>
   <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
-  </si>
-  <si>
     <t>sh110070</t>
   </si>
   <si>
     <t>凌钢转债</t>
   </si>
   <si>
-    <t>sh113591</t>
-  </si>
-  <si>
-    <t>胜达转债</t>
-  </si>
-  <si>
-    <t>sh113588</t>
-  </si>
-  <si>
-    <t>润达转债</t>
-  </si>
-  <si>
     <t>sh113643</t>
   </si>
   <si>
@@ -586,6 +526,12 @@
     <t>博瑞转债</t>
   </si>
   <si>
+    <t>sh118015</t>
+  </si>
+  <si>
+    <t>芯海转债</t>
+  </si>
+  <si>
     <t>sh118016</t>
   </si>
   <si>
@@ -596,42 +542,6 @@
   </si>
   <si>
     <t>银微转债</t>
-  </si>
-  <si>
-    <t>sh118015</t>
-  </si>
-  <si>
-    <t>芯海转债</t>
-  </si>
-  <si>
-    <t>sh118007</t>
-  </si>
-  <si>
-    <t>山石转债</t>
-  </si>
-  <si>
-    <t>sh118006</t>
-  </si>
-  <si>
-    <t>阿拉转债</t>
-  </si>
-  <si>
-    <t>sh118010</t>
-  </si>
-  <si>
-    <t>洁特转债</t>
-  </si>
-  <si>
-    <t>sh118018</t>
-  </si>
-  <si>
-    <t>瑞科转债</t>
-  </si>
-  <si>
-    <t>sh118017</t>
-  </si>
-  <si>
-    <t>深科转债</t>
   </si>
 </sst>
 </file>
@@ -1273,13 +1183,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1628,10 +1539,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1670,11 +1581,12 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>3.35</v>
+        <v>5.7</v>
       </c>
       <c r="D2" s="2">
-        <v>121.989910896765</v>
-      </c>
+        <v>122.208506713255</v>
+      </c>
+      <c r="E2" s="2"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9">
@@ -1685,11 +1597,12 @@
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="D3" s="2">
-        <v>129.697793924965</v>
-      </c>
+        <v>122.208506713255</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9">
@@ -1700,11 +1613,12 @@
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>5.84</v>
+        <v>6.01</v>
       </c>
       <c r="D4" s="2">
-        <v>120.230719344356</v>
-      </c>
+        <v>122.007964736343</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9">
@@ -1715,11 +1629,12 @@
         <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>2.94</v>
+        <v>3.4</v>
       </c>
       <c r="D5" s="2">
-        <v>119.665806146018</v>
-      </c>
+        <v>129.702239129399</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9">
@@ -1730,11 +1645,12 @@
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>2.485</v>
+        <v>5.84</v>
       </c>
       <c r="D6" s="2">
-        <v>129.235977741638</v>
-      </c>
+        <v>120.22392895889</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
@@ -1745,11 +1661,12 @@
         <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>3.2</v>
+        <v>2.217</v>
       </c>
       <c r="D7" s="2">
-        <v>125.382118497519</v>
-      </c>
+        <v>120.434723971996</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
@@ -1760,11 +1677,12 @@
         <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>2.217</v>
+        <v>3.2</v>
       </c>
       <c r="D8" s="2">
-        <v>120.459292128776</v>
-      </c>
+        <v>125.331277626309</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
@@ -1775,11 +1693,12 @@
         <v>19</v>
       </c>
       <c r="C9" s="2">
-        <v>3.912</v>
+        <v>2.485</v>
       </c>
       <c r="D9" s="2">
-        <v>123.156114267543</v>
-      </c>
+        <v>129.161402712328</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9">
@@ -1790,11 +1709,12 @@
         <v>21</v>
       </c>
       <c r="C10" s="2">
-        <v>4.993</v>
+        <v>6.346</v>
       </c>
       <c r="D10" s="2">
-        <v>121.439957713431</v>
-      </c>
+        <v>125.64457412544</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9">
@@ -1805,11 +1725,12 @@
         <v>23</v>
       </c>
       <c r="C11" s="2">
-        <v>6.346</v>
+        <v>4.993</v>
       </c>
       <c r="D11" s="2">
-        <v>125.645147056752</v>
-      </c>
+        <v>121.365154902833</v>
+      </c>
+      <c r="E11" s="2"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9">
@@ -1820,11 +1741,12 @@
         <v>25</v>
       </c>
       <c r="C12" s="2">
-        <v>5.496</v>
+        <v>3.746</v>
       </c>
       <c r="D12" s="2">
-        <v>124.305054076071</v>
-      </c>
+        <v>123.082471733304</v>
+      </c>
+      <c r="E12" s="2"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9">
@@ -1835,11 +1757,12 @@
         <v>27</v>
       </c>
       <c r="C13" s="2">
-        <v>4.596</v>
+        <v>2.188</v>
       </c>
       <c r="D13" s="2">
-        <v>120.804903848194</v>
-      </c>
+        <v>120.414323992965</v>
+      </c>
+      <c r="E13" s="2"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9">
@@ -1850,11 +1773,12 @@
         <v>29</v>
       </c>
       <c r="C14" s="2">
-        <v>3.746</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>123.107727170317</v>
-      </c>
+        <v>117.952975594569</v>
+      </c>
+      <c r="E14" s="2"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9">
@@ -1865,11 +1789,12 @@
         <v>31</v>
       </c>
       <c r="C15" s="2">
-        <v>2.188</v>
+        <v>3.797</v>
       </c>
       <c r="D15" s="2">
-        <v>120.393953132973</v>
-      </c>
+        <v>117.166171308751</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9">
@@ -1880,11 +1805,12 @@
         <v>33</v>
       </c>
       <c r="C16" s="2">
-        <v>2.496</v>
+        <v>3.781</v>
       </c>
       <c r="D16" s="2">
-        <v>123.623554782845</v>
-      </c>
+        <v>121.108095832548</v>
+      </c>
+      <c r="E16" s="2"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
@@ -1895,11 +1821,12 @@
         <v>35</v>
       </c>
       <c r="C17" s="2">
-        <v>3.781</v>
+        <v>5.806</v>
       </c>
       <c r="D17" s="2">
-        <v>121.177221026604</v>
-      </c>
+        <v>120.093744502809</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9">
@@ -1910,11 +1837,12 @@
         <v>37</v>
       </c>
       <c r="C18" s="2">
-        <v>5.98</v>
+        <v>4.596</v>
       </c>
       <c r="D18" s="2">
-        <v>114.364051053301</v>
-      </c>
+        <v>120.68213594129</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9">
@@ -1925,11 +1853,12 @@
         <v>39</v>
       </c>
       <c r="C19" s="2">
-        <v>6</v>
+        <v>3.011</v>
       </c>
       <c r="D19" s="2">
-        <v>117.96345785723</v>
-      </c>
+        <v>121.136250751311</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9">
@@ -1940,11 +1869,12 @@
         <v>41</v>
       </c>
       <c r="C20" s="2">
-        <v>4.189</v>
+        <v>5.98</v>
       </c>
       <c r="D20" s="2">
-        <v>120.912302756424</v>
-      </c>
+        <v>114.300817872756</v>
+      </c>
+      <c r="E20" s="2"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
@@ -1955,11 +1885,12 @@
         <v>43</v>
       </c>
       <c r="C21" s="2">
-        <v>6.698</v>
+        <v>6.35</v>
       </c>
       <c r="D21" s="2">
-        <v>114.878884940992</v>
-      </c>
+        <v>121.821173633168</v>
+      </c>
+      <c r="E21" s="2"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -1970,11 +1901,12 @@
         <v>45</v>
       </c>
       <c r="C22" s="2">
-        <v>3.798</v>
+        <v>5.29</v>
       </c>
       <c r="D22" s="2">
-        <v>117.199262416777</v>
-      </c>
+        <v>120.442238450499</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9">
@@ -1985,11 +1917,12 @@
         <v>47</v>
       </c>
       <c r="C23" s="2">
-        <v>2.073</v>
+        <v>6.698</v>
       </c>
       <c r="D23" s="2">
-        <v>120.508083398791</v>
-      </c>
+        <v>114.800180393216</v>
+      </c>
+      <c r="E23" s="2"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9">
@@ -2000,11 +1933,12 @@
         <v>49</v>
       </c>
       <c r="C24" s="2">
-        <v>3.011</v>
+        <v>4.595</v>
       </c>
       <c r="D24" s="2">
-        <v>121.162716989449</v>
-      </c>
+        <v>120.780465188271</v>
+      </c>
+      <c r="E24" s="2"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9">
@@ -2015,11 +1949,12 @@
         <v>51</v>
       </c>
       <c r="C25" s="2">
-        <v>5.806</v>
+        <v>3.4</v>
       </c>
       <c r="D25" s="2">
-        <v>120.081189000763</v>
-      </c>
+        <v>121.62827146443</v>
+      </c>
+      <c r="E25" s="2"/>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9">
@@ -2033,8 +1968,9 @@
         <v>3.6</v>
       </c>
       <c r="D26" s="2">
-        <v>121.66792732966</v>
-      </c>
+        <v>121.615576757967</v>
+      </c>
+      <c r="E26" s="2"/>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9">
@@ -2045,11 +1981,12 @@
         <v>55</v>
       </c>
       <c r="C27" s="2">
-        <v>5.996</v>
+        <v>2.4</v>
       </c>
       <c r="D27" s="2">
-        <v>115.123180283228</v>
-      </c>
+        <v>121.775942514343</v>
+      </c>
+      <c r="E27" s="2"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9">
@@ -2060,11 +1997,12 @@
         <v>57</v>
       </c>
       <c r="C28" s="2">
-        <v>6.35</v>
+        <v>5.228</v>
       </c>
       <c r="D28" s="2">
-        <v>121.82054305199</v>
-      </c>
+        <v>110.998297016948</v>
+      </c>
+      <c r="E28" s="2"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9">
@@ -2075,11 +2013,12 @@
         <v>59</v>
       </c>
       <c r="C29" s="2">
-        <v>3.212</v>
+        <v>7</v>
       </c>
       <c r="D29" s="2">
-        <v>121.855256265948</v>
-      </c>
+        <v>121.007400182369</v>
+      </c>
+      <c r="E29" s="2"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9">
@@ -2090,11 +2029,12 @@
         <v>61</v>
       </c>
       <c r="C30" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2">
-        <v>121.801264282139</v>
-      </c>
+        <v>116.231416088774</v>
+      </c>
+      <c r="E30" s="2"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
@@ -2105,11 +2045,12 @@
         <v>63</v>
       </c>
       <c r="C31" s="2">
-        <v>3.199</v>
+        <v>3.349</v>
       </c>
       <c r="D31" s="2">
-        <v>121.250966284914</v>
-      </c>
+        <v>121.59590373631</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9">
@@ -2120,11 +2061,12 @@
         <v>65</v>
       </c>
       <c r="C32" s="2">
-        <v>4.946</v>
+        <v>6</v>
       </c>
       <c r="D32" s="2">
-        <v>120.439026342324</v>
-      </c>
+        <v>120.327845186873</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9">
@@ -2135,11 +2077,12 @@
         <v>67</v>
       </c>
       <c r="C33" s="2">
-        <v>2.4</v>
+        <v>2.94</v>
       </c>
       <c r="D33" s="2">
-        <v>121.823233207769</v>
-      </c>
+        <v>119.315741352218</v>
+      </c>
+      <c r="E33" s="2"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9">
@@ -2150,11 +2093,12 @@
         <v>69</v>
       </c>
       <c r="C34" s="2">
-        <v>3.4</v>
+        <v>4.199</v>
       </c>
       <c r="D34" s="2">
-        <v>121.625487586061</v>
-      </c>
+        <v>136.546581422295</v>
+      </c>
+      <c r="E34" s="2"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9">
@@ -2165,11 +2109,12 @@
         <v>71</v>
       </c>
       <c r="C35" s="2">
-        <v>4</v>
+        <v>6.292</v>
       </c>
       <c r="D35" s="2">
-        <v>116.239442104632</v>
-      </c>
+        <v>126.235249764146</v>
+      </c>
+      <c r="E35" s="2"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9">
@@ -2180,11 +2125,12 @@
         <v>73</v>
       </c>
       <c r="C36" s="2">
-        <v>5.228</v>
+        <v>6.825</v>
       </c>
       <c r="D36" s="2">
-        <v>110.993718510803</v>
-      </c>
+        <v>118.444703028016</v>
+      </c>
+      <c r="E36" s="2"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9">
@@ -2195,11 +2141,12 @@
         <v>75</v>
       </c>
       <c r="C37" s="2">
-        <v>4.596</v>
+        <v>2.996</v>
       </c>
       <c r="D37" s="2">
-        <v>120.784281215055</v>
-      </c>
+        <v>121.263033639477</v>
+      </c>
+      <c r="E37" s="2"/>
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9">
@@ -2210,11 +2157,12 @@
         <v>77</v>
       </c>
       <c r="C38" s="2">
-        <v>5.29</v>
+        <v>6.573</v>
       </c>
       <c r="D38" s="2">
-        <v>120.398164905531</v>
-      </c>
+        <v>108.811031957239</v>
+      </c>
+      <c r="E38" s="2"/>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9">
@@ -2225,11 +2173,12 @@
         <v>79</v>
       </c>
       <c r="C39" s="2">
-        <v>3.97</v>
+        <v>4.498</v>
       </c>
       <c r="D39" s="2">
-        <v>121.395095285333</v>
-      </c>
+        <v>117.703269961079</v>
+      </c>
+      <c r="E39" s="2"/>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9">
@@ -2240,14 +2189,15 @@
         <v>81</v>
       </c>
       <c r="C40" s="2">
-        <v>4.199</v>
+        <v>3.017</v>
       </c>
       <c r="D40" s="2">
-        <v>136.561881387139</v>
-      </c>
+        <v>113.574001079056</v>
+      </c>
+      <c r="E40" s="2"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>82</v>
       </c>
@@ -2255,13 +2205,14 @@
         <v>83</v>
       </c>
       <c r="C41" s="2">
-        <v>6.293</v>
+        <v>4.5</v>
       </c>
       <c r="D41" s="2">
-        <v>126.256827797916</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>117.438220088514</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
@@ -2269,13 +2220,14 @@
         <v>85</v>
       </c>
       <c r="C42" s="2">
-        <v>6.825</v>
+        <v>5.999</v>
       </c>
       <c r="D42" s="2">
-        <v>118.420485667135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>118.349959793004</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2283,13 +2235,14 @@
         <v>87</v>
       </c>
       <c r="C43" s="2">
-        <v>2.996</v>
+        <v>6.491</v>
       </c>
       <c r="D43" s="2">
-        <v>121.29156295359</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>114.573722649771</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
         <v>88</v>
       </c>
@@ -2297,13 +2250,14 @@
         <v>89</v>
       </c>
       <c r="C44" s="2">
-        <v>4.498</v>
+        <v>3.631</v>
       </c>
       <c r="D44" s="2">
-        <v>117.656972745387</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>113.513749312878</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
@@ -2311,13 +2265,14 @@
         <v>91</v>
       </c>
       <c r="C45" s="2">
-        <v>6.573</v>
+        <v>3.586</v>
       </c>
       <c r="D45" s="2">
-        <v>108.806196223492</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>122.653015068136</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -2325,13 +2280,14 @@
         <v>93</v>
       </c>
       <c r="C46" s="2">
-        <v>5.999</v>
+        <v>2.999</v>
       </c>
       <c r="D46" s="2">
-        <v>118.388170912385</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>113.311118500451</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
         <v>94</v>
       </c>
@@ -2339,13 +2295,14 @@
         <v>95</v>
       </c>
       <c r="C47" s="2">
-        <v>3.631</v>
+        <v>5.259</v>
       </c>
       <c r="D47" s="2">
-        <v>113.524140591099</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>121.354820651447</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
         <v>96</v>
       </c>
@@ -2353,13 +2310,14 @@
         <v>97</v>
       </c>
       <c r="C48" s="2">
-        <v>4.5</v>
+        <v>5.769</v>
       </c>
       <c r="D48" s="2">
-        <v>117.410954622583</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>120.492760104019</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
         <v>98</v>
       </c>
@@ -2367,13 +2325,14 @@
         <v>99</v>
       </c>
       <c r="C49" s="2">
-        <v>6.492</v>
+        <v>3.199</v>
       </c>
       <c r="D49" s="2">
-        <v>114.548452373091</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>115.098549806292</v>
+      </c>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
         <v>100</v>
       </c>
@@ -2381,13 +2340,14 @@
         <v>101</v>
       </c>
       <c r="C50" s="2">
-        <v>2.993</v>
+        <v>4.585</v>
       </c>
       <c r="D50" s="2">
-        <v>118.342393709361</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>114.318001983785</v>
+      </c>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
         <v>102</v>
       </c>
@@ -2395,13 +2355,14 @@
         <v>103</v>
       </c>
       <c r="C51" s="2">
-        <v>2.999</v>
+        <v>2.441</v>
       </c>
       <c r="D51" s="2">
-        <v>113.350002529279</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>121.235693680051</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -2409,13 +2370,14 @@
         <v>105</v>
       </c>
       <c r="C52" s="2">
-        <v>3.018</v>
+        <v>3.963</v>
       </c>
       <c r="D52" s="2">
-        <v>113.55141763046</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>120.603603981709</v>
+      </c>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
         <v>106</v>
       </c>
@@ -2423,13 +2385,14 @@
         <v>107</v>
       </c>
       <c r="C53" s="2">
-        <v>4.611</v>
+        <v>5.136</v>
       </c>
       <c r="D53" s="2">
-        <v>115.503839879336</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>117.196362097403</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
@@ -2437,13 +2400,14 @@
         <v>109</v>
       </c>
       <c r="C54" s="2">
-        <v>5.259</v>
+        <v>5.996</v>
       </c>
       <c r="D54" s="2">
-        <v>121.333868445679</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>114.664231299416</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -2451,13 +2415,14 @@
         <v>111</v>
       </c>
       <c r="C55" s="2">
-        <v>3.199</v>
+        <v>5.156</v>
       </c>
       <c r="D55" s="2">
-        <v>115.054630258146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>119.825752008331</v>
+      </c>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -2465,13 +2430,14 @@
         <v>113</v>
       </c>
       <c r="C56" s="2">
-        <v>5.769</v>
+        <v>3.838</v>
       </c>
       <c r="D56" s="2">
-        <v>120.472067984248</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>117.615998826295</v>
+      </c>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
         <v>114</v>
       </c>
@@ -2479,13 +2445,14 @@
         <v>115</v>
       </c>
       <c r="C57" s="2">
-        <v>2.441</v>
+        <v>5.426</v>
       </c>
       <c r="D57" s="2">
-        <v>121.260528503978</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>120.235706557985</v>
+      </c>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
         <v>116</v>
       </c>
@@ -2493,13 +2460,14 @@
         <v>117</v>
       </c>
       <c r="C58" s="2">
-        <v>3.963</v>
+        <v>6.449</v>
       </c>
       <c r="D58" s="2">
-        <v>120.614418054437</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>114.490889112864</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
         <v>118</v>
       </c>
@@ -2507,13 +2475,14 @@
         <v>119</v>
       </c>
       <c r="C59" s="2">
-        <v>5.136</v>
+        <v>6.297</v>
       </c>
       <c r="D59" s="2">
-        <v>117.172571155337</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>120.09031254892</v>
+      </c>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
         <v>120</v>
       </c>
@@ -2521,13 +2490,14 @@
         <v>121</v>
       </c>
       <c r="C60" s="2">
-        <v>5.996</v>
+        <v>4.2</v>
       </c>
       <c r="D60" s="2">
-        <v>114.635352739791</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>121.424831504075</v>
+      </c>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
         <v>122</v>
       </c>
@@ -2535,13 +2505,14 @@
         <v>123</v>
       </c>
       <c r="C61" s="2">
-        <v>5.156</v>
+        <v>2.698</v>
       </c>
       <c r="D61" s="2">
-        <v>119.815745223765</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>123.723340003003</v>
+      </c>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
         <v>124</v>
       </c>
@@ -2549,13 +2520,14 @@
         <v>125</v>
       </c>
       <c r="C62" s="2">
-        <v>3.838</v>
+        <v>5.999</v>
       </c>
       <c r="D62" s="2">
-        <v>117.569883216862</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>120.971635900368</v>
+      </c>
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
         <v>126</v>
       </c>
@@ -2563,13 +2535,14 @@
         <v>127</v>
       </c>
       <c r="C63" s="2">
-        <v>5.426</v>
+        <v>6.398</v>
       </c>
       <c r="D63" s="2">
-        <v>120.240051719881</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>116.486541938491</v>
+      </c>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
         <v>128</v>
       </c>
@@ -2577,13 +2550,14 @@
         <v>129</v>
       </c>
       <c r="C64" s="2">
-        <v>6.297</v>
+        <v>4.049</v>
       </c>
       <c r="D64" s="2">
-        <v>120.121775493153</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>121.418319682284</v>
+      </c>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
         <v>130</v>
       </c>
@@ -2591,13 +2565,14 @@
         <v>131</v>
       </c>
       <c r="C65" s="2">
-        <v>6.398</v>
+        <v>2.862</v>
       </c>
       <c r="D65" s="2">
-        <v>117.190221183311</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>118.56093154333</v>
+      </c>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
         <v>132</v>
       </c>
@@ -2605,13 +2580,14 @@
         <v>133</v>
       </c>
       <c r="C66" s="2">
-        <v>2.862</v>
+        <v>6.961</v>
       </c>
       <c r="D66" s="2">
-        <v>118.600633960811</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>118.332313457061</v>
+      </c>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="2" t="s">
         <v>134</v>
       </c>
@@ -2619,13 +2595,14 @@
         <v>135</v>
       </c>
       <c r="C67" s="2">
-        <v>6.449</v>
+        <v>3.998</v>
       </c>
       <c r="D67" s="2">
-        <v>114.491392538292</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>120.786324887702</v>
+      </c>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
         <v>136</v>
       </c>
@@ -2633,13 +2610,14 @@
         <v>137</v>
       </c>
       <c r="C68" s="2">
-        <v>2.698</v>
+        <v>5.825</v>
       </c>
       <c r="D68" s="2">
-        <v>123.727479773656</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>123.839191765186</v>
+      </c>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
         <v>138</v>
       </c>
@@ -2647,13 +2625,14 @@
         <v>139</v>
       </c>
       <c r="C69" s="2">
-        <v>4.996</v>
+        <v>3.297</v>
       </c>
       <c r="D69" s="2">
-        <v>111.50802726058</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>116.327549939574</v>
+      </c>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
         <v>140</v>
       </c>
@@ -2661,13 +2640,14 @@
         <v>141</v>
       </c>
       <c r="C70" s="2">
-        <v>4.049</v>
+        <v>4.579</v>
       </c>
       <c r="D70" s="2">
-        <v>121.447300012887</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>120.931508243259</v>
+      </c>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="2" t="s">
         <v>142</v>
       </c>
@@ -2675,13 +2655,14 @@
         <v>143</v>
       </c>
       <c r="C71" s="2">
-        <v>4.2</v>
+        <v>1.613</v>
       </c>
       <c r="D71" s="2">
-        <v>121.404109754235</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>123.318716824373</v>
+      </c>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="2" t="s">
         <v>144</v>
       </c>
@@ -2689,13 +2670,14 @@
         <v>145</v>
       </c>
       <c r="C72" s="2">
-        <v>5.999</v>
+        <v>4.15</v>
       </c>
       <c r="D72" s="2">
-        <v>120.984608342506</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>121.475216909532</v>
+      </c>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="2" t="s">
         <v>146</v>
       </c>
@@ -2703,13 +2685,14 @@
         <v>147</v>
       </c>
       <c r="C73" s="2">
-        <v>6.961</v>
+        <v>6.026</v>
       </c>
       <c r="D73" s="2">
-        <v>118.332516098165</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>113.338950056051</v>
+      </c>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="2" t="s">
         <v>148</v>
       </c>
@@ -2717,13 +2700,14 @@
         <v>149</v>
       </c>
       <c r="C74" s="2">
-        <v>3.998</v>
+        <v>2.983</v>
       </c>
       <c r="D74" s="2">
-        <v>120.781330384156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>123.42378156679</v>
+      </c>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="2" t="s">
         <v>150</v>
       </c>
@@ -2731,13 +2715,14 @@
         <v>151</v>
       </c>
       <c r="C75" s="2">
-        <v>4.579</v>
+        <v>2.997</v>
       </c>
       <c r="D75" s="2">
-        <v>120.938110164478</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>120.295083818005</v>
+      </c>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="2" t="s">
         <v>152</v>
       </c>
@@ -2745,13 +2730,14 @@
         <v>153</v>
       </c>
       <c r="C76" s="2">
-        <v>4.15</v>
+        <v>2.297</v>
       </c>
       <c r="D76" s="2">
-        <v>121.474216090883</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>118.607551999917</v>
+      </c>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="2" t="s">
         <v>154</v>
       </c>
@@ -2759,13 +2745,14 @@
         <v>155</v>
       </c>
       <c r="C77" s="2">
-        <v>6.027</v>
+        <v>2.089</v>
       </c>
       <c r="D77" s="2">
-        <v>113.343905012089</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>115.252727442144</v>
+      </c>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="2" t="s">
         <v>156</v>
       </c>
@@ -2773,13 +2760,14 @@
         <v>157</v>
       </c>
       <c r="C78" s="2">
-        <v>5.1</v>
+        <v>2.171</v>
       </c>
       <c r="D78" s="2">
-        <v>115.359720949917</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>116.732001990274</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
         <v>158</v>
       </c>
@@ -2787,13 +2775,14 @@
         <v>159</v>
       </c>
       <c r="C79" s="2">
-        <v>2.983</v>
+        <v>5</v>
       </c>
       <c r="D79" s="2">
-        <v>123.426274049671</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>120.445640203504</v>
+      </c>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
         <v>160</v>
       </c>
@@ -2801,13 +2790,14 @@
         <v>161</v>
       </c>
       <c r="C80" s="2">
-        <v>1.613</v>
+        <v>5.699</v>
       </c>
       <c r="D80" s="2">
-        <v>123.304715164726</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>112.554982785286</v>
+      </c>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
         <v>162</v>
       </c>
@@ -2815,13 +2805,14 @@
         <v>163</v>
       </c>
       <c r="C81" s="2">
-        <v>2.997</v>
+        <v>5.999</v>
       </c>
       <c r="D81" s="2">
-        <v>120.33641442544</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>117.161127530787</v>
+      </c>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>164</v>
       </c>
@@ -2829,13 +2820,14 @@
         <v>165</v>
       </c>
       <c r="C82" s="2">
-        <v>5.825</v>
+        <v>6.42</v>
       </c>
       <c r="D82" s="2">
-        <v>123.815473958624</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>129.108623289578</v>
+      </c>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>166</v>
       </c>
@@ -2843,13 +2835,14 @@
         <v>167</v>
       </c>
       <c r="C83" s="2">
-        <v>2.297</v>
+        <v>4.85</v>
       </c>
       <c r="D83" s="2">
-        <v>119.823463989325</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>118.637884759904</v>
+      </c>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>168</v>
       </c>
@@ -2857,13 +2850,14 @@
         <v>169</v>
       </c>
       <c r="C84" s="2">
-        <v>2.089</v>
+        <v>4.65</v>
       </c>
       <c r="D84" s="2">
-        <v>115.266340194479</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>121.19235157737</v>
+      </c>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -2871,13 +2865,14 @@
         <v>171</v>
       </c>
       <c r="C85" s="2">
-        <v>2.249</v>
+        <v>4.1</v>
       </c>
       <c r="D85" s="2">
-        <v>117.030703376507</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>121.597267017794</v>
+      </c>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="2" t="s">
         <v>172</v>
       </c>
@@ -2885,13 +2880,14 @@
         <v>173</v>
       </c>
       <c r="C86" s="2">
-        <v>2.171</v>
+        <v>3.33</v>
       </c>
       <c r="D86" s="2">
-        <v>116.700977382144</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>121.81979875053</v>
+      </c>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="2" t="s">
         <v>174</v>
       </c>
@@ -2899,221 +2895,282 @@
         <v>175</v>
       </c>
       <c r="C87" s="2">
-        <v>4.775</v>
+        <v>5</v>
       </c>
       <c r="D87" s="2">
-        <v>121.049724109707</v>
-      </c>
+        <v>121.502960897923</v>
+      </c>
+      <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="2">
-        <v>5.499</v>
-      </c>
-      <c r="D88" s="2">
-        <v>113.327545443232</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="2">
-        <v>5</v>
-      </c>
-      <c r="D89" s="2">
-        <v>120.399448200669</v>
-      </c>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C90" s="2">
-        <v>5.699</v>
-      </c>
-      <c r="D90" s="2">
-        <v>112.557325807964</v>
-      </c>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C91" s="2">
-        <v>5.999</v>
-      </c>
-      <c r="D91" s="2">
-        <v>117.190911231469</v>
-      </c>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C92" s="2">
-        <v>6.42</v>
-      </c>
-      <c r="D92" s="2">
-        <v>129.094540919188</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C93" s="2">
-        <v>4.85</v>
-      </c>
-      <c r="D93" s="2">
-        <v>118.625249125071</v>
-      </c>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C94" s="2">
-        <v>4.65</v>
-      </c>
-      <c r="D94" s="2">
-        <v>121.233484609976</v>
-      </c>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C95" s="2">
-        <v>3.33</v>
-      </c>
-      <c r="D95" s="2">
-        <v>121.842307787216</v>
-      </c>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C96" s="2">
-        <v>5</v>
-      </c>
-      <c r="D96" s="2">
-        <v>121.520163542405</v>
-      </c>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C97" s="2">
-        <v>4.1</v>
-      </c>
-      <c r="D97" s="2">
-        <v>121.635998526793</v>
-      </c>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C98" s="2">
-        <v>2.674</v>
-      </c>
-      <c r="D98" s="2">
-        <v>120.680103700345</v>
-      </c>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C99" s="2">
-        <v>3.874</v>
-      </c>
-      <c r="D99" s="2">
-        <v>121.653164044284</v>
-      </c>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C100" s="2">
-        <v>4.4</v>
-      </c>
-      <c r="D100" s="2">
-        <v>115.127671719834</v>
-      </c>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C101" s="2">
-        <v>4.3</v>
-      </c>
-      <c r="D101" s="2">
-        <v>114.559256285896</v>
-      </c>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C102" s="2">
-        <v>3.6</v>
-      </c>
-      <c r="D102" s="2">
-        <v>121.138096580978</v>
-      </c>
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1.add bested from kgood
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
   <si>
     <t>code</t>
   </si>
@@ -28,24 +28,6 @@
     <t>expval</t>
   </si>
   <si>
-    <t>sz123162</t>
-  </si>
-  <si>
-    <t>东杰转债</t>
-  </si>
-  <si>
-    <t>sz123163</t>
-  </si>
-  <si>
-    <t>金沃转债</t>
-  </si>
-  <si>
-    <t>sz123164</t>
-  </si>
-  <si>
-    <t>法本转债</t>
-  </si>
-  <si>
     <t>sz123126</t>
   </si>
   <si>
@@ -58,16 +40,52 @@
     <t>雪榕转债</t>
   </si>
   <si>
+    <t>sz123106</t>
+  </si>
+  <si>
+    <t>正丹转债</t>
+  </si>
+  <si>
+    <t>sz123011</t>
+  </si>
+  <si>
+    <t>德尔转债</t>
+  </si>
+  <si>
+    <t>sz123010</t>
+  </si>
+  <si>
+    <t>博世转债</t>
+  </si>
+  <si>
     <t>sz123039</t>
   </si>
   <si>
     <t>开润转债</t>
   </si>
   <si>
-    <t>sz123106</t>
-  </si>
-  <si>
-    <t>正丹转债</t>
+    <t>sz123063</t>
+  </si>
+  <si>
+    <t>大禹转债</t>
+  </si>
+  <si>
+    <t>sz123059</t>
+  </si>
+  <si>
+    <t>银信转债</t>
+  </si>
+  <si>
+    <t>sz123044</t>
+  </si>
+  <si>
+    <t>红相转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
   </si>
   <si>
     <t>sz123093</t>
@@ -76,18 +94,6 @@
     <t>金陵转债</t>
   </si>
   <si>
-    <t>sz123063</t>
-  </si>
-  <si>
-    <t>大禹转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
-  </si>
-  <si>
     <t>sz123050</t>
   </si>
   <si>
@@ -100,6 +106,42 @@
     <t>宝莱转债</t>
   </si>
   <si>
+    <t>sz123116</t>
+  </si>
+  <si>
+    <t>万兴转债</t>
+  </si>
+  <si>
+    <t>sz123122</t>
+  </si>
+  <si>
+    <t>富瀚转债</t>
+  </si>
+  <si>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
+  </si>
+  <si>
+    <t>sz123061</t>
+  </si>
+  <si>
+    <t>航新转债</t>
+  </si>
+  <si>
+    <t>sz123087</t>
+  </si>
+  <si>
+    <t>明电转债</t>
+  </si>
+  <si>
+    <t>sz123132</t>
+  </si>
+  <si>
+    <t>回盛转债</t>
+  </si>
+  <si>
     <t>sz123129</t>
   </si>
   <si>
@@ -112,22 +154,10 @@
     <t>朗科转债</t>
   </si>
   <si>
-    <t>sz123116</t>
-  </si>
-  <si>
-    <t>万兴转债</t>
-  </si>
-  <si>
-    <t>sz123122</t>
-  </si>
-  <si>
-    <t>富瀚转债</t>
-  </si>
-  <si>
-    <t>sz123109</t>
-  </si>
-  <si>
-    <t>昌红转债</t>
+    <t>sz123101</t>
+  </si>
+  <si>
+    <t>拓斯转债</t>
   </si>
   <si>
     <t>sz123088</t>
@@ -136,10 +166,10 @@
     <t>威唐转债</t>
   </si>
   <si>
-    <t>sz123064</t>
-  </si>
-  <si>
-    <t>万孚转债</t>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>中陆转债</t>
   </si>
   <si>
     <t>sz123131</t>
@@ -148,64 +178,82 @@
     <t>奥飞转债</t>
   </si>
   <si>
+    <t>sz123124</t>
+  </si>
+  <si>
+    <t>晶瑞转2</t>
+  </si>
+  <si>
+    <t>sz123075</t>
+  </si>
+  <si>
+    <t>贝斯转债</t>
+  </si>
+  <si>
+    <t>sz123136</t>
+  </si>
+  <si>
+    <t>城市转债</t>
+  </si>
+  <si>
+    <t>sz123142</t>
+  </si>
+  <si>
+    <t>申昊转债</t>
+  </si>
+  <si>
+    <t>sz123153</t>
+  </si>
+  <si>
+    <t>英力转债</t>
+  </si>
+  <si>
+    <t>sz123141</t>
+  </si>
+  <si>
+    <t>宏丰转债</t>
+  </si>
+  <si>
+    <t>sz123160</t>
+  </si>
+  <si>
+    <t>泰福转债</t>
+  </si>
+  <si>
+    <t>sz123127</t>
+  </si>
+  <si>
+    <t>耐普转债</t>
+  </si>
+  <si>
+    <t>sz123168</t>
+  </si>
+  <si>
+    <t>惠云转债</t>
+  </si>
+  <si>
+    <t>sz123157</t>
+  </si>
+  <si>
+    <t>科蓝转债</t>
+  </si>
+  <si>
+    <t>sz123138</t>
+  </si>
+  <si>
+    <t>丝路转债</t>
+  </si>
+  <si>
     <t>sz123154</t>
   </si>
   <si>
     <t>火星转债</t>
   </si>
   <si>
-    <t>sz123101</t>
-  </si>
-  <si>
-    <t>拓斯转债</t>
-  </si>
-  <si>
-    <t>sz123136</t>
-  </si>
-  <si>
-    <t>城市转债</t>
-  </si>
-  <si>
-    <t>sz123153</t>
-  </si>
-  <si>
-    <t>英力转债</t>
-  </si>
-  <si>
-    <t>sz123155</t>
-  </si>
-  <si>
-    <t>中陆转债</t>
-  </si>
-  <si>
-    <t>sz123138</t>
-  </si>
-  <si>
-    <t>丝路转债</t>
-  </si>
-  <si>
-    <t>sz123124</t>
-  </si>
-  <si>
-    <t>晶瑞转2</t>
-  </si>
-  <si>
-    <t>sz123132</t>
-  </si>
-  <si>
-    <t>回盛转债</t>
-  </si>
-  <si>
-    <t>sz123127</t>
-  </si>
-  <si>
-    <t>耐普转债</t>
-  </si>
-  <si>
-    <t>sz123160</t>
-  </si>
-  <si>
-    <t>泰福转债</t>
+    <t>sz123151</t>
+  </si>
+  <si>
+    <t>康医转债</t>
   </si>
   <si>
     <t>sz123144</t>
@@ -214,10 +262,16 @@
     <t>裕兴转债</t>
   </si>
   <si>
-    <t>sz123159</t>
-  </si>
-  <si>
-    <t>崧盛转债</t>
+    <t>sz123147</t>
+  </si>
+  <si>
+    <t>中辰转债</t>
+  </si>
+  <si>
+    <t>sz123167</t>
+  </si>
+  <si>
+    <t>商络转债</t>
   </si>
   <si>
     <t>sz128138</t>
@@ -238,70 +292,124 @@
     <t>游族转债</t>
   </si>
   <si>
+    <t>sz127041</t>
+  </si>
+  <si>
+    <t>弘亚转债</t>
+  </si>
+  <si>
     <t>sz128118</t>
   </si>
   <si>
     <t>瀛通转债</t>
   </si>
   <si>
-    <t>sz128044</t>
-  </si>
-  <si>
-    <t>岭南转债</t>
-  </si>
-  <si>
     <t>sz128125</t>
   </si>
   <si>
     <t>华阳转债</t>
   </si>
   <si>
+    <t>sz127078</t>
+  </si>
+  <si>
+    <t>优彩转债</t>
+  </si>
+  <si>
+    <t>sz127079</t>
+  </si>
+  <si>
+    <t>华亚转债</t>
+  </si>
+  <si>
+    <t>sz128116</t>
+  </si>
+  <si>
+    <t>瑞达转债</t>
+  </si>
+  <si>
+    <t>sz127077</t>
+  </si>
+  <si>
+    <t>华宏转债</t>
+  </si>
+  <si>
+    <t>sz128066</t>
+  </si>
+  <si>
+    <t>亚泰转债</t>
+  </si>
+  <si>
     <t>sz128072</t>
   </si>
   <si>
     <t>翔鹭转债</t>
   </si>
   <si>
-    <t>sz127072</t>
-  </si>
-  <si>
-    <t>博实转债</t>
-  </si>
-  <si>
-    <t>sz127041</t>
-  </si>
-  <si>
-    <t>弘亚转债</t>
-  </si>
-  <si>
-    <t>sz128116</t>
-  </si>
-  <si>
-    <t>瑞达转债</t>
-  </si>
-  <si>
     <t>sz128049</t>
   </si>
   <si>
     <t>华源转债</t>
   </si>
   <si>
+    <t>sz128071</t>
+  </si>
+  <si>
+    <t>合兴转债</t>
+  </si>
+  <si>
+    <t>sz127051</t>
+  </si>
+  <si>
+    <t>博杰转债</t>
+  </si>
+  <si>
     <t>sz128117</t>
   </si>
   <si>
     <t>道恩转债</t>
   </si>
   <si>
-    <t>sz128071</t>
-  </si>
-  <si>
-    <t>合兴转债</t>
-  </si>
-  <si>
-    <t>sz127051</t>
-  </si>
-  <si>
-    <t>博杰转债</t>
+    <t>sz128123</t>
+  </si>
+  <si>
+    <t>国光转债</t>
+  </si>
+  <si>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>奥佳转债</t>
+  </si>
+  <si>
+    <t>sz128120</t>
+  </si>
+  <si>
+    <t>联诚转债</t>
+  </si>
+  <si>
+    <t>sz127035</t>
+  </si>
+  <si>
+    <t>濮耐转债</t>
+  </si>
+  <si>
+    <t>sz127026</t>
+  </si>
+  <si>
+    <t>超声转债</t>
+  </si>
+  <si>
+    <t>sz128143</t>
+  </si>
+  <si>
+    <t>锋龙转债</t>
+  </si>
+  <si>
+    <t>sz127054</t>
+  </si>
+  <si>
+    <t>双箭转债</t>
   </si>
   <si>
     <t>sz127055</t>
@@ -310,52 +418,124 @@
     <t>精装转债</t>
   </si>
   <si>
-    <t>sz128123</t>
-  </si>
-  <si>
-    <t>国光转债</t>
-  </si>
-  <si>
-    <t>sz128097</t>
-  </si>
-  <si>
-    <t>奥佳转债</t>
-  </si>
-  <si>
-    <t>sz128143</t>
-  </si>
-  <si>
-    <t>锋龙转债</t>
-  </si>
-  <si>
     <t>sz127062</t>
   </si>
   <si>
     <t>垒知转债</t>
   </si>
   <si>
-    <t>sz127054</t>
-  </si>
-  <si>
-    <t>双箭转债</t>
-  </si>
-  <si>
     <t>sh113589</t>
   </si>
   <si>
     <t>天创转债</t>
   </si>
   <si>
+    <t>sh113578</t>
+  </si>
+  <si>
+    <t>全筑转债</t>
+  </si>
+  <si>
     <t>sh113569</t>
   </si>
   <si>
     <t>科达转债</t>
   </si>
   <si>
-    <t>sh113578</t>
-  </si>
-  <si>
-    <t>全筑转债</t>
+    <t>sh113584</t>
+  </si>
+  <si>
+    <t>家悦转债</t>
+  </si>
+  <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
+    <t>sh113624</t>
+  </si>
+  <si>
+    <t>正川转债</t>
+  </si>
+  <si>
+    <t>sh113664</t>
+  </si>
+  <si>
+    <t>大元转债</t>
+  </si>
+  <si>
+    <t>sh113535</t>
+  </si>
+  <si>
+    <t>大业转债</t>
+  </si>
+  <si>
+    <t>sh113604</t>
+  </si>
+  <si>
+    <t>多伦转债</t>
+  </si>
+  <si>
+    <t>sh113530</t>
+  </si>
+  <si>
+    <t>大丰转债</t>
+  </si>
+  <si>
+    <t>sh113606</t>
+  </si>
+  <si>
+    <t>荣泰转债</t>
+  </si>
+  <si>
+    <t>sh113665</t>
+  </si>
+  <si>
+    <t>汇通转债</t>
+  </si>
+  <si>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <t>纵横转债</t>
+  </si>
+  <si>
+    <t>sh113527</t>
+  </si>
+  <si>
+    <t>维格转债</t>
+  </si>
+  <si>
+    <t>sh113593</t>
+  </si>
+  <si>
+    <t>沪工转债</t>
+  </si>
+  <si>
+    <t>sh113542</t>
+  </si>
+  <si>
+    <t>好客转债</t>
+  </si>
+  <si>
+    <t>sh113519</t>
+  </si>
+  <si>
+    <t>长久转债</t>
+  </si>
+  <si>
+    <t>sh113628</t>
+  </si>
+  <si>
+    <t>晨丰转债</t>
+  </si>
+  <si>
+    <t>sh113662</t>
+  </si>
+  <si>
+    <t>豪能转债</t>
   </si>
   <si>
     <t>sh113601</t>
@@ -364,64 +544,64 @@
     <t>塞力转债</t>
   </si>
   <si>
-    <t>sh113584</t>
-  </si>
-  <si>
-    <t>家悦转债</t>
-  </si>
-  <si>
-    <t>sh113530</t>
-  </si>
-  <si>
-    <t>大丰转债</t>
-  </si>
-  <si>
-    <t>sh113608</t>
-  </si>
-  <si>
-    <t>威派转债</t>
-  </si>
-  <si>
-    <t>sh113573</t>
-  </si>
-  <si>
-    <t>纵横转债</t>
-  </si>
-  <si>
-    <t>sh113606</t>
-  </si>
-  <si>
-    <t>荣泰转债</t>
-  </si>
-  <si>
-    <t>sh113604</t>
-  </si>
-  <si>
-    <t>多伦转债</t>
-  </si>
-  <si>
-    <t>sh113624</t>
-  </si>
-  <si>
-    <t>正川转债</t>
-  </si>
-  <si>
-    <t>sh113527</t>
-  </si>
-  <si>
-    <t>维格转债</t>
-  </si>
-  <si>
-    <t>sh113519</t>
-  </si>
-  <si>
-    <t>长久转债</t>
-  </si>
-  <si>
-    <t>sh113593</t>
-  </si>
-  <si>
-    <t>沪工转债</t>
+    <t>sh113610</t>
+  </si>
+  <si>
+    <t>灵康转债</t>
+  </si>
+  <si>
+    <t>sh113566</t>
+  </si>
+  <si>
+    <t>翔港转债</t>
+  </si>
+  <si>
+    <t>sh110058</t>
+  </si>
+  <si>
+    <t>永鼎转债</t>
+  </si>
+  <si>
+    <t>sh113600</t>
+  </si>
+  <si>
+    <t>新星转债</t>
+  </si>
+  <si>
+    <t>sh113532</t>
+  </si>
+  <si>
+    <t>海环转债</t>
+  </si>
+  <si>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>凌钢转债</t>
+  </si>
+  <si>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>华体转债</t>
+  </si>
+  <si>
+    <t>sh113546</t>
+  </si>
+  <si>
+    <t>迪贝转债</t>
+  </si>
+  <si>
+    <t>sh113591</t>
+  </si>
+  <si>
+    <t>胜达转债</t>
+  </si>
+  <si>
+    <t>sh113579</t>
+  </si>
+  <si>
+    <t>健友转债</t>
   </si>
   <si>
     <t>sh113625</t>
@@ -430,40 +610,16 @@
     <t>江山转债</t>
   </si>
   <si>
-    <t>sh113524</t>
-  </si>
-  <si>
-    <t>奇精转债</t>
-  </si>
-  <si>
-    <t>sh113610</t>
-  </si>
-  <si>
-    <t>灵康转债</t>
-  </si>
-  <si>
-    <t>sh113566</t>
-  </si>
-  <si>
-    <t>翔港转债</t>
-  </si>
-  <si>
-    <t>sh113628</t>
-  </si>
-  <si>
-    <t>晨丰转债</t>
-  </si>
-  <si>
-    <t>sh113542</t>
-  </si>
-  <si>
-    <t>好客转债</t>
-  </si>
-  <si>
-    <t>sh113597</t>
-  </si>
-  <si>
-    <t>佳力转债</t>
+    <t>sh113588</t>
+  </si>
+  <si>
+    <t>润达转债</t>
+  </si>
+  <si>
+    <t>sh113639</t>
+  </si>
+  <si>
+    <t>华正转债</t>
   </si>
   <si>
     <t>sh113594</t>
@@ -472,22 +628,10 @@
     <t>淳中转债</t>
   </si>
   <si>
-    <t>sh113546</t>
-  </si>
-  <si>
-    <t>迪贝转债</t>
-  </si>
-  <si>
-    <t>sh113574</t>
-  </si>
-  <si>
-    <t>华体转债</t>
-  </si>
-  <si>
-    <t>sh110070</t>
-  </si>
-  <si>
-    <t>凌钢转债</t>
+    <t>sh113638</t>
+  </si>
+  <si>
+    <t>台21转债</t>
   </si>
   <si>
     <t>sh113643</t>
@@ -496,16 +640,28 @@
     <t>风语转债</t>
   </si>
   <si>
-    <t>sh113639</t>
-  </si>
-  <si>
-    <t>华正转债</t>
-  </si>
-  <si>
-    <t>sh113638</t>
-  </si>
-  <si>
-    <t>台21转债</t>
+    <t>sh113663</t>
+  </si>
+  <si>
+    <t>新化转债</t>
+  </si>
+  <si>
+    <t>sh113657</t>
+  </si>
+  <si>
+    <t>再22转债</t>
+  </si>
+  <si>
+    <t>sh118029</t>
+  </si>
+  <si>
+    <t>富淼转债</t>
+  </si>
+  <si>
+    <t>sh118004</t>
+  </si>
+  <si>
+    <t>博瑞转债</t>
   </si>
   <si>
     <t>sh118020</t>
@@ -514,34 +670,34 @@
     <t>芳源转债</t>
   </si>
   <si>
-    <t>sh118021</t>
-  </si>
-  <si>
-    <t>新致转债</t>
-  </si>
-  <si>
-    <t>sh118004</t>
-  </si>
-  <si>
-    <t>博瑞转债</t>
-  </si>
-  <si>
-    <t>sh118015</t>
-  </si>
-  <si>
-    <t>芯海转债</t>
-  </si>
-  <si>
     <t>sh118016</t>
   </si>
   <si>
     <t>京源转债</t>
   </si>
   <si>
+    <t>sh118010</t>
+  </si>
+  <si>
+    <t>洁特转债</t>
+  </si>
+  <si>
     <t>sh118011</t>
   </si>
   <si>
     <t>银微转债</t>
+  </si>
+  <si>
+    <t>sh118008</t>
+  </si>
+  <si>
+    <t>海优转债</t>
+  </si>
+  <si>
+    <t>sh118012</t>
+  </si>
+  <si>
+    <t>微芯转债</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1698,7 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E87"/>
+      <selection activeCell="A2" sqref="A2:D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1581,12 +1737,11 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>5.7</v>
+        <v>3.4</v>
       </c>
       <c r="D2" s="2">
-        <v>122.208506713255</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>129.775951766309</v>
+      </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9">
@@ -1597,12 +1752,11 @@
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>3.1</v>
+        <v>5.84</v>
       </c>
       <c r="D3" s="2">
-        <v>122.208506713255</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>120.279602862675</v>
+      </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9">
@@ -1613,12 +1767,11 @@
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>6.01</v>
+        <v>3.2</v>
       </c>
       <c r="D4" s="2">
-        <v>122.007964736343</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>125.413323324186</v>
+      </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9">
@@ -1629,12 +1782,11 @@
         <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>3.4</v>
+        <v>2.506</v>
       </c>
       <c r="D5" s="2">
-        <v>129.702239129399</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>113.805497355318</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9">
@@ -1645,12 +1797,11 @@
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>5.84</v>
+        <v>4.296</v>
       </c>
       <c r="D6" s="2">
-        <v>120.22392895889</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>109.806364369788</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
@@ -1664,9 +1815,8 @@
         <v>2.217</v>
       </c>
       <c r="D7" s="2">
-        <v>120.434723971996</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>120.482464207574</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
@@ -1677,12 +1827,11 @@
         <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>3.2</v>
+        <v>6.346</v>
       </c>
       <c r="D8" s="2">
-        <v>125.331277626309</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>125.696979628134</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
@@ -1693,12 +1842,11 @@
         <v>19</v>
       </c>
       <c r="C9" s="2">
-        <v>2.485</v>
+        <v>3.912</v>
       </c>
       <c r="D9" s="2">
-        <v>129.161402712328</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>123.182534734273</v>
+      </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9">
@@ -1709,12 +1857,11 @@
         <v>21</v>
       </c>
       <c r="C10" s="2">
-        <v>6.346</v>
+        <v>5.496</v>
       </c>
       <c r="D10" s="2">
-        <v>125.64457412544</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>124.407318432992</v>
+      </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9">
@@ -1728,9 +1875,8 @@
         <v>4.993</v>
       </c>
       <c r="D11" s="2">
-        <v>121.365154902833</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>120.717906262882</v>
+      </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9">
@@ -1741,12 +1887,11 @@
         <v>25</v>
       </c>
       <c r="C12" s="2">
-        <v>3.746</v>
+        <v>2.485</v>
       </c>
       <c r="D12" s="2">
-        <v>123.082471733304</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>129.190190315899</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9">
@@ -1757,12 +1902,11 @@
         <v>27</v>
       </c>
       <c r="C13" s="2">
-        <v>2.188</v>
+        <v>3.746</v>
       </c>
       <c r="D13" s="2">
-        <v>120.414323992965</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>123.12034455477</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9">
@@ -1773,12 +1917,11 @@
         <v>29</v>
       </c>
       <c r="C14" s="2">
-        <v>6</v>
+        <v>2.188</v>
       </c>
       <c r="D14" s="2">
-        <v>117.952975594569</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>120.439833970523</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9">
@@ -1789,12 +1932,11 @@
         <v>31</v>
       </c>
       <c r="C15" s="2">
-        <v>3.797</v>
+        <v>3.781</v>
       </c>
       <c r="D15" s="2">
-        <v>117.166171308751</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>121.229735435196</v>
+      </c>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9">
@@ -1805,12 +1947,11 @@
         <v>33</v>
       </c>
       <c r="C16" s="2">
-        <v>3.781</v>
+        <v>5.806</v>
       </c>
       <c r="D16" s="2">
-        <v>121.108095832548</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>120.182520445783</v>
+      </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
@@ -1821,12 +1962,11 @@
         <v>35</v>
       </c>
       <c r="C17" s="2">
-        <v>5.806</v>
+        <v>4.596</v>
       </c>
       <c r="D17" s="2">
-        <v>120.093744502809</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>120.739367943445</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9">
@@ -1837,12 +1977,11 @@
         <v>37</v>
       </c>
       <c r="C18" s="2">
-        <v>4.596</v>
+        <v>2.496</v>
       </c>
       <c r="D18" s="2">
-        <v>120.68213594129</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>123.579781993773</v>
+      </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9">
@@ -1853,12 +1992,11 @@
         <v>39</v>
       </c>
       <c r="C19" s="2">
-        <v>3.011</v>
+        <v>4.189</v>
       </c>
       <c r="D19" s="2">
-        <v>121.136250751311</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>120.11591490354</v>
+      </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9">
@@ -1869,12 +2007,11 @@
         <v>41</v>
       </c>
       <c r="C20" s="2">
-        <v>5.98</v>
+        <v>7</v>
       </c>
       <c r="D20" s="2">
-        <v>114.300817872756</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>120.790615461815</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
@@ -1885,12 +2022,11 @@
         <v>43</v>
       </c>
       <c r="C21" s="2">
-        <v>6.35</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>121.821173633168</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>117.547832115359</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -1901,12 +2037,11 @@
         <v>45</v>
       </c>
       <c r="C22" s="2">
-        <v>5.29</v>
+        <v>3.797</v>
       </c>
       <c r="D22" s="2">
-        <v>120.442238450499</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>117.197375594109</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9">
@@ -1920,9 +2055,8 @@
         <v>6.698</v>
       </c>
       <c r="D23" s="2">
-        <v>114.800180393216</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>114.893447064604</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9">
@@ -1933,12 +2067,11 @@
         <v>49</v>
       </c>
       <c r="C24" s="2">
-        <v>4.595</v>
+        <v>3.011</v>
       </c>
       <c r="D24" s="2">
-        <v>120.780465188271</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>120.490423955852</v>
+      </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9">
@@ -1949,12 +2082,11 @@
         <v>51</v>
       </c>
       <c r="C25" s="2">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="D25" s="2">
-        <v>121.62827146443</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>121.727804581142</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9">
@@ -1965,12 +2097,11 @@
         <v>53</v>
       </c>
       <c r="C26" s="2">
-        <v>3.6</v>
+        <v>6.35</v>
       </c>
       <c r="D26" s="2">
-        <v>121.615576757967</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>121.310550578895</v>
+      </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9">
@@ -1981,12 +2112,11 @@
         <v>55</v>
       </c>
       <c r="C27" s="2">
-        <v>2.4</v>
+        <v>5.228</v>
       </c>
       <c r="D27" s="2">
-        <v>121.775942514343</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>111.042019832169</v>
+      </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9">
@@ -1997,12 +2127,11 @@
         <v>57</v>
       </c>
       <c r="C28" s="2">
-        <v>5.228</v>
+        <v>5.996</v>
       </c>
       <c r="D28" s="2">
-        <v>110.998297016948</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>114.529078733487</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9">
@@ -2013,12 +2142,11 @@
         <v>59</v>
       </c>
       <c r="C29" s="2">
-        <v>7</v>
+        <v>4.595</v>
       </c>
       <c r="D29" s="2">
-        <v>121.007400182369</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>120.798814397604</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9">
@@ -2029,12 +2157,11 @@
         <v>61</v>
       </c>
       <c r="C30" s="2">
-        <v>4</v>
+        <v>5.497</v>
       </c>
       <c r="D30" s="2">
-        <v>116.231416088774</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>116.108876217728</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
@@ -2045,12 +2172,11 @@
         <v>63</v>
       </c>
       <c r="C31" s="2">
-        <v>3.349</v>
+        <v>3.4</v>
       </c>
       <c r="D31" s="2">
-        <v>121.59590373631</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>121.672539737941</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9">
@@ -2061,12 +2187,11 @@
         <v>65</v>
       </c>
       <c r="C32" s="2">
-        <v>6</v>
+        <v>3.212</v>
       </c>
       <c r="D32" s="2">
-        <v>120.327845186873</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>121.815195216999</v>
+      </c>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9">
@@ -2077,12 +2202,11 @@
         <v>67</v>
       </c>
       <c r="C33" s="2">
-        <v>2.94</v>
+        <v>3.349</v>
       </c>
       <c r="D33" s="2">
-        <v>119.315741352218</v>
-      </c>
-      <c r="E33" s="2"/>
+        <v>121.678844361975</v>
+      </c>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9">
@@ -2093,12 +2217,11 @@
         <v>69</v>
       </c>
       <c r="C34" s="2">
-        <v>4.199</v>
+        <v>3.999</v>
       </c>
       <c r="D34" s="2">
-        <v>136.546581422295</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>115.837920142942</v>
+      </c>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9">
@@ -2109,12 +2232,11 @@
         <v>71</v>
       </c>
       <c r="C35" s="2">
-        <v>6.292</v>
+        <v>4.9</v>
       </c>
       <c r="D35" s="2">
-        <v>126.235249764146</v>
-      </c>
-      <c r="E35" s="2"/>
+        <v>120.803856366434</v>
+      </c>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9">
@@ -2125,12 +2247,11 @@
         <v>73</v>
       </c>
       <c r="C36" s="2">
-        <v>6.825</v>
+        <v>4.946</v>
       </c>
       <c r="D36" s="2">
-        <v>118.444703028016</v>
-      </c>
-      <c r="E36" s="2"/>
+        <v>120.357335457746</v>
+      </c>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9">
@@ -2141,12 +2262,11 @@
         <v>75</v>
       </c>
       <c r="C37" s="2">
-        <v>2.996</v>
+        <v>2.4</v>
       </c>
       <c r="D37" s="2">
-        <v>121.263033639477</v>
-      </c>
-      <c r="E37" s="2"/>
+        <v>121.750966520842</v>
+      </c>
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9">
@@ -2157,12 +2277,11 @@
         <v>77</v>
       </c>
       <c r="C38" s="2">
-        <v>6.573</v>
+        <v>5.29</v>
       </c>
       <c r="D38" s="2">
-        <v>108.811031957239</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>120.343475609508</v>
+      </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9">
@@ -2173,12 +2292,11 @@
         <v>79</v>
       </c>
       <c r="C39" s="2">
-        <v>4.498</v>
+        <v>7</v>
       </c>
       <c r="D39" s="2">
-        <v>117.703269961079</v>
-      </c>
-      <c r="E39" s="2"/>
+        <v>121.61875945595</v>
+      </c>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9">
@@ -2189,15 +2307,14 @@
         <v>81</v>
       </c>
       <c r="C40" s="2">
-        <v>3.017</v>
+        <v>6</v>
       </c>
       <c r="D40" s="2">
-        <v>113.574001079056</v>
-      </c>
-      <c r="E40" s="2"/>
+        <v>120.33721879917</v>
+      </c>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>82</v>
       </c>
@@ -2205,14 +2322,13 @@
         <v>83</v>
       </c>
       <c r="C41" s="2">
-        <v>4.5</v>
+        <v>5.705</v>
       </c>
       <c r="D41" s="2">
-        <v>117.438220088514</v>
-      </c>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5">
+        <v>120.125083415283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
@@ -2220,14 +2336,13 @@
         <v>85</v>
       </c>
       <c r="C42" s="2">
-        <v>5.999</v>
+        <v>3.965</v>
       </c>
       <c r="D42" s="2">
-        <v>118.349959793004</v>
-      </c>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5">
+        <v>121.518728525994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2235,14 +2350,13 @@
         <v>87</v>
       </c>
       <c r="C43" s="2">
-        <v>6.491</v>
+        <v>4.199</v>
       </c>
       <c r="D43" s="2">
-        <v>114.573722649771</v>
-      </c>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5">
+        <v>135.896704725403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>88</v>
       </c>
@@ -2250,14 +2364,13 @@
         <v>89</v>
       </c>
       <c r="C44" s="2">
-        <v>3.631</v>
+        <v>6.292</v>
       </c>
       <c r="D44" s="2">
-        <v>113.513749312878</v>
-      </c>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5">
+        <v>126.285924954847</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
@@ -2265,14 +2378,13 @@
         <v>91</v>
       </c>
       <c r="C45" s="2">
-        <v>3.586</v>
+        <v>6.825</v>
       </c>
       <c r="D45" s="2">
-        <v>122.653015068136</v>
-      </c>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5">
+        <v>118.450505960349</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -2280,14 +2392,13 @@
         <v>93</v>
       </c>
       <c r="C46" s="2">
-        <v>2.999</v>
+        <v>5.999</v>
       </c>
       <c r="D46" s="2">
-        <v>113.311118500451</v>
-      </c>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5">
+        <v>118.454977941225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
         <v>94</v>
       </c>
@@ -2295,14 +2406,13 @@
         <v>95</v>
       </c>
       <c r="C47" s="2">
-        <v>5.259</v>
+        <v>2.996</v>
       </c>
       <c r="D47" s="2">
-        <v>121.354820651447</v>
-      </c>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5">
+        <v>121.33880822345</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>96</v>
       </c>
@@ -2310,14 +2420,13 @@
         <v>97</v>
       </c>
       <c r="C48" s="2">
-        <v>5.769</v>
+        <v>4.498</v>
       </c>
       <c r="D48" s="2">
-        <v>120.492760104019</v>
-      </c>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5">
+        <v>117.731624487481</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>98</v>
       </c>
@@ -2325,14 +2434,13 @@
         <v>99</v>
       </c>
       <c r="C49" s="2">
-        <v>3.199</v>
+        <v>6</v>
       </c>
       <c r="D49" s="2">
-        <v>115.098549806292</v>
-      </c>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5">
+        <v>122.016076420943</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>100</v>
       </c>
@@ -2340,14 +2448,13 @@
         <v>101</v>
       </c>
       <c r="C50" s="2">
-        <v>4.585</v>
+        <v>3.4</v>
       </c>
       <c r="D50" s="2">
-        <v>114.318001983785</v>
-      </c>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5">
+        <v>121.687162654827</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>102</v>
       </c>
@@ -2355,14 +2462,13 @@
         <v>103</v>
       </c>
       <c r="C51" s="2">
-        <v>2.441</v>
+        <v>6.491</v>
       </c>
       <c r="D51" s="2">
-        <v>121.235693680051</v>
-      </c>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5">
+        <v>114.618168977266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -2370,14 +2476,13 @@
         <v>105</v>
       </c>
       <c r="C52" s="2">
-        <v>3.963</v>
+        <v>5.15</v>
       </c>
       <c r="D52" s="2">
-        <v>120.603603981709</v>
-      </c>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5">
+        <v>121.321903047271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>106</v>
       </c>
@@ -2385,14 +2490,13 @@
         <v>107</v>
       </c>
       <c r="C53" s="2">
-        <v>5.136</v>
+        <v>4.611</v>
       </c>
       <c r="D53" s="2">
-        <v>117.196362097403</v>
-      </c>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5">
+        <v>115.583637604527</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
@@ -2400,14 +2504,13 @@
         <v>109</v>
       </c>
       <c r="C54" s="2">
-        <v>5.996</v>
+        <v>3.017</v>
       </c>
       <c r="D54" s="2">
-        <v>114.664231299416</v>
-      </c>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5">
+        <v>113.591931881949</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -2415,14 +2518,13 @@
         <v>111</v>
       </c>
       <c r="C55" s="2">
-        <v>5.156</v>
+        <v>3.631</v>
       </c>
       <c r="D55" s="2">
-        <v>119.825752008331</v>
-      </c>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5">
+        <v>112.0027948355</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -2430,14 +2532,13 @@
         <v>113</v>
       </c>
       <c r="C56" s="2">
-        <v>3.838</v>
+        <v>2.999</v>
       </c>
       <c r="D56" s="2">
-        <v>117.615998826295</v>
-      </c>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5">
+        <v>113.343063522845</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>114</v>
       </c>
@@ -2445,14 +2546,13 @@
         <v>115</v>
       </c>
       <c r="C57" s="2">
-        <v>5.426</v>
+        <v>5.259</v>
       </c>
       <c r="D57" s="2">
-        <v>120.235706557985</v>
-      </c>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5">
+        <v>120.988517612503</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>116</v>
       </c>
@@ -2460,14 +2560,13 @@
         <v>117</v>
       </c>
       <c r="C58" s="2">
-        <v>6.449</v>
+        <v>3.586</v>
       </c>
       <c r="D58" s="2">
-        <v>114.490889112864</v>
-      </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5">
+        <v>122.605621389474</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
         <v>118</v>
       </c>
@@ -2475,14 +2574,13 @@
         <v>119</v>
       </c>
       <c r="C59" s="2">
-        <v>6.297</v>
+        <v>3.199</v>
       </c>
       <c r="D59" s="2">
-        <v>120.09031254892</v>
-      </c>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5">
+        <v>115.118027966129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>120</v>
       </c>
@@ -2490,14 +2588,13 @@
         <v>121</v>
       </c>
       <c r="C60" s="2">
-        <v>4.2</v>
+        <v>4.585</v>
       </c>
       <c r="D60" s="2">
-        <v>121.424831504075</v>
-      </c>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5">
+        <v>114.328048264931</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>122</v>
       </c>
@@ -2505,14 +2602,13 @@
         <v>123</v>
       </c>
       <c r="C61" s="2">
-        <v>2.698</v>
+        <v>2.598</v>
       </c>
       <c r="D61" s="2">
-        <v>123.723340003003</v>
-      </c>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5">
+        <v>117.242648272933</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>124</v>
       </c>
@@ -2520,14 +2616,13 @@
         <v>125</v>
       </c>
       <c r="C62" s="2">
-        <v>5.999</v>
+        <v>6.262</v>
       </c>
       <c r="D62" s="2">
-        <v>120.971635900368</v>
-      </c>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5">
+        <v>114.1078787666</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>126</v>
       </c>
@@ -2535,14 +2630,13 @@
         <v>127</v>
       </c>
       <c r="C63" s="2">
-        <v>6.398</v>
+        <v>6.997</v>
       </c>
       <c r="D63" s="2">
-        <v>116.486541938491</v>
-      </c>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5">
+        <v>112.335093234604</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>128</v>
       </c>
@@ -2550,14 +2644,13 @@
         <v>129</v>
       </c>
       <c r="C64" s="2">
-        <v>4.049</v>
+        <v>2.441</v>
       </c>
       <c r="D64" s="2">
-        <v>121.418319682284</v>
-      </c>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5">
+        <v>121.299882377375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>130</v>
       </c>
@@ -2565,14 +2658,13 @@
         <v>131</v>
       </c>
       <c r="C65" s="2">
-        <v>2.862</v>
+        <v>5.136</v>
       </c>
       <c r="D65" s="2">
-        <v>118.56093154333</v>
-      </c>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5">
+        <v>117.223711274716</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>132</v>
       </c>
@@ -2580,14 +2672,13 @@
         <v>133</v>
       </c>
       <c r="C66" s="2">
-        <v>6.961</v>
+        <v>5.768</v>
       </c>
       <c r="D66" s="2">
-        <v>118.332313457061</v>
-      </c>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5">
+        <v>120.434961602486</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>134</v>
       </c>
@@ -2595,14 +2686,13 @@
         <v>135</v>
       </c>
       <c r="C67" s="2">
-        <v>3.998</v>
+        <v>3.962</v>
       </c>
       <c r="D67" s="2">
-        <v>120.786324887702</v>
-      </c>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5">
+        <v>120.576345498157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>136</v>
       </c>
@@ -2610,14 +2700,13 @@
         <v>137</v>
       </c>
       <c r="C68" s="2">
-        <v>5.825</v>
+        <v>5.996</v>
       </c>
       <c r="D68" s="2">
-        <v>123.839191765186</v>
-      </c>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5">
+        <v>114.728399925257</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>138</v>
       </c>
@@ -2625,14 +2714,13 @@
         <v>139</v>
       </c>
       <c r="C69" s="2">
-        <v>3.297</v>
+        <v>3.838</v>
       </c>
       <c r="D69" s="2">
-        <v>116.327549939574</v>
-      </c>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5">
+        <v>117.681987352817</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>140</v>
       </c>
@@ -2640,14 +2728,13 @@
         <v>141</v>
       </c>
       <c r="C70" s="2">
-        <v>4.579</v>
+        <v>5.156</v>
       </c>
       <c r="D70" s="2">
-        <v>120.931508243259</v>
-      </c>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5">
+        <v>119.887253060459</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
         <v>142</v>
       </c>
@@ -2655,14 +2742,13 @@
         <v>143</v>
       </c>
       <c r="C71" s="2">
-        <v>1.613</v>
+        <v>6.449</v>
       </c>
       <c r="D71" s="2">
-        <v>123.318716824373</v>
-      </c>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5">
+        <v>114.590728794408</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>144</v>
       </c>
@@ -2670,12 +2756,11 @@
         <v>145</v>
       </c>
       <c r="C72" s="2">
-        <v>4.15</v>
+        <v>4.2</v>
       </c>
       <c r="D72" s="2">
-        <v>121.475216909532</v>
-      </c>
-      <c r="E72" s="2"/>
+        <v>120.748956704197</v>
+      </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="2" t="s">
@@ -2685,12 +2770,12 @@
         <v>147</v>
       </c>
       <c r="C73" s="2">
-        <v>6.026</v>
+        <v>4.049</v>
       </c>
       <c r="D73" s="2">
-        <v>113.338950056051</v>
-      </c>
-      <c r="E73" s="2"/>
+        <v>121.508660437695</v>
+      </c>
+      <c r="E73" s="4"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="2" t="s">
@@ -2700,12 +2785,12 @@
         <v>149</v>
       </c>
       <c r="C74" s="2">
-        <v>2.983</v>
+        <v>4.5</v>
       </c>
       <c r="D74" s="2">
-        <v>123.42378156679</v>
-      </c>
-      <c r="E74" s="2"/>
+        <v>121.435326339034</v>
+      </c>
+      <c r="E74" s="4"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="2" t="s">
@@ -2715,12 +2800,12 @@
         <v>151</v>
       </c>
       <c r="C75" s="2">
-        <v>2.997</v>
+        <v>4.996</v>
       </c>
       <c r="D75" s="2">
-        <v>120.295083818005</v>
-      </c>
-      <c r="E75" s="2"/>
+        <v>111.519834923959</v>
+      </c>
+      <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="2" t="s">
@@ -2730,12 +2815,12 @@
         <v>153</v>
       </c>
       <c r="C76" s="2">
-        <v>2.297</v>
+        <v>6.398</v>
       </c>
       <c r="D76" s="2">
-        <v>118.607551999917</v>
-      </c>
-      <c r="E76" s="2"/>
+        <v>116.524579871644</v>
+      </c>
+      <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="2" t="s">
@@ -2745,12 +2830,12 @@
         <v>155</v>
       </c>
       <c r="C77" s="2">
-        <v>2.089</v>
+        <v>6.297</v>
       </c>
       <c r="D77" s="2">
-        <v>115.252727442144</v>
-      </c>
-      <c r="E77" s="2"/>
+        <v>120.12028224046</v>
+      </c>
+      <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="2" t="s">
@@ -2760,12 +2845,12 @@
         <v>157</v>
       </c>
       <c r="C78" s="2">
-        <v>2.171</v>
+        <v>5.999</v>
       </c>
       <c r="D78" s="2">
-        <v>116.732001990274</v>
-      </c>
-      <c r="E78" s="2"/>
+        <v>120.242382218536</v>
+      </c>
+      <c r="E78" s="4"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
@@ -2775,12 +2860,12 @@
         <v>159</v>
       </c>
       <c r="C79" s="2">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="D79" s="2">
-        <v>120.445640203504</v>
-      </c>
-      <c r="E79" s="2"/>
+        <v>120.691215451086</v>
+      </c>
+      <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
@@ -2790,12 +2875,12 @@
         <v>161</v>
       </c>
       <c r="C80" s="2">
-        <v>5.699</v>
+        <v>2.698</v>
       </c>
       <c r="D80" s="2">
-        <v>112.554982785286</v>
-      </c>
-      <c r="E80" s="2"/>
+        <v>123.733458503589</v>
+      </c>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
@@ -2805,12 +2890,12 @@
         <v>163</v>
       </c>
       <c r="C81" s="2">
-        <v>5.999</v>
+        <v>2.862</v>
       </c>
       <c r="D81" s="2">
-        <v>117.161127530787</v>
-      </c>
-      <c r="E81" s="2"/>
+        <v>118.587534861657</v>
+      </c>
+      <c r="E81" s="4"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
@@ -2820,12 +2905,12 @@
         <v>165</v>
       </c>
       <c r="C82" s="2">
-        <v>6.42</v>
+        <v>3.998</v>
       </c>
       <c r="D82" s="2">
-        <v>129.108623289578</v>
-      </c>
-      <c r="E82" s="2"/>
+        <v>120.849900705582</v>
+      </c>
+      <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
@@ -2835,12 +2920,12 @@
         <v>167</v>
       </c>
       <c r="C83" s="2">
-        <v>4.85</v>
+        <v>6.026</v>
       </c>
       <c r="D83" s="2">
-        <v>118.637884759904</v>
-      </c>
-      <c r="E83" s="2"/>
+        <v>113.37813849384</v>
+      </c>
+      <c r="E83" s="4"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
@@ -2850,12 +2935,12 @@
         <v>169</v>
       </c>
       <c r="C84" s="2">
-        <v>4.65</v>
+        <v>6.961</v>
       </c>
       <c r="D84" s="2">
-        <v>121.19235157737</v>
-      </c>
-      <c r="E84" s="2"/>
+        <v>116.819633731372</v>
+      </c>
+      <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="2" t="s">
@@ -2865,12 +2950,12 @@
         <v>171</v>
       </c>
       <c r="C85" s="2">
-        <v>4.1</v>
+        <v>4.15</v>
       </c>
       <c r="D85" s="2">
-        <v>121.597267017794</v>
-      </c>
-      <c r="E85" s="2"/>
+        <v>121.522778661912</v>
+      </c>
+      <c r="E85" s="4"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="2" t="s">
@@ -2880,12 +2965,12 @@
         <v>173</v>
       </c>
       <c r="C86" s="2">
-        <v>3.33</v>
+        <v>5</v>
       </c>
       <c r="D86" s="2">
-        <v>121.81979875053</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>118.282741592876</v>
+      </c>
+      <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="2" t="s">
@@ -2895,168 +2980,376 @@
         <v>175</v>
       </c>
       <c r="C87" s="2">
+        <v>5.425</v>
+      </c>
+      <c r="D87" s="2">
+        <v>120.192537966406</v>
+      </c>
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="2">
+        <v>4.579</v>
+      </c>
+      <c r="D88" s="2">
+        <v>120.178690721871</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C89" s="2">
+        <v>1.613</v>
+      </c>
+      <c r="D89" s="2">
+        <v>123.344741607021</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" s="2">
+        <v>2.61</v>
+      </c>
+      <c r="D90" s="2">
+        <v>113.341644332494</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" s="2">
+        <v>4.53</v>
+      </c>
+      <c r="D91" s="2">
+        <v>125.128287384503</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C92" s="2">
+        <v>4.585</v>
+      </c>
+      <c r="D92" s="2">
+        <v>111.292231416993</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2.171</v>
+      </c>
+      <c r="D93" s="2">
+        <v>116.758422180035</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2.089</v>
+      </c>
+      <c r="D94" s="2">
+        <v>115.281480022734</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2.297</v>
+      </c>
+      <c r="D95" s="2">
+        <v>118.615247747684</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" s="2">
+        <v>4.743</v>
+      </c>
+      <c r="D96" s="2">
+        <v>121.077279787689</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C97" s="2">
+        <v>5.023</v>
+      </c>
+      <c r="D97" s="2">
+        <v>113.341966810433</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C98" s="2">
+        <v>5.825</v>
+      </c>
+      <c r="D98" s="2">
+        <v>123.752309443714</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" s="2">
+        <v>5.499</v>
+      </c>
+      <c r="D99" s="2">
+        <v>113.335312235118</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C100" s="2">
+        <v>5.699</v>
+      </c>
+      <c r="D100" s="2">
+        <v>112.659069083155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C101" s="2">
+        <v>2.997</v>
+      </c>
+      <c r="D101" s="2">
+        <v>120.244510982794</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C102" s="2">
+        <v>5.999</v>
+      </c>
+      <c r="D102" s="2">
+        <v>117.178586943754</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C103" s="2">
         <v>5</v>
       </c>
-      <c r="D87" s="2">
-        <v>121.502960897923</v>
-      </c>
-      <c r="E87" s="2"/>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="4"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
+      <c r="D103" s="2">
+        <v>120.383304199724</v>
+      </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
+      <c r="A104" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C104" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="D104" s="2">
+        <v>120.311825532132</v>
+      </c>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
+      <c r="A105" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C105" s="2">
+        <v>5.1</v>
+      </c>
+      <c r="D105" s="2">
+        <v>115.077469233506</v>
+      </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
+      <c r="A106" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C106" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D106" s="2">
+        <v>114.723826222184</v>
+      </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
+      <c r="A107" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C107" s="2">
+        <v>4.65</v>
+      </c>
+      <c r="D107" s="2">
+        <v>121.243297761316</v>
+      </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
+      <c r="A108" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C108" s="2">
+        <v>6.42</v>
+      </c>
+      <c r="D108" s="2">
+        <v>128.548728992991</v>
+      </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="A109" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C109" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="D109" s="2">
+        <v>121.847468332011</v>
+      </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
+      <c r="A110" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C110" s="2">
+        <v>4.4</v>
+      </c>
+      <c r="D110" s="2">
+        <v>115.228107075058</v>
+      </c>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
+      <c r="A111" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C111" s="2">
+        <v>5</v>
+      </c>
+      <c r="D111" s="2">
+        <v>121.523525722995</v>
+      </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
+      <c r="A112" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C112" s="2">
+        <v>6.94</v>
+      </c>
+      <c r="D112" s="2">
+        <v>120.336526013041</v>
+      </c>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
+      <c r="A113" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C113" s="2">
+        <v>5</v>
+      </c>
+      <c r="D113" s="2">
+        <v>121.570322648168</v>
+      </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4"/>

</xml_diff>

<commit_message>
1. policy 1 shrink market value
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7270"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>code</t>
   </si>
@@ -34,28 +34,28 @@
     <t>瑞丰转债</t>
   </si>
   <si>
-    <t>sz123056</t>
-  </si>
-  <si>
-    <t>雪榕转债</t>
-  </si>
-  <si>
     <t>sz123106</t>
   </si>
   <si>
     <t>正丹转债</t>
   </si>
   <si>
+    <t>sz123010</t>
+  </si>
+  <si>
+    <t>博世转债</t>
+  </si>
+  <si>
     <t>sz123011</t>
   </si>
   <si>
     <t>德尔转债</t>
   </si>
   <si>
-    <t>sz123010</t>
-  </si>
-  <si>
-    <t>博世转债</t>
+    <t>sz123059</t>
+  </si>
+  <si>
+    <t>银信转债</t>
   </si>
   <si>
     <t>sz123039</t>
@@ -64,40 +64,34 @@
     <t>开润转债</t>
   </si>
   <si>
-    <t>sz123063</t>
-  </si>
-  <si>
-    <t>大禹转债</t>
-  </si>
-  <si>
-    <t>sz123059</t>
-  </si>
-  <si>
-    <t>银信转债</t>
-  </si>
-  <si>
-    <t>sz123044</t>
-  </si>
-  <si>
-    <t>红相转债</t>
-  </si>
-  <si>
     <t>sz123082</t>
   </si>
   <si>
     <t>北陆转债</t>
   </si>
   <si>
+    <t>sz123050</t>
+  </si>
+  <si>
+    <t>聚飞转债</t>
+  </si>
+  <si>
     <t>sz123093</t>
   </si>
   <si>
     <t>金陵转债</t>
   </si>
   <si>
-    <t>sz123050</t>
-  </si>
-  <si>
-    <t>聚飞转债</t>
+    <t>sz123116</t>
+  </si>
+  <si>
+    <t>万兴转债</t>
+  </si>
+  <si>
+    <t>sz123061</t>
+  </si>
+  <si>
+    <t>航新转债</t>
   </si>
   <si>
     <t>sz123065</t>
@@ -106,16 +100,10 @@
     <t>宝莱转债</t>
   </si>
   <si>
-    <t>sz123116</t>
-  </si>
-  <si>
-    <t>万兴转债</t>
-  </si>
-  <si>
-    <t>sz123122</t>
-  </si>
-  <si>
-    <t>富瀚转债</t>
+    <t>sz123087</t>
+  </si>
+  <si>
+    <t>明电转债</t>
   </si>
   <si>
     <t>sz123109</t>
@@ -124,42 +112,12 @@
     <t>昌红转债</t>
   </si>
   <si>
-    <t>sz123061</t>
-  </si>
-  <si>
-    <t>航新转债</t>
-  </si>
-  <si>
-    <t>sz123087</t>
-  </si>
-  <si>
-    <t>明电转债</t>
-  </si>
-  <si>
-    <t>sz123132</t>
-  </si>
-  <si>
-    <t>回盛转债</t>
-  </si>
-  <si>
-    <t>sz123129</t>
-  </si>
-  <si>
-    <t>锦鸡转债</t>
-  </si>
-  <si>
     <t>sz123100</t>
   </si>
   <si>
     <t>朗科转债</t>
   </si>
   <si>
-    <t>sz123101</t>
-  </si>
-  <si>
-    <t>拓斯转债</t>
-  </si>
-  <si>
     <t>sz123088</t>
   </si>
   <si>
@@ -172,22 +130,10 @@
     <t>中陆转债</t>
   </si>
   <si>
-    <t>sz123131</t>
-  </si>
-  <si>
-    <t>奥飞转债</t>
-  </si>
-  <si>
-    <t>sz123124</t>
-  </si>
-  <si>
-    <t>晶瑞转2</t>
-  </si>
-  <si>
-    <t>sz123075</t>
-  </si>
-  <si>
-    <t>贝斯转债</t>
+    <t>sz123089</t>
+  </si>
+  <si>
+    <t>九洲转2</t>
   </si>
   <si>
     <t>sz123136</t>
@@ -196,10 +142,10 @@
     <t>城市转债</t>
   </si>
   <si>
-    <t>sz123142</t>
-  </si>
-  <si>
-    <t>申昊转债</t>
+    <t>sz123160</t>
+  </si>
+  <si>
+    <t>泰福转债</t>
   </si>
   <si>
     <t>sz123153</t>
@@ -214,60 +160,36 @@
     <t>宏丰转债</t>
   </si>
   <si>
-    <t>sz123160</t>
-  </si>
-  <si>
-    <t>泰福转债</t>
-  </si>
-  <si>
     <t>sz123127</t>
   </si>
   <si>
     <t>耐普转债</t>
   </si>
   <si>
+    <t>sz123138</t>
+  </si>
+  <si>
+    <t>丝路转债</t>
+  </si>
+  <si>
+    <t>sz123157</t>
+  </si>
+  <si>
+    <t>科蓝转债</t>
+  </si>
+  <si>
+    <t>sz123152</t>
+  </si>
+  <si>
+    <t>润禾转债</t>
+  </si>
+  <si>
     <t>sz123168</t>
   </si>
   <si>
     <t>惠云转债</t>
   </si>
   <si>
-    <t>sz123157</t>
-  </si>
-  <si>
-    <t>科蓝转债</t>
-  </si>
-  <si>
-    <t>sz123138</t>
-  </si>
-  <si>
-    <t>丝路转债</t>
-  </si>
-  <si>
-    <t>sz123154</t>
-  </si>
-  <si>
-    <t>火星转债</t>
-  </si>
-  <si>
-    <t>sz123151</t>
-  </si>
-  <si>
-    <t>康医转债</t>
-  </si>
-  <si>
-    <t>sz123144</t>
-  </si>
-  <si>
-    <t>裕兴转债</t>
-  </si>
-  <si>
-    <t>sz123147</t>
-  </si>
-  <si>
-    <t>中辰转债</t>
-  </si>
-  <si>
     <t>sz123167</t>
   </si>
   <si>
@@ -280,22 +202,10 @@
     <t>侨银转债</t>
   </si>
   <si>
-    <t>sz128063</t>
-  </si>
-  <si>
-    <t>未来转债</t>
-  </si>
-  <si>
-    <t>sz128074</t>
-  </si>
-  <si>
-    <t>游族转债</t>
-  </si>
-  <si>
-    <t>sz127041</t>
-  </si>
-  <si>
-    <t>弘亚转债</t>
+    <t>sz128125</t>
+  </si>
+  <si>
+    <t>华阳转债</t>
   </si>
   <si>
     <t>sz128118</t>
@@ -304,34 +214,16 @@
     <t>瀛通转债</t>
   </si>
   <si>
-    <t>sz128125</t>
-  </si>
-  <si>
-    <t>华阳转债</t>
-  </si>
-  <si>
-    <t>sz127078</t>
-  </si>
-  <si>
-    <t>优彩转债</t>
-  </si>
-  <si>
     <t>sz127079</t>
   </si>
   <si>
     <t>华亚转债</t>
   </si>
   <si>
-    <t>sz128116</t>
-  </si>
-  <si>
-    <t>瑞达转债</t>
-  </si>
-  <si>
-    <t>sz127077</t>
-  </si>
-  <si>
-    <t>华宏转债</t>
+    <t>sz128072</t>
+  </si>
+  <si>
+    <t>翔鹭转债</t>
   </si>
   <si>
     <t>sz128066</t>
@@ -340,36 +232,24 @@
     <t>亚泰转债</t>
   </si>
   <si>
-    <t>sz128072</t>
-  </si>
-  <si>
-    <t>翔鹭转债</t>
-  </si>
-  <si>
     <t>sz128049</t>
   </si>
   <si>
     <t>华源转债</t>
   </si>
   <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
     <t>sz128071</t>
   </si>
   <si>
     <t>合兴转债</t>
   </si>
   <si>
-    <t>sz127051</t>
-  </si>
-  <si>
-    <t>博杰转债</t>
-  </si>
-  <si>
-    <t>sz128117</t>
-  </si>
-  <si>
-    <t>道恩转债</t>
-  </si>
-  <si>
     <t>sz128123</t>
   </si>
   <si>
@@ -382,72 +262,30 @@
     <t>奥佳转债</t>
   </si>
   <si>
+    <t>sz128143</t>
+  </si>
+  <si>
+    <t>锋龙转债</t>
+  </si>
+  <si>
     <t>sz128120</t>
   </si>
   <si>
     <t>联诚转债</t>
   </si>
   <si>
-    <t>sz127035</t>
-  </si>
-  <si>
-    <t>濮耐转债</t>
-  </si>
-  <si>
-    <t>sz127026</t>
-  </si>
-  <si>
-    <t>超声转债</t>
-  </si>
-  <si>
-    <t>sz128143</t>
-  </si>
-  <si>
-    <t>锋龙转债</t>
-  </si>
-  <si>
-    <t>sz127054</t>
-  </si>
-  <si>
-    <t>双箭转债</t>
-  </si>
-  <si>
-    <t>sz127055</t>
-  </si>
-  <si>
-    <t>精装转债</t>
-  </si>
-  <si>
     <t>sz127062</t>
   </si>
   <si>
     <t>垒知转债</t>
   </si>
   <si>
-    <t>sh113589</t>
-  </si>
-  <si>
-    <t>天创转债</t>
-  </si>
-  <si>
     <t>sh113578</t>
   </si>
   <si>
     <t>全筑转债</t>
   </si>
   <si>
-    <t>sh113569</t>
-  </si>
-  <si>
-    <t>科达转债</t>
-  </si>
-  <si>
-    <t>sh113584</t>
-  </si>
-  <si>
-    <t>家悦转债</t>
-  </si>
-  <si>
     <t>sh113608</t>
   </si>
   <si>
@@ -460,34 +298,28 @@
     <t>正川转债</t>
   </si>
   <si>
+    <t>sh113535</t>
+  </si>
+  <si>
+    <t>大业转债</t>
+  </si>
+  <si>
     <t>sh113664</t>
   </si>
   <si>
     <t>大元转债</t>
   </si>
   <si>
-    <t>sh113535</t>
-  </si>
-  <si>
-    <t>大业转债</t>
-  </si>
-  <si>
-    <t>sh113604</t>
-  </si>
-  <si>
-    <t>多伦转债</t>
-  </si>
-  <si>
-    <t>sh113530</t>
-  </si>
-  <si>
-    <t>大丰转债</t>
-  </si>
-  <si>
-    <t>sh113606</t>
-  </si>
-  <si>
-    <t>荣泰转债</t>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <t>纵横转债</t>
+  </si>
+  <si>
+    <t>sh113527</t>
+  </si>
+  <si>
+    <t>维格转债</t>
   </si>
   <si>
     <t>sh113665</t>
@@ -496,36 +328,12 @@
     <t>汇通转债</t>
   </si>
   <si>
-    <t>sh113573</t>
-  </si>
-  <si>
-    <t>纵横转债</t>
-  </si>
-  <si>
-    <t>sh113527</t>
-  </si>
-  <si>
-    <t>维格转债</t>
-  </si>
-  <si>
     <t>sh113593</t>
   </si>
   <si>
     <t>沪工转债</t>
   </si>
   <si>
-    <t>sh113542</t>
-  </si>
-  <si>
-    <t>好客转债</t>
-  </si>
-  <si>
-    <t>sh113519</t>
-  </si>
-  <si>
-    <t>长久转债</t>
-  </si>
-  <si>
     <t>sh113628</t>
   </si>
   <si>
@@ -538,10 +346,16 @@
     <t>豪能转债</t>
   </si>
   <si>
-    <t>sh113601</t>
-  </si>
-  <si>
-    <t>塞力转债</t>
+    <t>sh113600</t>
+  </si>
+  <si>
+    <t>新星转债</t>
+  </si>
+  <si>
+    <t>sh113566</t>
+  </si>
+  <si>
+    <t>翔港转债</t>
   </si>
   <si>
     <t>sh113610</t>
@@ -550,22 +364,16 @@
     <t>灵康转债</t>
   </si>
   <si>
-    <t>sh113566</t>
-  </si>
-  <si>
-    <t>翔港转债</t>
-  </si>
-  <si>
     <t>sh110058</t>
   </si>
   <si>
     <t>永鼎转债</t>
   </si>
   <si>
-    <t>sh113600</t>
-  </si>
-  <si>
-    <t>新星转债</t>
+    <t>sh113524</t>
+  </si>
+  <si>
+    <t>奇精转债</t>
   </si>
   <si>
     <t>sh113532</t>
@@ -586,6 +394,12 @@
     <t>华体转债</t>
   </si>
   <si>
+    <t>sh113597</t>
+  </si>
+  <si>
+    <t>佳力转债</t>
+  </si>
+  <si>
     <t>sh113546</t>
   </si>
   <si>
@@ -598,58 +412,22 @@
     <t>胜达转债</t>
   </si>
   <si>
-    <t>sh113579</t>
-  </si>
-  <si>
-    <t>健友转债</t>
-  </si>
-  <si>
-    <t>sh113625</t>
-  </si>
-  <si>
-    <t>江山转债</t>
-  </si>
-  <si>
-    <t>sh113588</t>
-  </si>
-  <si>
-    <t>润达转债</t>
-  </si>
-  <si>
-    <t>sh113639</t>
-  </si>
-  <si>
-    <t>华正转债</t>
-  </si>
-  <si>
     <t>sh113594</t>
   </si>
   <si>
     <t>淳中转债</t>
   </si>
   <si>
-    <t>sh113638</t>
-  </si>
-  <si>
-    <t>台21转债</t>
-  </si>
-  <si>
     <t>sh113643</t>
   </si>
   <si>
     <t>风语转债</t>
   </si>
   <si>
-    <t>sh113663</t>
-  </si>
-  <si>
-    <t>新化转债</t>
-  </si>
-  <si>
-    <t>sh113657</t>
-  </si>
-  <si>
-    <t>再22转债</t>
+    <t>sh118004</t>
+  </si>
+  <si>
+    <t>博瑞转债</t>
   </si>
   <si>
     <t>sh118029</t>
@@ -658,16 +436,10 @@
     <t>富淼转债</t>
   </si>
   <si>
-    <t>sh118004</t>
-  </si>
-  <si>
-    <t>博瑞转债</t>
-  </si>
-  <si>
-    <t>sh118020</t>
-  </si>
-  <si>
-    <t>芳源转债</t>
+    <t>sh118010</t>
+  </si>
+  <si>
+    <t>洁特转债</t>
   </si>
   <si>
     <t>sh118016</t>
@@ -676,28 +448,34 @@
     <t>京源转债</t>
   </si>
   <si>
-    <t>sh118010</t>
-  </si>
-  <si>
-    <t>洁特转债</t>
-  </si>
-  <si>
     <t>sh118011</t>
   </si>
   <si>
     <t>银微转债</t>
   </si>
   <si>
-    <t>sh118008</t>
-  </si>
-  <si>
-    <t>海优转债</t>
-  </si>
-  <si>
     <t>sh118012</t>
   </si>
   <si>
     <t>微芯转债</t>
+  </si>
+  <si>
+    <t>sh118015</t>
+  </si>
+  <si>
+    <t>芯海转债</t>
+  </si>
+  <si>
+    <t>sh118021</t>
+  </si>
+  <si>
+    <t>新致转债</t>
+  </si>
+  <si>
+    <t>sh118018</t>
+  </si>
+  <si>
+    <t>瑞科转债</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1476,7 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D113"/>
+      <selection activeCell="A2" sqref="A2:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1740,7 +1518,7 @@
         <v>3.4</v>
       </c>
       <c r="D2" s="2">
-        <v>129.775951766309</v>
+        <v>129.76316664172</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -1752,10 +1530,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>5.84</v>
+        <v>3.2</v>
       </c>
       <c r="D3" s="2">
-        <v>120.279602862675</v>
+        <v>125.401219952057</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -1767,10 +1545,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>3.2</v>
+        <v>4.296</v>
       </c>
       <c r="D4" s="2">
-        <v>125.413323324186</v>
+        <v>109.804962560254</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -1785,7 +1563,7 @@
         <v>2.506</v>
       </c>
       <c r="D5" s="2">
-        <v>113.805497355318</v>
+        <v>113.806318834882</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -1797,10 +1575,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>4.296</v>
+        <v>3.912</v>
       </c>
       <c r="D6" s="2">
-        <v>109.806364369788</v>
+        <v>123.187258100764</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -1815,7 +1593,7 @@
         <v>2.217</v>
       </c>
       <c r="D7" s="2">
-        <v>120.482464207574</v>
+        <v>120.478251720559</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -1827,10 +1605,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>6.346</v>
+        <v>4.993</v>
       </c>
       <c r="D8" s="2">
-        <v>125.696979628134</v>
+        <v>120.733946609513</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -1842,10 +1620,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="2">
-        <v>3.912</v>
+        <v>3.746</v>
       </c>
       <c r="D9" s="2">
-        <v>123.182534734273</v>
+        <v>123.150996842618</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -1857,10 +1635,10 @@
         <v>21</v>
       </c>
       <c r="C10" s="2">
-        <v>5.496</v>
+        <v>2.485</v>
       </c>
       <c r="D10" s="2">
-        <v>124.407318432992</v>
+        <v>129.187261590947</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -1872,10 +1650,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="2">
-        <v>4.993</v>
+        <v>3.781</v>
       </c>
       <c r="D11" s="2">
-        <v>120.717906262882</v>
+        <v>121.219314776923</v>
       </c>
       <c r="I11" s="3"/>
     </row>
@@ -1887,10 +1665,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="2">
-        <v>2.485</v>
+        <v>2.496</v>
       </c>
       <c r="D12" s="2">
-        <v>129.190190315899</v>
+        <v>123.634747845875</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1902,10 +1680,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="2">
-        <v>3.746</v>
+        <v>2.188</v>
       </c>
       <c r="D13" s="2">
-        <v>123.12034455477</v>
+        <v>120.417915563804</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -1917,10 +1695,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="2">
-        <v>2.188</v>
+        <v>4.189</v>
       </c>
       <c r="D14" s="2">
-        <v>120.439833970523</v>
+        <v>120.111869693754</v>
       </c>
       <c r="I14" s="3"/>
     </row>
@@ -1932,10 +1710,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="2">
-        <v>3.781</v>
+        <v>4.596</v>
       </c>
       <c r="D15" s="2">
-        <v>121.229735435196</v>
+        <v>120.753599277366</v>
       </c>
       <c r="I15" s="3"/>
     </row>
@@ -1947,10 +1725,10 @@
         <v>33</v>
       </c>
       <c r="C16" s="2">
-        <v>5.806</v>
+        <v>3.797</v>
       </c>
       <c r="D16" s="2">
-        <v>120.182520445783</v>
+        <v>117.236997790117</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -1962,10 +1740,10 @@
         <v>35</v>
       </c>
       <c r="C17" s="2">
-        <v>4.596</v>
+        <v>3.011</v>
       </c>
       <c r="D17" s="2">
-        <v>120.739367943445</v>
+        <v>120.47916486129</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -1977,10 +1755,10 @@
         <v>37</v>
       </c>
       <c r="C18" s="2">
-        <v>2.496</v>
+        <v>3.6</v>
       </c>
       <c r="D18" s="2">
-        <v>123.579781993773</v>
+        <v>121.708027083837</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -1992,10 +1770,10 @@
         <v>39</v>
       </c>
       <c r="C19" s="2">
-        <v>4.189</v>
+        <v>3.062</v>
       </c>
       <c r="D19" s="2">
-        <v>120.11591490354</v>
+        <v>120.012593383832</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -2007,10 +1785,10 @@
         <v>41</v>
       </c>
       <c r="C20" s="2">
-        <v>7</v>
+        <v>4.595</v>
       </c>
       <c r="D20" s="2">
-        <v>120.790615461815</v>
+        <v>120.834641307683</v>
       </c>
       <c r="I20" s="3"/>
     </row>
@@ -2022,10 +1800,10 @@
         <v>43</v>
       </c>
       <c r="C21" s="2">
-        <v>6</v>
+        <v>3.349</v>
       </c>
       <c r="D21" s="2">
-        <v>117.547832115359</v>
+        <v>121.653710450319</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -2037,10 +1815,10 @@
         <v>45</v>
       </c>
       <c r="C22" s="2">
-        <v>3.797</v>
+        <v>3.4</v>
       </c>
       <c r="D22" s="2">
-        <v>117.197375594109</v>
+        <v>121.647462154123</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -2052,10 +1830,10 @@
         <v>47</v>
       </c>
       <c r="C23" s="2">
-        <v>6.698</v>
+        <v>3.212</v>
       </c>
       <c r="D23" s="2">
-        <v>114.893447064604</v>
+        <v>121.820741939106</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -2067,10 +1845,10 @@
         <v>49</v>
       </c>
       <c r="C24" s="2">
-        <v>3.011</v>
+        <v>3.999</v>
       </c>
       <c r="D24" s="2">
-        <v>120.490423955852</v>
+        <v>115.8500233387</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -2082,10 +1860,10 @@
         <v>51</v>
       </c>
       <c r="C25" s="2">
-        <v>3.6</v>
+        <v>2.4</v>
       </c>
       <c r="D25" s="2">
-        <v>121.727804581142</v>
+        <v>121.806488786687</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -2097,10 +1875,10 @@
         <v>53</v>
       </c>
       <c r="C26" s="2">
-        <v>6.35</v>
+        <v>4.946</v>
       </c>
       <c r="D26" s="2">
-        <v>121.310550578895</v>
+        <v>120.394088888362</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2112,10 +1890,10 @@
         <v>55</v>
       </c>
       <c r="C27" s="2">
-        <v>5.228</v>
+        <v>2.92</v>
       </c>
       <c r="D27" s="2">
-        <v>111.042019832169</v>
+        <v>124.644309932764</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2127,10 +1905,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="2">
-        <v>5.996</v>
+        <v>4.9</v>
       </c>
       <c r="D28" s="2">
-        <v>114.529078733487</v>
+        <v>120.783694412345</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2142,10 +1920,10 @@
         <v>59</v>
       </c>
       <c r="C29" s="2">
-        <v>4.595</v>
+        <v>3.965</v>
       </c>
       <c r="D29" s="2">
-        <v>120.798814397604</v>
+        <v>121.58395243433</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2157,10 +1935,10 @@
         <v>61</v>
       </c>
       <c r="C30" s="2">
-        <v>5.497</v>
+        <v>4.199</v>
       </c>
       <c r="D30" s="2">
-        <v>116.108876217728</v>
+        <v>135.945079123204</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2172,10 +1950,10 @@
         <v>63</v>
       </c>
       <c r="C31" s="2">
-        <v>3.4</v>
+        <v>4.498</v>
       </c>
       <c r="D31" s="2">
-        <v>121.672539737941</v>
+        <v>117.772058183503</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2187,10 +1965,10 @@
         <v>65</v>
       </c>
       <c r="C32" s="2">
-        <v>3.212</v>
+        <v>2.996</v>
       </c>
       <c r="D32" s="2">
-        <v>121.815195216999</v>
+        <v>121.344176916595</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -2202,10 +1980,10 @@
         <v>67</v>
       </c>
       <c r="C33" s="2">
-        <v>3.349</v>
+        <v>3.4</v>
       </c>
       <c r="D33" s="2">
-        <v>121.678844361975</v>
+        <v>121.66324795478</v>
       </c>
       <c r="I33" s="3"/>
     </row>
@@ -2217,10 +1995,10 @@
         <v>69</v>
       </c>
       <c r="C34" s="2">
-        <v>3.999</v>
+        <v>3.017</v>
       </c>
       <c r="D34" s="2">
-        <v>115.837920142942</v>
+        <v>113.587744734612</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -2232,10 +2010,10 @@
         <v>71</v>
       </c>
       <c r="C35" s="2">
-        <v>4.9</v>
+        <v>4.61</v>
       </c>
       <c r="D35" s="2">
-        <v>120.803856366434</v>
+        <v>115.579851193076</v>
       </c>
       <c r="I35" s="3"/>
     </row>
@@ -2247,10 +2025,10 @@
         <v>73</v>
       </c>
       <c r="C36" s="2">
-        <v>4.946</v>
+        <v>3.631</v>
       </c>
       <c r="D36" s="2">
-        <v>120.357335457746</v>
+        <v>112.02090025084</v>
       </c>
       <c r="I36" s="3"/>
     </row>
@@ -2262,10 +2040,10 @@
         <v>75</v>
       </c>
       <c r="C37" s="2">
-        <v>2.4</v>
+        <v>3.586</v>
       </c>
       <c r="D37" s="2">
-        <v>121.750966520842</v>
+        <v>122.658596760807</v>
       </c>
       <c r="I37" s="3"/>
     </row>
@@ -2277,10 +2055,10 @@
         <v>77</v>
       </c>
       <c r="C38" s="2">
-        <v>5.29</v>
+        <v>2.999</v>
       </c>
       <c r="D38" s="2">
-        <v>120.343475609508</v>
+        <v>113.360890668105</v>
       </c>
       <c r="I38" s="3"/>
     </row>
@@ -2292,10 +2070,10 @@
         <v>79</v>
       </c>
       <c r="C39" s="2">
-        <v>7</v>
+        <v>3.199</v>
       </c>
       <c r="D39" s="2">
-        <v>121.61875945595</v>
+        <v>115.111794762512</v>
       </c>
       <c r="I39" s="3"/>
     </row>
@@ -2307,10 +2085,10 @@
         <v>81</v>
       </c>
       <c r="C40" s="2">
-        <v>6</v>
+        <v>4.585</v>
       </c>
       <c r="D40" s="2">
-        <v>120.33721879917</v>
+        <v>114.365488521304</v>
       </c>
       <c r="I40" s="3"/>
     </row>
@@ -2322,10 +2100,10 @@
         <v>83</v>
       </c>
       <c r="C41" s="2">
-        <v>5.705</v>
+        <v>2.441</v>
       </c>
       <c r="D41" s="2">
-        <v>120.125083415283</v>
+        <v>121.33075452544</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2336,10 +2114,10 @@
         <v>85</v>
       </c>
       <c r="C42" s="2">
-        <v>3.965</v>
+        <v>2.598</v>
       </c>
       <c r="D42" s="2">
-        <v>121.518728525994</v>
+        <v>117.262056763633</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2350,10 +2128,10 @@
         <v>87</v>
       </c>
       <c r="C43" s="2">
-        <v>4.199</v>
+        <v>3.962</v>
       </c>
       <c r="D43" s="2">
-        <v>135.896704725403</v>
+        <v>120.624790337788</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2364,10 +2142,10 @@
         <v>89</v>
       </c>
       <c r="C44" s="2">
-        <v>6.292</v>
+        <v>3.838</v>
       </c>
       <c r="D44" s="2">
-        <v>126.285924954847</v>
+        <v>117.692691567851</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2378,10 +2156,10 @@
         <v>91</v>
       </c>
       <c r="C45" s="2">
-        <v>6.825</v>
+        <v>4.2</v>
       </c>
       <c r="D45" s="2">
-        <v>118.450505960349</v>
+        <v>120.758632956399</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2392,10 +2170,10 @@
         <v>93</v>
       </c>
       <c r="C46" s="2">
-        <v>5.999</v>
+        <v>4.049</v>
       </c>
       <c r="D46" s="2">
-        <v>118.454977941225</v>
+        <v>121.50256384254</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2406,10 +2184,10 @@
         <v>95</v>
       </c>
       <c r="C47" s="2">
-        <v>2.996</v>
+        <v>4.996</v>
       </c>
       <c r="D47" s="2">
-        <v>121.33880822345</v>
+        <v>111.515610846578</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2420,10 +2198,10 @@
         <v>97</v>
       </c>
       <c r="C48" s="2">
-        <v>4.498</v>
+        <v>4.5</v>
       </c>
       <c r="D48" s="2">
-        <v>117.731624487481</v>
+        <v>121.415555854299</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2434,10 +2212,10 @@
         <v>99</v>
       </c>
       <c r="C49" s="2">
-        <v>6</v>
+        <v>2.698</v>
       </c>
       <c r="D49" s="2">
-        <v>122.016076420943</v>
+        <v>123.772326114032</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2448,10 +2226,10 @@
         <v>101</v>
       </c>
       <c r="C50" s="2">
-        <v>3.4</v>
+        <v>2.862</v>
       </c>
       <c r="D50" s="2">
-        <v>121.687162654827</v>
+        <v>118.582071117832</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2462,10 +2240,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="2">
-        <v>6.491</v>
+        <v>3.6</v>
       </c>
       <c r="D51" s="2">
-        <v>114.618168977266</v>
+        <v>120.672267353831</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2476,10 +2254,10 @@
         <v>105</v>
       </c>
       <c r="C52" s="2">
-        <v>5.15</v>
+        <v>3.998</v>
       </c>
       <c r="D52" s="2">
-        <v>121.321903047271</v>
+        <v>120.867611688206</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2490,10 +2268,10 @@
         <v>107</v>
       </c>
       <c r="C53" s="2">
-        <v>4.611</v>
+        <v>4.15</v>
       </c>
       <c r="D53" s="2">
-        <v>115.583637604527</v>
+        <v>121.553985749427</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2504,10 +2282,10 @@
         <v>109</v>
       </c>
       <c r="C54" s="2">
-        <v>3.017</v>
+        <v>5</v>
       </c>
       <c r="D54" s="2">
-        <v>113.591931881949</v>
+        <v>118.334188164411</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2518,10 +2296,10 @@
         <v>111</v>
       </c>
       <c r="C55" s="2">
-        <v>3.631</v>
+        <v>4.53</v>
       </c>
       <c r="D55" s="2">
-        <v>112.0027948355</v>
+        <v>125.19376818464</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2532,10 +2310,10 @@
         <v>113</v>
       </c>
       <c r="C56" s="2">
-        <v>2.999</v>
+        <v>1.613</v>
       </c>
       <c r="D56" s="2">
-        <v>113.343063522845</v>
+        <v>123.367511808638</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2546,10 +2324,10 @@
         <v>115</v>
       </c>
       <c r="C57" s="2">
-        <v>5.259</v>
+        <v>4.579</v>
       </c>
       <c r="D57" s="2">
-        <v>120.988517612503</v>
+        <v>120.202129721351</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2560,10 +2338,10 @@
         <v>117</v>
       </c>
       <c r="C58" s="2">
-        <v>3.586</v>
+        <v>2.61</v>
       </c>
       <c r="D58" s="2">
-        <v>122.605621389474</v>
+        <v>113.334750794027</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2574,10 +2352,10 @@
         <v>119</v>
       </c>
       <c r="C59" s="2">
-        <v>3.199</v>
+        <v>3.297</v>
       </c>
       <c r="D59" s="2">
-        <v>115.118027966129</v>
+        <v>114.8044105367</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2591,7 +2369,7 @@
         <v>4.585</v>
       </c>
       <c r="D60" s="2">
-        <v>114.328048264931</v>
+        <v>111.329321179521</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2602,10 +2380,10 @@
         <v>123</v>
       </c>
       <c r="C61" s="2">
-        <v>2.598</v>
+        <v>2.171</v>
       </c>
       <c r="D61" s="2">
-        <v>117.242648272933</v>
+        <v>116.790527112932</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2616,10 +2394,10 @@
         <v>125</v>
       </c>
       <c r="C62" s="2">
-        <v>6.262</v>
+        <v>2.089</v>
       </c>
       <c r="D62" s="2">
-        <v>114.1078787666</v>
+        <v>115.276598306457</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2630,10 +2408,10 @@
         <v>127</v>
       </c>
       <c r="C63" s="2">
-        <v>6.997</v>
+        <v>2.982</v>
       </c>
       <c r="D63" s="2">
-        <v>112.335093234604</v>
+        <v>123.385593396095</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2644,10 +2422,10 @@
         <v>129</v>
       </c>
       <c r="C64" s="2">
-        <v>2.441</v>
+        <v>2.297</v>
       </c>
       <c r="D64" s="2">
-        <v>121.299882377375</v>
+        <v>118.604888153986</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2658,10 +2436,10 @@
         <v>131</v>
       </c>
       <c r="C65" s="2">
-        <v>5.136</v>
+        <v>4.743</v>
       </c>
       <c r="D65" s="2">
-        <v>117.223711274716</v>
+        <v>121.085182249007</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2672,10 +2450,10 @@
         <v>133</v>
       </c>
       <c r="C66" s="2">
-        <v>5.768</v>
+        <v>2.997</v>
       </c>
       <c r="D66" s="2">
-        <v>120.434961602486</v>
+        <v>120.256031610811</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2686,10 +2464,10 @@
         <v>135</v>
       </c>
       <c r="C67" s="2">
-        <v>3.962</v>
+        <v>5</v>
       </c>
       <c r="D67" s="2">
-        <v>120.576345498157</v>
+        <v>120.406780591333</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2700,10 +2478,10 @@
         <v>137</v>
       </c>
       <c r="C68" s="2">
-        <v>5.996</v>
+        <v>4.65</v>
       </c>
       <c r="D68" s="2">
-        <v>114.728399925257</v>
+        <v>121.292762582372</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2714,10 +2492,10 @@
         <v>139</v>
       </c>
       <c r="C69" s="2">
-        <v>3.838</v>
+        <v>4.5</v>
       </c>
       <c r="D69" s="2">
-        <v>117.681987352817</v>
+        <v>114.710671038184</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2728,10 +2506,10 @@
         <v>141</v>
       </c>
       <c r="C70" s="2">
-        <v>5.156</v>
+        <v>4.4</v>
       </c>
       <c r="D70" s="2">
-        <v>119.887253060459</v>
+        <v>115.222202479935</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2742,10 +2520,10 @@
         <v>143</v>
       </c>
       <c r="C71" s="2">
-        <v>6.449</v>
+        <v>3.33</v>
       </c>
       <c r="D71" s="2">
-        <v>114.590728794408</v>
+        <v>121.870177720954</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2756,10 +2534,10 @@
         <v>145</v>
       </c>
       <c r="C72" s="2">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="D72" s="2">
-        <v>120.748956704197</v>
+        <v>121.541502596678</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2770,10 +2548,10 @@
         <v>147</v>
       </c>
       <c r="C73" s="2">
-        <v>4.049</v>
+        <v>5</v>
       </c>
       <c r="D73" s="2">
-        <v>121.508660437695</v>
+        <v>121.578285123304</v>
       </c>
       <c r="E73" s="4"/>
     </row>
@@ -2785,10 +2563,10 @@
         <v>149</v>
       </c>
       <c r="C74" s="2">
-        <v>4.5</v>
+        <v>4.1</v>
       </c>
       <c r="D74" s="2">
-        <v>121.435326339034</v>
+        <v>121.556277443612</v>
       </c>
       <c r="E74" s="4"/>
     </row>
@@ -2800,10 +2578,10 @@
         <v>151</v>
       </c>
       <c r="C75" s="2">
-        <v>4.996</v>
+        <v>4.85</v>
       </c>
       <c r="D75" s="2">
-        <v>111.519834923959</v>
+        <v>118.264361543614</v>
       </c>
       <c r="E75" s="4"/>
     </row>
@@ -2815,541 +2593,245 @@
         <v>153</v>
       </c>
       <c r="C76" s="2">
-        <v>6.398</v>
+        <v>4.3</v>
       </c>
       <c r="D76" s="2">
-        <v>116.524579871644</v>
+        <v>114.516772025331</v>
       </c>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="2">
-        <v>6.297</v>
-      </c>
-      <c r="D77" s="2">
-        <v>120.12028224046</v>
-      </c>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
       <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C78" s="2">
-        <v>5.999</v>
-      </c>
-      <c r="D78" s="2">
-        <v>120.242382218536</v>
-      </c>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
       <c r="E78" s="4"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C79" s="2">
-        <v>3.6</v>
-      </c>
-      <c r="D79" s="2">
-        <v>120.691215451086</v>
-      </c>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
       <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C80" s="2">
-        <v>2.698</v>
-      </c>
-      <c r="D80" s="2">
-        <v>123.733458503589</v>
-      </c>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
       <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C81" s="2">
-        <v>2.862</v>
-      </c>
-      <c r="D81" s="2">
-        <v>118.587534861657</v>
-      </c>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
       <c r="E81" s="4"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C82" s="2">
-        <v>3.998</v>
-      </c>
-      <c r="D82" s="2">
-        <v>120.849900705582</v>
-      </c>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
       <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C83" s="2">
-        <v>6.026</v>
-      </c>
-      <c r="D83" s="2">
-        <v>113.37813849384</v>
-      </c>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
       <c r="E83" s="4"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C84" s="2">
-        <v>6.961</v>
-      </c>
-      <c r="D84" s="2">
-        <v>116.819633731372</v>
-      </c>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" s="2">
-        <v>4.15</v>
-      </c>
-      <c r="D85" s="2">
-        <v>121.522778661912</v>
-      </c>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C86" s="2">
-        <v>5</v>
-      </c>
-      <c r="D86" s="2">
-        <v>118.282741592876</v>
-      </c>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
       <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C87" s="2">
-        <v>5.425</v>
-      </c>
-      <c r="D87" s="2">
-        <v>120.192537966406</v>
-      </c>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="2">
-        <v>4.579</v>
-      </c>
-      <c r="D88" s="2">
-        <v>120.178690721871</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="2">
-        <v>1.613</v>
-      </c>
-      <c r="D89" s="2">
-        <v>123.344741607021</v>
-      </c>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C90" s="2">
-        <v>2.61</v>
-      </c>
-      <c r="D90" s="2">
-        <v>113.341644332494</v>
-      </c>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C91" s="2">
-        <v>4.53</v>
-      </c>
-      <c r="D91" s="2">
-        <v>125.128287384503</v>
-      </c>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C92" s="2">
-        <v>4.585</v>
-      </c>
-      <c r="D92" s="2">
-        <v>111.292231416993</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C93" s="2">
-        <v>2.171</v>
-      </c>
-      <c r="D93" s="2">
-        <v>116.758422180035</v>
-      </c>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C94" s="2">
-        <v>2.089</v>
-      </c>
-      <c r="D94" s="2">
-        <v>115.281480022734</v>
-      </c>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C95" s="2">
-        <v>2.297</v>
-      </c>
-      <c r="D95" s="2">
-        <v>118.615247747684</v>
-      </c>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C96" s="2">
-        <v>4.743</v>
-      </c>
-      <c r="D96" s="2">
-        <v>121.077279787689</v>
-      </c>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C97" s="2">
-        <v>5.023</v>
-      </c>
-      <c r="D97" s="2">
-        <v>113.341966810433</v>
-      </c>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C98" s="2">
-        <v>5.825</v>
-      </c>
-      <c r="D98" s="2">
-        <v>123.752309443714</v>
-      </c>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C99" s="2">
-        <v>5.499</v>
-      </c>
-      <c r="D99" s="2">
-        <v>113.335312235118</v>
-      </c>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C100" s="2">
-        <v>5.699</v>
-      </c>
-      <c r="D100" s="2">
-        <v>112.659069083155</v>
-      </c>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C101" s="2">
-        <v>2.997</v>
-      </c>
-      <c r="D101" s="2">
-        <v>120.244510982794</v>
-      </c>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C102" s="2">
-        <v>5.999</v>
-      </c>
-      <c r="D102" s="2">
-        <v>117.178586943754</v>
-      </c>
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C103" s="2">
-        <v>5</v>
-      </c>
-      <c r="D103" s="2">
-        <v>120.383304199724</v>
-      </c>
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C104" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="D104" s="2">
-        <v>120.311825532132</v>
-      </c>
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C105" s="2">
-        <v>5.1</v>
-      </c>
-      <c r="D105" s="2">
-        <v>115.077469233506</v>
-      </c>
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C106" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="D106" s="2">
-        <v>114.723826222184</v>
-      </c>
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C107" s="2">
-        <v>4.65</v>
-      </c>
-      <c r="D107" s="2">
-        <v>121.243297761316</v>
-      </c>
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C108" s="2">
-        <v>6.42</v>
-      </c>
-      <c r="D108" s="2">
-        <v>128.548728992991</v>
-      </c>
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C109" s="2">
-        <v>3.33</v>
-      </c>
-      <c r="D109" s="2">
-        <v>121.847468332011</v>
-      </c>
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C110" s="2">
-        <v>4.4</v>
-      </c>
-      <c r="D110" s="2">
-        <v>115.228107075058</v>
-      </c>
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C111" s="2">
-        <v>5</v>
-      </c>
-      <c r="D111" s="2">
-        <v>121.523525722995</v>
-      </c>
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C112" s="2">
-        <v>6.94</v>
-      </c>
-      <c r="D112" s="2">
-        <v>120.336526013041</v>
-      </c>
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C113" s="2">
-        <v>5</v>
-      </c>
-      <c r="D113" s="2">
-        <v>121.570322648168</v>
-      </c>
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4"/>

</xml_diff>

<commit_message>
1.add some in kgoodlist
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7270"/>
+    <workbookView windowWidth="18350" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>code</t>
   </si>
@@ -37,6 +37,12 @@
     <t>侨银转债</t>
   </si>
   <si>
+    <t>sh113610</t>
+  </si>
+  <si>
+    <t>灵康转债</t>
+  </si>
+  <si>
     <t>sz123126</t>
   </si>
   <si>
@@ -55,64 +61,88 @@
     <t>正川转债</t>
   </si>
   <si>
-    <t>sh113610</t>
-  </si>
-  <si>
-    <t>灵康转债</t>
-  </si>
-  <si>
     <t>sz123106</t>
   </si>
   <si>
     <t>正丹转债</t>
   </si>
   <si>
+    <t>sz128118</t>
+  </si>
+  <si>
+    <t>瀛通转债</t>
+  </si>
+  <si>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>中陆转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
+  </si>
+  <si>
+    <t>sh118010</t>
+  </si>
+  <si>
+    <t>洁特转债</t>
+  </si>
+  <si>
+    <t>sh118004</t>
+  </si>
+  <si>
+    <t>博瑞转债</t>
+  </si>
+  <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
+    <t>sh113593</t>
+  </si>
+  <si>
+    <t>沪工转债</t>
+  </si>
+  <si>
     <t>sz128125</t>
   </si>
   <si>
     <t>华阳转债</t>
   </si>
   <si>
-    <t>sz128118</t>
-  </si>
-  <si>
-    <t>瀛通转债</t>
-  </si>
-  <si>
-    <t>sh113593</t>
-  </si>
-  <si>
-    <t>沪工转债</t>
-  </si>
-  <si>
-    <t>sz128117</t>
-  </si>
-  <si>
-    <t>道恩转债</t>
-  </si>
-  <si>
-    <t>sh113600</t>
-  </si>
-  <si>
-    <t>新星转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
-  </si>
-  <si>
     <t>sh113573</t>
   </si>
   <si>
     <t>纵横转债</t>
   </si>
   <si>
-    <t>sh118004</t>
-  </si>
-  <si>
-    <t>博瑞转债</t>
+    <t>sh118015</t>
+  </si>
+  <si>
+    <t>芯海转债</t>
+  </si>
+  <si>
+    <t>sz123103</t>
+  </si>
+  <si>
+    <t>震安转债</t>
+  </si>
+  <si>
+    <t>sz127059</t>
+  </si>
+  <si>
+    <t>永东转2</t>
   </si>
   <si>
     <t>sz123039</t>
@@ -121,10 +151,22 @@
     <t>开润转债</t>
   </si>
   <si>
-    <t>sh113628</t>
-  </si>
-  <si>
-    <t>晨丰转债</t>
+    <t>sh118006</t>
+  </si>
+  <si>
+    <t>阿拉转债</t>
+  </si>
+  <si>
+    <t>sh113618</t>
+  </si>
+  <si>
+    <t>美诺转债</t>
+  </si>
+  <si>
+    <t>sz127062</t>
+  </si>
+  <si>
+    <t>垒知转债</t>
   </si>
   <si>
     <t>sz123065</t>
@@ -133,52 +175,94 @@
     <t>宝莱转债</t>
   </si>
   <si>
+    <t>sh118016</t>
+  </si>
+  <si>
+    <t>京源转债</t>
+  </si>
+  <si>
+    <t>sz123153</t>
+  </si>
+  <si>
+    <t>英力转债</t>
+  </si>
+  <si>
+    <t>sh118012</t>
+  </si>
+  <si>
+    <t>微芯转债</t>
+  </si>
+  <si>
+    <t>sz123090</t>
+  </si>
+  <si>
+    <t>三诺转债</t>
+  </si>
+  <si>
+    <t>sh118011</t>
+  </si>
+  <si>
+    <t>银微转债</t>
+  </si>
+  <si>
+    <t>sz123100</t>
+  </si>
+  <si>
+    <t>朗科转债</t>
+  </si>
+  <si>
+    <t>sz123088</t>
+  </si>
+  <si>
+    <t>威唐转债</t>
+  </si>
+  <si>
+    <t>sh113649</t>
+  </si>
+  <si>
+    <t>丰山转债</t>
+  </si>
+  <si>
+    <t>sh118018</t>
+  </si>
+  <si>
+    <t>瑞科转债</t>
+  </si>
+  <si>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>华体转债</t>
+  </si>
+  <si>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>奥佳转债</t>
+  </si>
+  <si>
+    <t>sh118014</t>
+  </si>
+  <si>
+    <t>高测转债</t>
+  </si>
+  <si>
     <t>sz128123</t>
   </si>
   <si>
     <t>国光转债</t>
   </si>
   <si>
-    <t>sz127059</t>
-  </si>
-  <si>
-    <t>永东转2</t>
-  </si>
-  <si>
-    <t>sz123109</t>
-  </si>
-  <si>
-    <t>昌红转债</t>
-  </si>
-  <si>
-    <t>sz123088</t>
-  </si>
-  <si>
-    <t>威唐转债</t>
-  </si>
-  <si>
-    <t>sz128066</t>
-  </si>
-  <si>
-    <t>亚泰转债</t>
-  </si>
-  <si>
-    <t>sz123100</t>
-  </si>
-  <si>
-    <t>朗科转债</t>
-  </si>
-  <si>
-    <t>sz128072</t>
-  </si>
-  <si>
-    <t>翔鹭转债</t>
-  </si>
-  <si>
-    <t>sh113574</t>
-  </si>
-  <si>
-    <t>华体转债</t>
+    <t>sh113030</t>
+  </si>
+  <si>
+    <t>东风转债</t>
+  </si>
+  <si>
+    <t>sh113565</t>
+  </si>
+  <si>
+    <t>宏辉转债</t>
   </si>
   <si>
     <t>sh110070</t>
@@ -187,28 +271,16 @@
     <t>凌钢转债</t>
   </si>
   <si>
-    <t>sz128071</t>
-  </si>
-  <si>
-    <t>合兴转债</t>
-  </si>
-  <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
-  </si>
-  <si>
-    <t>sz128097</t>
-  </si>
-  <si>
-    <t>奥佳转债</t>
+    <t>sz128074</t>
+  </si>
+  <si>
+    <t>游族转债</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -237,34 +309,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -278,14 +322,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,6 +361,21 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -375,7 +426,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,49 +462,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,121 +600,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,21 +667,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,6 +700,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,148 +771,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -855,52 +927,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1200,10 +1272,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J132"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1247,10 +1319,10 @@
         <v>4.199</v>
       </c>
       <c r="D2" s="2">
-        <v>135.91468736394</v>
+        <v>135.982404705242</v>
       </c>
       <c r="E2" s="2">
-        <v>3.603</v>
+        <v>3.195</v>
       </c>
       <c r="I2" s="4"/>
     </row>
@@ -1262,13 +1334,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>3.4</v>
+        <v>4.579</v>
       </c>
       <c r="D3" s="2">
-        <v>129.688878291263</v>
+        <v>120.330281436165</v>
       </c>
       <c r="E3" s="2">
-        <v>4.419</v>
+        <v>3.233</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -1280,13 +1352,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="D4" s="2">
-        <v>120.658565128376</v>
+        <v>129.756562623298</v>
       </c>
       <c r="E4" s="2">
-        <v>3.581</v>
+        <v>4.008</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -1298,13 +1370,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>4.049</v>
+        <v>4.2</v>
       </c>
       <c r="D5" s="2">
-        <v>121.426901717032</v>
+        <v>120.711752097152</v>
       </c>
       <c r="E5" s="2">
-        <v>4.047</v>
+        <v>3.173</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -1316,13 +1388,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>4.579</v>
+        <v>4.049</v>
       </c>
       <c r="D6" s="2">
-        <v>120.198179200499</v>
+        <v>120.725334314585</v>
       </c>
       <c r="E6" s="2">
-        <v>3.641</v>
+        <v>3.638</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -1337,10 +1409,10 @@
         <v>3.2</v>
       </c>
       <c r="D7" s="2">
-        <v>124.669854957655</v>
+        <v>124.705877079236</v>
       </c>
       <c r="E7" s="2">
-        <v>3.951</v>
+        <v>3.543</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -1352,13 +1424,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>4.498</v>
+        <v>2.996</v>
       </c>
       <c r="D8" s="2">
-        <v>117.663418164897</v>
+        <v>119.942740346496</v>
       </c>
       <c r="E8" s="2">
-        <v>3.301</v>
+        <v>2.816</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -1370,13 +1442,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>2.996</v>
+        <v>3.6</v>
       </c>
       <c r="D9" s="2">
-        <v>121.178760416809</v>
+        <v>121.351195624862</v>
       </c>
       <c r="E9" s="2">
-        <v>3.225</v>
+        <v>4.932</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -1388,13 +1460,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>3.998</v>
+        <v>4.993</v>
       </c>
       <c r="D10" s="2">
-        <v>120.762416907872</v>
+        <v>120.684096254828</v>
       </c>
       <c r="E10" s="2">
-        <v>3.274</v>
+        <v>3.249</v>
       </c>
       <c r="I10" s="4"/>
     </row>
@@ -1406,13 +1478,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>3.585</v>
+        <v>4.595</v>
       </c>
       <c r="D11" s="2">
-        <v>122.593974581931</v>
+        <v>120.165677604251</v>
       </c>
       <c r="E11" s="2">
-        <v>3.225</v>
+        <v>3.564</v>
       </c>
       <c r="I11" s="4"/>
     </row>
@@ -1424,13 +1496,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>4.53</v>
+        <v>4.4</v>
       </c>
       <c r="D12" s="2">
-        <v>125.104684139965</v>
+        <v>114.975333122115</v>
       </c>
       <c r="E12" s="2">
-        <v>3.34</v>
+        <v>4.808</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -1442,13 +1514,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>4.993</v>
+        <v>4.65</v>
       </c>
       <c r="D13" s="2">
-        <v>120.613849127649</v>
+        <v>120.826564594299</v>
       </c>
       <c r="E13" s="2">
-        <v>3.658</v>
+        <v>4.326</v>
       </c>
       <c r="I13" s="4"/>
     </row>
@@ -1460,13 +1532,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>2.698</v>
+        <v>3.584</v>
       </c>
       <c r="D14" s="2">
-        <v>123.625445109461</v>
+        <v>121.595248057558</v>
       </c>
       <c r="E14" s="2">
-        <v>3.016</v>
+        <v>2.816</v>
       </c>
       <c r="I14" s="4"/>
     </row>
@@ -1478,13 +1550,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>4.65</v>
+        <v>3.997</v>
       </c>
       <c r="D15" s="2">
-        <v>120.700947678509</v>
+        <v>119.504406991155</v>
       </c>
       <c r="E15" s="2">
-        <v>4.737</v>
+        <v>2.866</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -1496,13 +1568,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>2.217</v>
+        <v>4.498</v>
       </c>
       <c r="D16" s="2">
-        <v>119.156804218491</v>
+        <v>116.59129074623</v>
       </c>
       <c r="E16" s="2">
-        <v>2.71</v>
+        <v>2.893</v>
       </c>
       <c r="I16" s="4"/>
     </row>
@@ -1514,13 +1586,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="2">
-        <v>4.15</v>
+        <v>2.698</v>
       </c>
       <c r="D17" s="2">
-        <v>121.283316136986</v>
+        <v>122.401266004354</v>
       </c>
       <c r="E17" s="2">
-        <v>4.37</v>
+        <v>2.608</v>
       </c>
       <c r="I17" s="4"/>
     </row>
@@ -1532,13 +1604,13 @@
         <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>2.188</v>
+        <v>4.1</v>
       </c>
       <c r="D18" s="2">
-        <v>120.363905984605</v>
+        <v>121.273012018076</v>
       </c>
       <c r="E18" s="2">
-        <v>3.4</v>
+        <v>4.871</v>
       </c>
       <c r="I18" s="4"/>
     </row>
@@ -1550,13 +1622,13 @@
         <v>40</v>
       </c>
       <c r="C19" s="2">
-        <v>3.199</v>
+        <v>2.494</v>
       </c>
       <c r="D19" s="2">
-        <v>115.014827560864</v>
+        <v>120.307661557063</v>
       </c>
       <c r="E19" s="2">
-        <v>3.293</v>
+        <v>3.51</v>
       </c>
       <c r="I19" s="4"/>
     </row>
@@ -1571,10 +1643,10 @@
         <v>3.792</v>
       </c>
       <c r="D20" s="2">
-        <v>120.111770714182</v>
+        <v>120.185685023187</v>
       </c>
       <c r="E20" s="2">
-        <v>4.997</v>
+        <v>4.586</v>
       </c>
       <c r="I20" s="4"/>
     </row>
@@ -1586,13 +1658,13 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>4.596</v>
+        <v>2.216</v>
       </c>
       <c r="D21" s="2">
-        <v>120.020506477889</v>
+        <v>119.144655388885</v>
       </c>
       <c r="E21" s="2">
-        <v>3.973</v>
+        <v>2.301</v>
       </c>
       <c r="I21" s="4"/>
     </row>
@@ -1604,13 +1676,13 @@
         <v>46</v>
       </c>
       <c r="C22" s="2">
-        <v>3.011</v>
+        <v>3.871</v>
       </c>
       <c r="D22" s="2">
-        <v>120.39154266428</v>
+        <v>121.308148653974</v>
       </c>
       <c r="E22" s="2">
-        <v>3.679</v>
+        <v>4.521</v>
       </c>
       <c r="I22" s="4"/>
     </row>
@@ -1622,13 +1694,13 @@
         <v>48</v>
       </c>
       <c r="C23" s="2">
-        <v>4.61</v>
+        <v>4.767</v>
       </c>
       <c r="D23" s="2">
-        <v>115.504584718195</v>
+        <v>114.383613848105</v>
       </c>
       <c r="E23" s="2">
-        <v>2.019</v>
+        <v>3.353</v>
       </c>
       <c r="I23" s="4"/>
     </row>
@@ -1640,13 +1712,13 @@
         <v>50</v>
       </c>
       <c r="C24" s="2">
-        <v>3.797</v>
+        <v>3.96</v>
       </c>
       <c r="D24" s="2">
-        <v>116.467684095643</v>
+        <v>120.165902704649</v>
       </c>
       <c r="E24" s="2">
-        <v>3.833</v>
+        <v>4.622</v>
       </c>
       <c r="I24" s="4"/>
     </row>
@@ -1658,13 +1730,13 @@
         <v>52</v>
       </c>
       <c r="C25" s="2">
-        <v>3.016</v>
+        <v>2.188</v>
       </c>
       <c r="D25" s="2">
-        <v>113.466634957555</v>
+        <v>119.334315493595</v>
       </c>
       <c r="E25" s="2">
-        <v>2.359</v>
+        <v>2.992</v>
       </c>
       <c r="I25" s="4"/>
     </row>
@@ -1676,13 +1748,13 @@
         <v>54</v>
       </c>
       <c r="C26" s="2">
-        <v>2.089</v>
+        <v>3.325</v>
       </c>
       <c r="D26" s="2">
-        <v>113.967664674608</v>
+        <v>121.24078425492</v>
       </c>
       <c r="E26" s="2">
-        <v>2.97</v>
+        <v>4.912</v>
       </c>
       <c r="I26" s="4"/>
     </row>
@@ -1694,13 +1766,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2">
-        <v>2.171</v>
+        <v>3.4</v>
       </c>
       <c r="D27" s="2">
-        <v>116.609237421252</v>
+        <v>121.134997018438</v>
       </c>
       <c r="E27" s="2">
-        <v>3.005</v>
+        <v>4.871</v>
       </c>
       <c r="I27" s="4"/>
     </row>
@@ -1712,13 +1784,13 @@
         <v>58</v>
       </c>
       <c r="C28" s="2">
-        <v>2.999</v>
+        <v>4.999</v>
       </c>
       <c r="D28" s="2">
-        <v>113.237215295459</v>
+        <v>121.13108537564</v>
       </c>
       <c r="E28" s="2">
-        <v>2.348</v>
+        <v>4.827</v>
       </c>
       <c r="I28" s="4"/>
     </row>
@@ -1730,13 +1802,13 @@
         <v>60</v>
       </c>
       <c r="C29" s="2">
-        <v>2.249</v>
+        <v>4.984</v>
       </c>
       <c r="D29" s="2">
-        <v>115.925172997997</v>
+        <v>116.291466727588</v>
       </c>
       <c r="E29" s="2">
-        <v>2.879</v>
+        <v>3.288</v>
       </c>
       <c r="I29" s="4"/>
     </row>
@@ -1748,109 +1820,228 @@
         <v>62</v>
       </c>
       <c r="C30" s="2">
+        <v>4.997</v>
+      </c>
+      <c r="D30" s="2">
+        <v>121.030316627922</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4.825</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.797</v>
+      </c>
+      <c r="D31" s="2">
+        <v>116.500272379531</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3.425</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3.011</v>
+      </c>
+      <c r="D32" s="2">
+        <v>120.402870660027</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3.271</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4.994</v>
+      </c>
+      <c r="D33" s="2">
+        <v>120.086219200616</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.806</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>114.298685154915</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.948</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2.087</v>
+      </c>
+      <c r="D35" s="2">
+        <v>113.965027582808</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2.562</v>
+      </c>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="2">
         <v>4.583</v>
       </c>
-      <c r="D30" s="2">
-        <v>113.240036920708</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2.879</v>
-      </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="2">
+        <v>113.258255783762</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2.469</v>
+      </c>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="A37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4.833</v>
+      </c>
+      <c r="D37" s="2">
+        <v>113.87869144294</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4.863</v>
+      </c>
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="A38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3.199</v>
+      </c>
+      <c r="D38" s="2">
+        <v>113.927605679988</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2.885</v>
+      </c>
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="A39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2.945</v>
+      </c>
+      <c r="D39" s="2">
+        <v>115.232866710712</v>
+      </c>
+      <c r="E39" s="2">
+        <v>2.296</v>
+      </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="I40" s="4"/>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2.248</v>
+      </c>
+      <c r="D40" s="2">
+        <v>115.909758170348</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2.471</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="D41" s="2">
+        <v>115.51684977622</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2.597</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="A42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="2">
+        <v>6.823</v>
+      </c>
+      <c r="D42" s="2">
+        <v>118.266074241386</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2.044</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3"/>
@@ -1943,12 +2134,12 @@
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3"/>
@@ -2146,12 +2337,11 @@
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:4">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3"/>
@@ -2416,12 +2606,6 @@
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1.the last year is set for 1.5 for selected
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7270"/>
+    <workbookView windowWidth="18350" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="clause" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>code</t>
   </si>
@@ -43,6 +56,12 @@
     <t>瑞丰转债</t>
   </si>
   <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
     <t>sh113610</t>
   </si>
   <si>
@@ -55,10 +74,58 @@
     <t>正川转债</t>
   </si>
   <si>
-    <t>sh113608</t>
-  </si>
-  <si>
-    <t>威派转债</t>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>中陆转债</t>
+  </si>
+  <si>
+    <t>sz128125</t>
+  </si>
+  <si>
+    <t>华阳转债</t>
+  </si>
+  <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
+    <t>sz123103</t>
+  </si>
+  <si>
+    <t>震安转债</t>
+  </si>
+  <si>
+    <t>sh118010</t>
+  </si>
+  <si>
+    <t>洁特转债</t>
+  </si>
+  <si>
+    <t>sz123106</t>
+  </si>
+  <si>
+    <t>正丹转债</t>
+  </si>
+  <si>
+    <t>sz123093</t>
+  </si>
+  <si>
+    <t>金陵转债</t>
+  </si>
+  <si>
+    <t>sh113665</t>
+  </si>
+  <si>
+    <t>汇通转债</t>
+  </si>
+  <si>
+    <t>sz127062</t>
+  </si>
+  <si>
+    <t>垒知转债</t>
   </si>
   <si>
     <t>sz128118</t>
@@ -67,16 +134,106 @@
     <t>瀛通转债</t>
   </si>
   <si>
-    <t>sz123106</t>
-  </si>
-  <si>
-    <t>正丹转债</t>
-  </si>
-  <si>
-    <t>sh118010</t>
-  </si>
-  <si>
-    <t>洁特转债</t>
+    <t>sz123039</t>
+  </si>
+  <si>
+    <t>开润转债</t>
+  </si>
+  <si>
+    <t>sh113593</t>
+  </si>
+  <si>
+    <t>沪工转债</t>
+  </si>
+  <si>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
+  </si>
+  <si>
+    <t>sh113600</t>
+  </si>
+  <si>
+    <t>新星转债</t>
+  </si>
+  <si>
+    <t>sh118006</t>
+  </si>
+  <si>
+    <t>阿拉转债</t>
+  </si>
+  <si>
+    <t>sz123171</t>
+  </si>
+  <si>
+    <t>共同转债</t>
+  </si>
+  <si>
+    <t>sz123065</t>
+  </si>
+  <si>
+    <t>宝莱转债</t>
+  </si>
+  <si>
+    <t>sh118016</t>
+  </si>
+  <si>
+    <t>京源转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
+    <t>sz123159</t>
+  </si>
+  <si>
+    <t>崧盛转债</t>
+  </si>
+  <si>
+    <t>sz123168</t>
+  </si>
+  <si>
+    <t>惠云转债</t>
+  </si>
+  <si>
+    <t>sh111003</t>
+  </si>
+  <si>
+    <t>聚合转债</t>
+  </si>
+  <si>
+    <t>sh118029</t>
+  </si>
+  <si>
+    <t>富淼转债</t>
+  </si>
+  <si>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>奥佳转债</t>
+  </si>
+  <si>
+    <t>sh118014</t>
+  </si>
+  <si>
+    <t>高测转债</t>
+  </si>
+  <si>
+    <t>sh118011</t>
+  </si>
+  <si>
+    <t>银微转债</t>
+  </si>
+  <si>
+    <t>sz123166</t>
+  </si>
+  <si>
+    <t>蒙泰转债</t>
   </si>
   <si>
     <t>sh118015</t>
@@ -85,70 +242,28 @@
     <t>芯海转债</t>
   </si>
   <si>
-    <t>sz123093</t>
-  </si>
-  <si>
-    <t>金陵转债</t>
-  </si>
-  <si>
-    <t>sz123155</t>
-  </si>
-  <si>
-    <t>中陆转债</t>
-  </si>
-  <si>
-    <t>sz123109</t>
-  </si>
-  <si>
-    <t>昌红转债</t>
-  </si>
-  <si>
-    <t>sh113593</t>
-  </si>
-  <si>
-    <t>沪工转债</t>
-  </si>
-  <si>
-    <t>sz128117</t>
-  </si>
-  <si>
-    <t>道恩转债</t>
-  </si>
-  <si>
-    <t>sz128125</t>
-  </si>
-  <si>
-    <t>华阳转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
-  </si>
-  <si>
-    <t>sz123103</t>
-  </si>
-  <si>
-    <t>震安转债</t>
-  </si>
-  <si>
-    <t>sh113573</t>
-  </si>
-  <si>
-    <t>纵横转债</t>
-  </si>
-  <si>
-    <t>sz123039</t>
-  </si>
-  <si>
-    <t>开润转债</t>
-  </si>
-  <si>
-    <t>sz127062</t>
-  </si>
-  <si>
-    <t>垒知转债</t>
+    <t>sh113649</t>
+  </si>
+  <si>
+    <t>丰山转债</t>
+  </si>
+  <si>
+    <t>sh118012</t>
+  </si>
+  <si>
+    <t>微芯转债</t>
+  </si>
+  <si>
+    <t>sz123156</t>
+  </si>
+  <si>
+    <t>博汇转债</t>
+  </si>
+  <si>
+    <t>sh118018</t>
+  </si>
+  <si>
+    <t>瑞科转债</t>
   </si>
   <si>
     <t>sz127059</t>
@@ -157,34 +272,10 @@
     <t>永东转2</t>
   </si>
   <si>
-    <t>sh118006</t>
-  </si>
-  <si>
-    <t>阿拉转债</t>
-  </si>
-  <si>
-    <t>sz123065</t>
-  </si>
-  <si>
-    <t>宝莱转债</t>
-  </si>
-  <si>
-    <t>sh118011</t>
-  </si>
-  <si>
-    <t>银微转债</t>
-  </si>
-  <si>
-    <t>sh118004</t>
-  </si>
-  <si>
-    <t>博瑞转债</t>
-  </si>
-  <si>
-    <t>sz123153</t>
-  </si>
-  <si>
-    <t>英力转债</t>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>华体转债</t>
   </si>
   <si>
     <t>sh113618</t>
@@ -193,46 +284,22 @@
     <t>美诺转债</t>
   </si>
   <si>
-    <t>sh111003</t>
-  </si>
-  <si>
-    <t>聚合转债</t>
-  </si>
-  <si>
-    <t>sh113649</t>
-  </si>
-  <si>
-    <t>丰山转债</t>
-  </si>
-  <si>
-    <t>sh113574</t>
-  </si>
-  <si>
-    <t>华体转债</t>
-  </si>
-  <si>
-    <t>sh118018</t>
-  </si>
-  <si>
-    <t>瑞科转债</t>
-  </si>
-  <si>
     <t>sz123100</t>
   </si>
   <si>
     <t>朗科转债</t>
   </si>
   <si>
-    <t>sz128097</t>
-  </si>
-  <si>
-    <t>奥佳转债</t>
-  </si>
-  <si>
-    <t>sz123090</t>
-  </si>
-  <si>
-    <t>三诺转债</t>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>凌钢转债</t>
+  </si>
+  <si>
+    <t>sz128072</t>
+  </si>
+  <si>
+    <t>翔鹭转债</t>
   </si>
   <si>
     <t>sz127071</t>
@@ -241,10 +308,16 @@
     <t>天箭转债</t>
   </si>
   <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
+    <t>sz128071</t>
+  </si>
+  <si>
+    <t>合兴转债</t>
+  </si>
+  <si>
+    <t>sz128123</t>
+  </si>
+  <si>
+    <t>国光转债</t>
   </si>
   <si>
     <t>sh113030</t>
@@ -253,22 +326,16 @@
     <t>东风转债</t>
   </si>
   <si>
-    <t>sh110070</t>
-  </si>
-  <si>
-    <t>凌钢转债</t>
-  </si>
-  <si>
-    <t>sz128123</t>
-  </si>
-  <si>
-    <t>国光转债</t>
+    <t>sz123048</t>
+  </si>
+  <si>
+    <t>应急转债</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -297,34 +364,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -338,14 +377,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,6 +416,21 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -435,7 +481,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,49 +517,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,121 +655,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,21 +722,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,6 +755,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,148 +826,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -915,52 +982,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1262,8 +1329,8 @@
   <sheetPr/>
   <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1307,10 +1374,10 @@
         <v>4.199</v>
       </c>
       <c r="D2" s="2">
-        <v>135.967852132714</v>
+        <v>134.858049333215</v>
       </c>
       <c r="E2" s="2">
-        <v>3.14</v>
+        <v>2.888</v>
       </c>
       <c r="I2" s="4"/>
     </row>
@@ -1325,10 +1392,10 @@
         <v>3.4</v>
       </c>
       <c r="D3" s="2">
-        <v>128.858596249388</v>
+        <v>128.924452409233</v>
       </c>
       <c r="E3" s="2">
-        <v>3.953</v>
+        <v>3.701</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -1340,13 +1407,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>4.579</v>
+        <v>4.2</v>
       </c>
       <c r="D4" s="2">
-        <v>120.302920042733</v>
+        <v>119.430094021366</v>
       </c>
       <c r="E4" s="2">
-        <v>3.178</v>
+        <v>2.866</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -1358,13 +1425,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>4.049</v>
+        <v>4.579</v>
       </c>
       <c r="D5" s="2">
-        <v>120.734280691874</v>
+        <v>119.188187118695</v>
       </c>
       <c r="E5" s="2">
-        <v>3.584</v>
+        <v>2.926</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -1376,13 +1443,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>4.2</v>
+        <v>4.049</v>
       </c>
       <c r="D6" s="2">
-        <v>120.679675097355</v>
+        <v>120.723246081037</v>
       </c>
       <c r="E6" s="2">
-        <v>3.118</v>
+        <v>3.332</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -1394,13 +1461,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>2.996</v>
+        <v>3.6</v>
       </c>
       <c r="D7" s="2">
-        <v>119.981391909983</v>
+        <v>121.505395636933</v>
       </c>
       <c r="E7" s="2">
-        <v>2.762</v>
+        <v>4.625</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -1412,13 +1479,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>3.2</v>
+        <v>4.497</v>
       </c>
       <c r="D8" s="2">
-        <v>124.685989853621</v>
+        <v>116.648745558245</v>
       </c>
       <c r="E8" s="2">
-        <v>3.488</v>
+        <v>2.586</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -1430,13 +1497,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>4.4</v>
+        <v>3.583</v>
       </c>
       <c r="D9" s="2">
-        <v>115.019657622983</v>
+        <v>121.665192465013</v>
       </c>
       <c r="E9" s="2">
-        <v>4.753</v>
+        <v>2.51</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -1448,13 +1515,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>4.1</v>
+        <v>2.494</v>
       </c>
       <c r="D10" s="2">
-        <v>121.352592749892</v>
+        <v>120.460943818505</v>
       </c>
       <c r="E10" s="2">
-        <v>4.816</v>
+        <v>3.203</v>
       </c>
       <c r="I10" s="4"/>
     </row>
@@ -1466,13 +1533,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>2.485</v>
+        <v>4.4</v>
       </c>
       <c r="D11" s="2">
-        <v>128.289014994689</v>
+        <v>115.057408002718</v>
       </c>
       <c r="E11" s="2">
-        <v>3.312</v>
+        <v>4.501</v>
       </c>
       <c r="I11" s="4"/>
     </row>
@@ -1484,13 +1551,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="D12" s="2">
-        <v>121.358291892986</v>
+        <v>124.713898502435</v>
       </c>
       <c r="E12" s="2">
-        <v>4.877</v>
+        <v>3.236</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -1502,13 +1569,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>4.595</v>
+        <v>2.485</v>
       </c>
       <c r="D13" s="2">
-        <v>120.14365740467</v>
+        <v>128.356493535591</v>
       </c>
       <c r="E13" s="2">
-        <v>3.51</v>
+        <v>3.06</v>
       </c>
       <c r="I13" s="4"/>
     </row>
@@ -1520,13 +1587,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>3.997</v>
+        <v>3.6</v>
       </c>
       <c r="D14" s="2">
-        <v>119.519784063762</v>
+        <v>120.217980114154</v>
       </c>
       <c r="E14" s="2">
-        <v>2.811</v>
+        <v>4.967</v>
       </c>
       <c r="I14" s="4"/>
     </row>
@@ -1538,13 +1605,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>3.584</v>
+        <v>3.96</v>
       </c>
       <c r="D15" s="2">
-        <v>121.606966906455</v>
+        <v>120.299141797923</v>
       </c>
       <c r="E15" s="2">
-        <v>2.762</v>
+        <v>4.315</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -1556,13 +1623,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>4.498</v>
+        <v>2.996</v>
       </c>
       <c r="D16" s="2">
-        <v>116.580845055446</v>
+        <v>119.898986041026</v>
       </c>
       <c r="E16" s="2">
-        <v>2.838</v>
+        <v>2.51</v>
       </c>
       <c r="I16" s="4"/>
     </row>
@@ -1574,13 +1641,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="2">
-        <v>4.993</v>
+        <v>2.216</v>
       </c>
       <c r="D17" s="2">
-        <v>120.618141356509</v>
+        <v>117.338230070739</v>
       </c>
       <c r="E17" s="2">
-        <v>3.195</v>
+        <v>1.995</v>
       </c>
       <c r="I17" s="4"/>
     </row>
@@ -1592,13 +1659,13 @@
         <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>2.494</v>
+        <v>3.997</v>
       </c>
       <c r="D18" s="2">
-        <v>120.307473888831</v>
+        <v>119.502247619324</v>
       </c>
       <c r="E18" s="2">
-        <v>3.455</v>
+        <v>2.559</v>
       </c>
       <c r="I18" s="4"/>
     </row>
@@ -1610,13 +1677,13 @@
         <v>40</v>
       </c>
       <c r="C19" s="2">
-        <v>2.698</v>
+        <v>4.595</v>
       </c>
       <c r="D19" s="2">
-        <v>122.378496363629</v>
+        <v>120.11175275425</v>
       </c>
       <c r="E19" s="2">
-        <v>2.553</v>
+        <v>3.258</v>
       </c>
       <c r="I19" s="4"/>
     </row>
@@ -1628,13 +1695,13 @@
         <v>42</v>
       </c>
       <c r="C20" s="2">
-        <v>2.216</v>
+        <v>4.53</v>
       </c>
       <c r="D20" s="2">
-        <v>119.163066789678</v>
+        <v>124.063945311645</v>
       </c>
       <c r="E20" s="2">
-        <v>2.247</v>
+        <v>2.625</v>
       </c>
       <c r="I20" s="4"/>
     </row>
@@ -1646,13 +1713,13 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>3.96</v>
+        <v>3.87</v>
       </c>
       <c r="D21" s="2">
-        <v>120.215302944788</v>
+        <v>121.337101958881</v>
       </c>
       <c r="E21" s="2">
-        <v>4.567</v>
+        <v>4.214</v>
       </c>
       <c r="I21" s="4"/>
     </row>
@@ -1664,13 +1731,13 @@
         <v>46</v>
       </c>
       <c r="C22" s="2">
-        <v>3.792</v>
+        <v>3.799</v>
       </c>
       <c r="D22" s="2">
-        <v>120.191136637177</v>
+        <v>121.094190356348</v>
       </c>
       <c r="E22" s="2">
-        <v>4.532</v>
+        <v>4.921</v>
       </c>
       <c r="I22" s="4"/>
     </row>
@@ -1682,13 +1749,13 @@
         <v>48</v>
       </c>
       <c r="C23" s="2">
-        <v>3.871</v>
+        <v>2.188</v>
       </c>
       <c r="D23" s="2">
-        <v>121.313382898453</v>
+        <v>119.376286174947</v>
       </c>
       <c r="E23" s="2">
-        <v>4.466</v>
+        <v>2.685</v>
       </c>
       <c r="I23" s="4"/>
     </row>
@@ -1700,13 +1767,13 @@
         <v>50</v>
       </c>
       <c r="C24" s="2">
-        <v>2.188</v>
+        <v>3.325</v>
       </c>
       <c r="D24" s="2">
-        <v>119.335577426063</v>
+        <v>121.278711917137</v>
       </c>
       <c r="E24" s="2">
-        <v>2.937</v>
+        <v>4.606</v>
       </c>
       <c r="I24" s="4"/>
     </row>
@@ -1718,13 +1785,13 @@
         <v>52</v>
       </c>
       <c r="C25" s="2">
-        <v>4.997</v>
+        <v>4.993</v>
       </c>
       <c r="D25" s="2">
-        <v>121.07020906286</v>
+        <v>119.359190640898</v>
       </c>
       <c r="E25" s="2">
-        <v>4.77</v>
+        <v>2.943</v>
       </c>
       <c r="I25" s="4"/>
     </row>
@@ -1736,13 +1803,13 @@
         <v>54</v>
       </c>
       <c r="C26" s="2">
-        <v>4.65</v>
+        <v>2.943</v>
       </c>
       <c r="D26" s="2">
-        <v>120.641635786162</v>
+        <v>119.072777235544</v>
       </c>
       <c r="E26" s="2">
-        <v>4.271</v>
+        <v>4.751</v>
       </c>
       <c r="I26" s="4"/>
     </row>
@@ -1754,13 +1821,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2">
-        <v>3.4</v>
+        <v>4.9</v>
       </c>
       <c r="D27" s="2">
-        <v>121.103044932712</v>
+        <v>120.376688696152</v>
       </c>
       <c r="E27" s="2">
-        <v>4.816</v>
+        <v>4.907</v>
       </c>
       <c r="I27" s="4"/>
     </row>
@@ -1772,13 +1839,13 @@
         <v>58</v>
       </c>
       <c r="C28" s="2">
-        <v>4.767</v>
+        <v>2.037</v>
       </c>
       <c r="D28" s="2">
-        <v>114.307736520609</v>
+        <v>120.686852696566</v>
       </c>
       <c r="E28" s="2">
-        <v>3.299</v>
+        <v>4.192</v>
       </c>
       <c r="I28" s="4"/>
     </row>
@@ -1790,13 +1857,13 @@
         <v>60</v>
       </c>
       <c r="C29" s="2">
-        <v>2.038</v>
+        <v>4.5</v>
       </c>
       <c r="D29" s="2">
-        <v>120.614877839224</v>
+        <v>114.340963045083</v>
       </c>
       <c r="E29" s="2">
-        <v>4.444</v>
+        <v>4.967</v>
       </c>
       <c r="I29" s="4"/>
     </row>
@@ -1808,13 +1875,13 @@
         <v>62</v>
       </c>
       <c r="C30" s="2">
-        <v>4.994</v>
+        <v>4.583</v>
       </c>
       <c r="D30" s="2">
-        <v>120.07483924211</v>
+        <v>113.336049003838</v>
       </c>
       <c r="E30" s="2">
-        <v>4.751</v>
+        <v>2.162</v>
       </c>
       <c r="I30" s="4"/>
     </row>
@@ -1826,13 +1893,13 @@
         <v>64</v>
       </c>
       <c r="C31" s="2">
-        <v>2.087</v>
+        <v>4.832</v>
       </c>
       <c r="D31" s="2">
-        <v>113.982083642229</v>
+        <v>114.044734827006</v>
       </c>
       <c r="E31" s="2">
-        <v>2.507</v>
+        <v>4.556</v>
       </c>
       <c r="I31" s="4"/>
     </row>
@@ -1844,13 +1911,13 @@
         <v>66</v>
       </c>
       <c r="C32" s="2">
-        <v>4.3</v>
+        <v>4.997</v>
       </c>
       <c r="D32" s="2">
-        <v>114.257432948478</v>
+        <v>121.021561046122</v>
       </c>
       <c r="E32" s="2">
-        <v>4.893</v>
+        <v>4.518</v>
       </c>
       <c r="I32" s="4"/>
     </row>
@@ -1862,13 +1929,13 @@
         <v>68</v>
       </c>
       <c r="C33" s="2">
-        <v>3.797</v>
+        <v>2.999</v>
       </c>
       <c r="D33" s="2">
-        <v>116.459531923093</v>
+        <v>121.118691622955</v>
       </c>
       <c r="E33" s="2">
-        <v>3.37</v>
+        <v>4.849</v>
       </c>
       <c r="I33" s="4"/>
     </row>
@@ -1880,13 +1947,13 @@
         <v>70</v>
       </c>
       <c r="C34" s="2">
-        <v>4.583</v>
+        <v>4.1</v>
       </c>
       <c r="D34" s="2">
-        <v>113.246427072294</v>
+        <v>121.151656502254</v>
       </c>
       <c r="E34" s="2">
-        <v>2.414</v>
+        <v>4.564</v>
       </c>
       <c r="I34" s="4"/>
     </row>
@@ -1898,13 +1965,13 @@
         <v>72</v>
       </c>
       <c r="C35" s="2">
-        <v>4.984</v>
+        <v>4.993</v>
       </c>
       <c r="D35" s="2">
-        <v>116.217024263587</v>
+        <v>120.113295713659</v>
       </c>
       <c r="E35" s="2">
-        <v>3.233</v>
+        <v>4.499</v>
       </c>
       <c r="I35" s="4"/>
     </row>
@@ -1916,13 +1983,13 @@
         <v>74</v>
       </c>
       <c r="C36" s="2">
-        <v>4.95</v>
+        <v>4.999</v>
       </c>
       <c r="D36" s="2">
-        <v>111.890877302064</v>
+        <v>121.126102709602</v>
       </c>
       <c r="E36" s="2">
-        <v>4.904</v>
+        <v>4.521</v>
       </c>
       <c r="I36" s="4"/>
     </row>
@@ -1934,13 +2001,13 @@
         <v>76</v>
       </c>
       <c r="C37" s="2">
-        <v>2.248</v>
+        <v>3.969</v>
       </c>
       <c r="D37" s="2">
-        <v>115.904369645813</v>
+        <v>120.9031795667</v>
       </c>
       <c r="E37" s="2">
-        <v>2.416</v>
+        <v>4.636</v>
       </c>
       <c r="I37" s="4"/>
     </row>
@@ -1952,13 +2019,13 @@
         <v>78</v>
       </c>
       <c r="C38" s="2">
-        <v>2.945</v>
+        <v>4.3</v>
       </c>
       <c r="D38" s="2">
-        <v>115.222970588007</v>
+        <v>114.283822030466</v>
       </c>
       <c r="E38" s="2">
-        <v>2.241</v>
+        <v>4.641</v>
       </c>
       <c r="I38" s="4"/>
     </row>
@@ -1970,13 +2037,13 @@
         <v>80</v>
       </c>
       <c r="C39" s="2">
-        <v>2.17</v>
+        <v>3.792</v>
       </c>
       <c r="D39" s="2">
-        <v>115.508092656898</v>
+        <v>120.094384652916</v>
       </c>
       <c r="E39" s="2">
-        <v>2.543</v>
+        <v>4.28</v>
       </c>
       <c r="I39" s="4"/>
     </row>
@@ -1988,77 +2055,167 @@
         <v>82</v>
       </c>
       <c r="C40" s="2">
+        <v>2.086</v>
+      </c>
+      <c r="D40" s="2">
+        <v>113.978107727346</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2.255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="2">
+        <v>4.767</v>
+      </c>
+      <c r="D41" s="2">
+        <v>114.244722700767</v>
+      </c>
+      <c r="E41" s="2">
+        <v>3.047</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3.797</v>
+      </c>
+      <c r="D42" s="2">
+        <v>116.44489293139</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3.118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="D43" s="2">
+        <v>115.54575529836</v>
+      </c>
+      <c r="E43" s="2">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3.016</v>
+      </c>
+      <c r="D44" s="2">
+        <v>111.977713064067</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.644</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="2">
+        <v>4.949</v>
+      </c>
+      <c r="D45" s="2">
+        <v>111.888569414535</v>
+      </c>
+      <c r="E45" s="2">
+        <v>4.652</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2.999</v>
+      </c>
+      <c r="D46" s="2">
+        <v>111.773796890189</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1.633</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="2">
         <v>3.199</v>
       </c>
-      <c r="D40" s="2">
-        <v>113.879538641155</v>
-      </c>
-      <c r="E40" s="2">
-        <v>2.83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="2">
+        <v>113.890917093887</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2.578</v>
+      </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="A48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2.945</v>
+      </c>
+      <c r="D48" s="2">
+        <v>113.732399644775</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1.989</v>
+      </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="A49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3.79</v>
+      </c>
+      <c r="D49" s="2">
+        <v>111.135311586902</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2.282</v>
+      </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3"/>

</xml_diff>

<commit_message>
1.add crash time and crash threshold for bombs and missiles
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>code</t>
   </si>
@@ -50,24 +50,24 @@
     <t>侨银转债</t>
   </si>
   <si>
+    <t>sh113610</t>
+  </si>
+  <si>
+    <t>灵康转债</t>
+  </si>
+  <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
     <t>sz123126</t>
   </si>
   <si>
     <t>瑞丰转债</t>
   </si>
   <si>
-    <t>sh113608</t>
-  </si>
-  <si>
-    <t>威派转债</t>
-  </si>
-  <si>
-    <t>sh113610</t>
-  </si>
-  <si>
-    <t>灵康转债</t>
-  </si>
-  <si>
     <t>sh113624</t>
   </si>
   <si>
@@ -80,18 +80,30 @@
     <t>中陆转债</t>
   </si>
   <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
+    <t>sz123106</t>
+  </si>
+  <si>
+    <t>正丹转债</t>
+  </si>
+  <si>
+    <t>sz128118</t>
+  </si>
+  <si>
+    <t>瀛通转债</t>
+  </si>
+  <si>
     <t>sz128125</t>
   </si>
   <si>
     <t>华阳转债</t>
   </si>
   <si>
-    <t>sz128117</t>
-  </si>
-  <si>
-    <t>道恩转债</t>
-  </si>
-  <si>
     <t>sz123103</t>
   </si>
   <si>
@@ -104,10 +116,10 @@
     <t>洁特转债</t>
   </si>
   <si>
-    <t>sz123106</t>
-  </si>
-  <si>
-    <t>正丹转债</t>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
   </si>
   <si>
     <t>sz123093</t>
@@ -122,16 +134,28 @@
     <t>汇通转债</t>
   </si>
   <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
     <t>sz127062</t>
   </si>
   <si>
     <t>垒知转债</t>
   </si>
   <si>
-    <t>sz128118</t>
-  </si>
-  <si>
-    <t>瀛通转债</t>
+    <t>sh118006</t>
+  </si>
+  <si>
+    <t>阿拉转债</t>
+  </si>
+  <si>
+    <t>sh113600</t>
+  </si>
+  <si>
+    <t>新星转债</t>
   </si>
   <si>
     <t>sz123039</t>
@@ -146,22 +170,22 @@
     <t>沪工转债</t>
   </si>
   <si>
-    <t>sz123109</t>
-  </si>
-  <si>
-    <t>昌红转债</t>
-  </si>
-  <si>
-    <t>sh113600</t>
-  </si>
-  <si>
-    <t>新星转债</t>
-  </si>
-  <si>
-    <t>sh118006</t>
-  </si>
-  <si>
-    <t>阿拉转债</t>
+    <t>sh118011</t>
+  </si>
+  <si>
+    <t>银微转债</t>
+  </si>
+  <si>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <t>纵横转债</t>
+  </si>
+  <si>
+    <t>sh118014</t>
+  </si>
+  <si>
+    <t>高测转债</t>
   </si>
   <si>
     <t>sz123171</t>
@@ -170,22 +194,112 @@
     <t>共同转债</t>
   </si>
   <si>
+    <t>sh118012</t>
+  </si>
+  <si>
+    <t>微芯转债</t>
+  </si>
+  <si>
+    <t>sz123168</t>
+  </si>
+  <si>
+    <t>惠云转债</t>
+  </si>
+  <si>
+    <t>sh118016</t>
+  </si>
+  <si>
+    <t>京源转债</t>
+  </si>
+  <si>
     <t>sz123065</t>
   </si>
   <si>
     <t>宝莱转债</t>
   </si>
   <si>
-    <t>sh118016</t>
-  </si>
-  <si>
-    <t>京源转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
+    <t>sh118015</t>
+  </si>
+  <si>
+    <t>芯海转债</t>
+  </si>
+  <si>
+    <t>sh118029</t>
+  </si>
+  <si>
+    <t>富淼转债</t>
+  </si>
+  <si>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>凌钢转债</t>
+  </si>
+  <si>
+    <t>sh111003</t>
+  </si>
+  <si>
+    <t>聚合转债</t>
+  </si>
+  <si>
+    <t>sh113618</t>
+  </si>
+  <si>
+    <t>美诺转债</t>
+  </si>
+  <si>
+    <t>sz123156</t>
+  </si>
+  <si>
+    <t>博汇转债</t>
+  </si>
+  <si>
+    <t>sh118018</t>
+  </si>
+  <si>
+    <t>瑞科转债</t>
+  </si>
+  <si>
+    <t>sz127059</t>
+  </si>
+  <si>
+    <t>永东转2</t>
+  </si>
+  <si>
+    <t>sz123153</t>
+  </si>
+  <si>
+    <t>英力转债</t>
+  </si>
+  <si>
+    <t>sh118009</t>
+  </si>
+  <si>
+    <t>华锐转债</t>
+  </si>
+  <si>
+    <t>sz123061</t>
+  </si>
+  <si>
+    <t>航新转债</t>
+  </si>
+  <si>
+    <t>sz123166</t>
+  </si>
+  <si>
+    <t>蒙泰转债</t>
+  </si>
+  <si>
+    <t>sz123100</t>
+  </si>
+  <si>
+    <t>朗科转债</t>
+  </si>
+  <si>
+    <t>sz123152</t>
+  </si>
+  <si>
+    <t>润禾转债</t>
   </si>
   <si>
     <t>sz123159</t>
@@ -194,22 +308,82 @@
     <t>崧盛转债</t>
   </si>
   <si>
-    <t>sz123168</t>
-  </si>
-  <si>
-    <t>惠云转债</t>
-  </si>
-  <si>
-    <t>sh111003</t>
-  </si>
-  <si>
-    <t>聚合转债</t>
-  </si>
-  <si>
-    <t>sh118029</t>
-  </si>
-  <si>
-    <t>富淼转债</t>
+    <t>sz127079</t>
+  </si>
+  <si>
+    <t>华亚转债</t>
+  </si>
+  <si>
+    <t>sz123087</t>
+  </si>
+  <si>
+    <t>明电转债</t>
+  </si>
+  <si>
+    <t>sh113643</t>
+  </si>
+  <si>
+    <t>风语转债</t>
+  </si>
+  <si>
+    <t>sz123089</t>
+  </si>
+  <si>
+    <t>九洲转2</t>
+  </si>
+  <si>
+    <t>sh113649</t>
+  </si>
+  <si>
+    <t>丰山转债</t>
+  </si>
+  <si>
+    <t>sh118007</t>
+  </si>
+  <si>
+    <t>山石转债</t>
+  </si>
+  <si>
+    <t>sz123163</t>
+  </si>
+  <si>
+    <t>金沃转债</t>
+  </si>
+  <si>
+    <t>sh113660</t>
+  </si>
+  <si>
+    <t>寿22转债</t>
+  </si>
+  <si>
+    <t>sh113662</t>
+  </si>
+  <si>
+    <t>豪能转债</t>
+  </si>
+  <si>
+    <t>sz123160</t>
+  </si>
+  <si>
+    <t>泰福转债</t>
+  </si>
+  <si>
+    <t>sh113597</t>
+  </si>
+  <si>
+    <t>佳力转债</t>
+  </si>
+  <si>
+    <t>sz128072</t>
+  </si>
+  <si>
+    <t>翔鹭转债</t>
+  </si>
+  <si>
+    <t>sh118004</t>
+  </si>
+  <si>
+    <t>博瑞转债</t>
   </si>
   <si>
     <t>sz128097</t>
@@ -218,58 +392,46 @@
     <t>奥佳转债</t>
   </si>
   <si>
-    <t>sh118014</t>
-  </si>
-  <si>
-    <t>高测转债</t>
-  </si>
-  <si>
-    <t>sh118011</t>
-  </si>
-  <si>
-    <t>银微转债</t>
-  </si>
-  <si>
-    <t>sz123166</t>
-  </si>
-  <si>
-    <t>蒙泰转债</t>
-  </si>
-  <si>
-    <t>sh118015</t>
-  </si>
-  <si>
-    <t>芯海转债</t>
-  </si>
-  <si>
-    <t>sh113649</t>
-  </si>
-  <si>
-    <t>丰山转债</t>
-  </si>
-  <si>
-    <t>sh118012</t>
-  </si>
-  <si>
-    <t>微芯转债</t>
-  </si>
-  <si>
-    <t>sz123156</t>
-  </si>
-  <si>
-    <t>博汇转债</t>
-  </si>
-  <si>
-    <t>sh118018</t>
-  </si>
-  <si>
-    <t>瑞科转债</t>
-  </si>
-  <si>
-    <t>sz127059</t>
-  </si>
-  <si>
-    <t>永东转2</t>
+    <t>sz123143</t>
+  </si>
+  <si>
+    <t>胜蓝转债</t>
+  </si>
+  <si>
+    <t>sz127072</t>
+  </si>
+  <si>
+    <t>博实转债</t>
+  </si>
+  <si>
+    <t>sz123088</t>
+  </si>
+  <si>
+    <t>威唐转债</t>
+  </si>
+  <si>
+    <t>sz128071</t>
+  </si>
+  <si>
+    <t>合兴转债</t>
+  </si>
+  <si>
+    <t>sh113565</t>
+  </si>
+  <si>
+    <t>宏辉转债</t>
+  </si>
+  <si>
+    <t>sh113664</t>
+  </si>
+  <si>
+    <t>大元转债</t>
+  </si>
+  <si>
+    <t>sz123090</t>
+  </si>
+  <si>
+    <t>三诺转债</t>
   </si>
   <si>
     <t>sh113574</t>
@@ -278,46 +440,34 @@
     <t>华体转债</t>
   </si>
   <si>
-    <t>sh113618</t>
-  </si>
-  <si>
-    <t>美诺转债</t>
-  </si>
-  <si>
-    <t>sz123100</t>
-  </si>
-  <si>
-    <t>朗科转债</t>
-  </si>
-  <si>
-    <t>sh110070</t>
-  </si>
-  <si>
-    <t>凌钢转债</t>
-  </si>
-  <si>
-    <t>sz128072</t>
-  </si>
-  <si>
-    <t>翔鹭转债</t>
-  </si>
-  <si>
     <t>sz127071</t>
   </si>
   <si>
     <t>天箭转债</t>
   </si>
   <si>
-    <t>sz128071</t>
-  </si>
-  <si>
-    <t>合兴转债</t>
-  </si>
-  <si>
-    <t>sz128123</t>
-  </si>
-  <si>
-    <t>国光转债</t>
+    <t>sz123130</t>
+  </si>
+  <si>
+    <t>设研转债</t>
+  </si>
+  <si>
+    <t>sz123048</t>
+  </si>
+  <si>
+    <t>应急转债</t>
+  </si>
+  <si>
+    <t>sz128101</t>
+  </si>
+  <si>
+    <t>联创转债</t>
+  </si>
+  <si>
+    <t>sz128095</t>
+  </si>
+  <si>
+    <t>恩捷转债</t>
   </si>
   <si>
     <t>sh113030</t>
@@ -326,10 +476,10 @@
     <t>东风转债</t>
   </si>
   <si>
-    <t>sz123048</t>
-  </si>
-  <si>
-    <t>应急转债</t>
+    <t>sh113582</t>
+  </si>
+  <si>
+    <t>火炬转债</t>
   </si>
 </sst>
 </file>
@@ -977,8 +1127,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1330,7 +1480,7 @@
   <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E49"/>
+      <selection activeCell="A2" sqref="A2:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1374,12 +1524,12 @@
         <v>4.199</v>
       </c>
       <c r="D2" s="2">
-        <v>134.858049333215</v>
+        <v>134.836018187784</v>
       </c>
       <c r="E2" s="2">
-        <v>2.888</v>
-      </c>
-      <c r="I2" s="4"/>
+        <v>2.833</v>
+      </c>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
@@ -1389,15 +1539,15 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>3.4</v>
+        <v>4.579</v>
       </c>
       <c r="D3" s="2">
-        <v>128.924452409233</v>
+        <v>119.246962652178</v>
       </c>
       <c r="E3" s="2">
-        <v>3.701</v>
-      </c>
-      <c r="I3" s="4"/>
+        <v>2.871</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
@@ -1410,12 +1560,12 @@
         <v>4.2</v>
       </c>
       <c r="D4" s="2">
-        <v>119.430094021366</v>
+        <v>119.457633076098</v>
       </c>
       <c r="E4" s="2">
-        <v>2.866</v>
-      </c>
-      <c r="I4" s="4"/>
+        <v>2.811</v>
+      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
@@ -1425,15 +1575,15 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>4.579</v>
+        <v>3.4</v>
       </c>
       <c r="D5" s="2">
-        <v>119.188187118695</v>
+        <v>128.953627113165</v>
       </c>
       <c r="E5" s="2">
-        <v>2.926</v>
-      </c>
-      <c r="I5" s="4"/>
+        <v>3.647</v>
+      </c>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
@@ -1446,12 +1596,12 @@
         <v>4.049</v>
       </c>
       <c r="D6" s="2">
-        <v>120.723246081037</v>
+        <v>120.802380846276</v>
       </c>
       <c r="E6" s="2">
-        <v>3.332</v>
-      </c>
-      <c r="I6" s="4"/>
+        <v>3.277</v>
+      </c>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
@@ -1464,12 +1614,12 @@
         <v>3.6</v>
       </c>
       <c r="D7" s="2">
-        <v>121.505395636933</v>
+        <v>121.55701841432</v>
       </c>
       <c r="E7" s="2">
-        <v>4.625</v>
-      </c>
-      <c r="I7" s="4"/>
+        <v>4.57</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
@@ -1479,15 +1629,15 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>4.497</v>
+        <v>3.583</v>
       </c>
       <c r="D8" s="2">
-        <v>116.648745558245</v>
+        <v>121.696359755225</v>
       </c>
       <c r="E8" s="2">
-        <v>2.586</v>
-      </c>
-      <c r="I8" s="4"/>
+        <v>2.455</v>
+      </c>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
@@ -1497,15 +1647,15 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>3.583</v>
+        <v>3.2</v>
       </c>
       <c r="D9" s="2">
-        <v>121.665192465013</v>
+        <v>124.82010115078</v>
       </c>
       <c r="E9" s="2">
-        <v>2.51</v>
-      </c>
-      <c r="I9" s="4"/>
+        <v>3.181</v>
+      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
@@ -1515,15 +1665,15 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>2.494</v>
+        <v>2.995</v>
       </c>
       <c r="D10" s="2">
-        <v>120.460943818505</v>
+        <v>120.054344930916</v>
       </c>
       <c r="E10" s="2">
-        <v>3.203</v>
-      </c>
-      <c r="I10" s="4"/>
+        <v>2.455</v>
+      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -1533,15 +1683,15 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>4.4</v>
+        <v>4.497</v>
       </c>
       <c r="D11" s="2">
-        <v>115.057408002718</v>
+        <v>116.691284650949</v>
       </c>
       <c r="E11" s="2">
-        <v>4.501</v>
-      </c>
-      <c r="I11" s="4"/>
+        <v>2.532</v>
+      </c>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
@@ -1551,15 +1701,15 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>3.2</v>
+        <v>2.494</v>
       </c>
       <c r="D12" s="2">
-        <v>124.713898502435</v>
+        <v>120.536989768912</v>
       </c>
       <c r="E12" s="2">
-        <v>3.236</v>
-      </c>
-      <c r="I12" s="4"/>
+        <v>3.148</v>
+      </c>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
@@ -1569,15 +1719,15 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>2.485</v>
+        <v>4.4</v>
       </c>
       <c r="D13" s="2">
-        <v>128.356493535591</v>
+        <v>115.16170637888</v>
       </c>
       <c r="E13" s="2">
-        <v>3.06</v>
-      </c>
-      <c r="I13" s="4"/>
+        <v>4.447</v>
+      </c>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
@@ -1587,15 +1737,15 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>3.6</v>
+        <v>4.595</v>
       </c>
       <c r="D14" s="2">
-        <v>120.217980114154</v>
+        <v>120.293335925331</v>
       </c>
       <c r="E14" s="2">
-        <v>4.967</v>
-      </c>
-      <c r="I14" s="4"/>
+        <v>3.203</v>
+      </c>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
@@ -1605,15 +1755,15 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>3.96</v>
+        <v>2.485</v>
       </c>
       <c r="D15" s="2">
-        <v>120.299141797923</v>
+        <v>128.455979300584</v>
       </c>
       <c r="E15" s="2">
-        <v>4.315</v>
-      </c>
-      <c r="I15" s="4"/>
+        <v>3.006</v>
+      </c>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
@@ -1623,15 +1773,15 @@
         <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>2.996</v>
+        <v>3.6</v>
       </c>
       <c r="D16" s="2">
-        <v>119.898986041026</v>
+        <v>120.29490835667</v>
       </c>
       <c r="E16" s="2">
-        <v>2.51</v>
-      </c>
-      <c r="I16" s="4"/>
+        <v>4.912</v>
+      </c>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
@@ -1641,15 +1791,15 @@
         <v>36</v>
       </c>
       <c r="C17" s="2">
-        <v>2.216</v>
+        <v>4.993</v>
       </c>
       <c r="D17" s="2">
-        <v>117.338230070739</v>
+        <v>119.486766190884</v>
       </c>
       <c r="E17" s="2">
-        <v>1.995</v>
-      </c>
-      <c r="I17" s="4"/>
+        <v>2.888</v>
+      </c>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
@@ -1659,15 +1809,15 @@
         <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>3.997</v>
+        <v>3.96</v>
       </c>
       <c r="D18" s="2">
-        <v>119.502247619324</v>
+        <v>120.380551963968</v>
       </c>
       <c r="E18" s="2">
-        <v>2.559</v>
-      </c>
-      <c r="I18" s="4"/>
+        <v>4.26</v>
+      </c>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
@@ -1677,15 +1827,15 @@
         <v>40</v>
       </c>
       <c r="C19" s="2">
-        <v>4.595</v>
+        <v>3.87</v>
       </c>
       <c r="D19" s="2">
-        <v>120.11175275425</v>
+        <v>121.533378831596</v>
       </c>
       <c r="E19" s="2">
-        <v>3.258</v>
-      </c>
-      <c r="I19" s="4"/>
+        <v>4.159</v>
+      </c>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
@@ -1698,12 +1848,12 @@
         <v>4.53</v>
       </c>
       <c r="D20" s="2">
-        <v>124.063945311645</v>
+        <v>124.160376834716</v>
       </c>
       <c r="E20" s="2">
-        <v>2.625</v>
-      </c>
-      <c r="I20" s="4"/>
+        <v>2.57</v>
+      </c>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
@@ -1713,15 +1863,15 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>3.87</v>
+        <v>2.216</v>
       </c>
       <c r="D21" s="2">
-        <v>121.337101958881</v>
+        <v>117.356733299704</v>
       </c>
       <c r="E21" s="2">
-        <v>4.214</v>
-      </c>
-      <c r="I21" s="4"/>
+        <v>1.94</v>
+      </c>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
@@ -1731,15 +1881,15 @@
         <v>46</v>
       </c>
       <c r="C22" s="2">
-        <v>3.799</v>
+        <v>3.997</v>
       </c>
       <c r="D22" s="2">
-        <v>121.094190356348</v>
+        <v>119.526832547555</v>
       </c>
       <c r="E22" s="2">
-        <v>4.921</v>
-      </c>
-      <c r="I22" s="4"/>
+        <v>2.504</v>
+      </c>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
@@ -1749,15 +1899,15 @@
         <v>48</v>
       </c>
       <c r="C23" s="2">
-        <v>2.188</v>
+        <v>4.997</v>
       </c>
       <c r="D23" s="2">
-        <v>119.376286174947</v>
+        <v>121.268626636971</v>
       </c>
       <c r="E23" s="2">
-        <v>2.685</v>
-      </c>
-      <c r="I23" s="4"/>
+        <v>4.463</v>
+      </c>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
@@ -1767,15 +1917,15 @@
         <v>50</v>
       </c>
       <c r="C24" s="2">
-        <v>3.325</v>
+        <v>2.698</v>
       </c>
       <c r="D24" s="2">
-        <v>121.278711917137</v>
+        <v>122.419706863928</v>
       </c>
       <c r="E24" s="2">
-        <v>4.606</v>
-      </c>
-      <c r="I24" s="4"/>
+        <v>2.247</v>
+      </c>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
@@ -1785,15 +1935,15 @@
         <v>52</v>
       </c>
       <c r="C25" s="2">
-        <v>4.993</v>
+        <v>4.832</v>
       </c>
       <c r="D25" s="2">
-        <v>119.359190640898</v>
+        <v>114.161937455809</v>
       </c>
       <c r="E25" s="2">
-        <v>2.943</v>
-      </c>
-      <c r="I25" s="4"/>
+        <v>4.501</v>
+      </c>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
@@ -1803,15 +1953,15 @@
         <v>54</v>
       </c>
       <c r="C26" s="2">
-        <v>2.943</v>
+        <v>3.799</v>
       </c>
       <c r="D26" s="2">
-        <v>119.072777235544</v>
+        <v>121.219639228263</v>
       </c>
       <c r="E26" s="2">
-        <v>4.751</v>
-      </c>
-      <c r="I26" s="4"/>
+        <v>4.866</v>
+      </c>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
@@ -1821,15 +1971,15 @@
         <v>56</v>
       </c>
       <c r="C27" s="2">
-        <v>4.9</v>
+        <v>4.999</v>
       </c>
       <c r="D27" s="2">
-        <v>120.376688696152</v>
+        <v>121.344976441918</v>
       </c>
       <c r="E27" s="2">
-        <v>4.907</v>
-      </c>
-      <c r="I27" s="4"/>
+        <v>4.466</v>
+      </c>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
@@ -1839,15 +1989,15 @@
         <v>58</v>
       </c>
       <c r="C28" s="2">
-        <v>2.037</v>
+        <v>4.9</v>
       </c>
       <c r="D28" s="2">
-        <v>120.686852696566</v>
+        <v>120.517390063568</v>
       </c>
       <c r="E28" s="2">
-        <v>4.192</v>
-      </c>
-      <c r="I28" s="4"/>
+        <v>4.852</v>
+      </c>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
@@ -1857,15 +2007,15 @@
         <v>60</v>
       </c>
       <c r="C29" s="2">
-        <v>4.5</v>
+        <v>3.325</v>
       </c>
       <c r="D29" s="2">
-        <v>114.340963045083</v>
+        <v>121.420209798318</v>
       </c>
       <c r="E29" s="2">
-        <v>4.967</v>
-      </c>
-      <c r="I29" s="4"/>
+        <v>4.551</v>
+      </c>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
@@ -1875,15 +2025,15 @@
         <v>62</v>
       </c>
       <c r="C30" s="2">
-        <v>4.583</v>
+        <v>2.188</v>
       </c>
       <c r="D30" s="2">
-        <v>113.336049003838</v>
+        <v>119.389540644629</v>
       </c>
       <c r="E30" s="2">
-        <v>2.162</v>
-      </c>
-      <c r="I30" s="4"/>
+        <v>2.63</v>
+      </c>
+      <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
@@ -1893,15 +2043,15 @@
         <v>64</v>
       </c>
       <c r="C31" s="2">
-        <v>4.832</v>
+        <v>4.1</v>
       </c>
       <c r="D31" s="2">
-        <v>114.044734827006</v>
+        <v>121.293799899794</v>
       </c>
       <c r="E31" s="2">
-        <v>4.556</v>
-      </c>
-      <c r="I31" s="4"/>
+        <v>4.51</v>
+      </c>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
@@ -1911,15 +2061,15 @@
         <v>66</v>
       </c>
       <c r="C32" s="2">
-        <v>4.997</v>
+        <v>4.5</v>
       </c>
       <c r="D32" s="2">
-        <v>121.021561046122</v>
+        <v>114.426651426972</v>
       </c>
       <c r="E32" s="2">
-        <v>4.518</v>
-      </c>
-      <c r="I32" s="4"/>
+        <v>4.912</v>
+      </c>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
@@ -1929,15 +2079,15 @@
         <v>68</v>
       </c>
       <c r="C33" s="2">
-        <v>2.999</v>
+        <v>2.17</v>
       </c>
       <c r="D33" s="2">
-        <v>121.118691622955</v>
+        <v>115.671069761495</v>
       </c>
       <c r="E33" s="2">
-        <v>4.849</v>
-      </c>
-      <c r="I33" s="4"/>
+        <v>2.236</v>
+      </c>
+      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
@@ -1947,15 +2097,15 @@
         <v>70</v>
       </c>
       <c r="C34" s="2">
-        <v>4.1</v>
+        <v>2.037</v>
       </c>
       <c r="D34" s="2">
-        <v>121.151656502254</v>
+        <v>120.745753882064</v>
       </c>
       <c r="E34" s="2">
-        <v>4.564</v>
-      </c>
-      <c r="I34" s="4"/>
+        <v>4.137</v>
+      </c>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
@@ -1965,15 +2115,15 @@
         <v>72</v>
       </c>
       <c r="C35" s="2">
-        <v>4.993</v>
+        <v>4.767</v>
       </c>
       <c r="D35" s="2">
-        <v>120.113295713659</v>
+        <v>113.382775566767</v>
       </c>
       <c r="E35" s="2">
-        <v>4.499</v>
-      </c>
-      <c r="I35" s="4"/>
+        <v>2.992</v>
+      </c>
+      <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
@@ -1983,15 +2133,15 @@
         <v>74</v>
       </c>
       <c r="C36" s="2">
-        <v>4.999</v>
+        <v>3.969</v>
       </c>
       <c r="D36" s="2">
-        <v>121.126102709602</v>
+        <v>121.077923318133</v>
       </c>
       <c r="E36" s="2">
-        <v>4.521</v>
-      </c>
-      <c r="I36" s="4"/>
+        <v>4.581</v>
+      </c>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="2" t="s">
@@ -2001,15 +2151,15 @@
         <v>76</v>
       </c>
       <c r="C37" s="2">
-        <v>3.969</v>
+        <v>4.3</v>
       </c>
       <c r="D37" s="2">
-        <v>120.9031795667</v>
+        <v>114.441923608872</v>
       </c>
       <c r="E37" s="2">
-        <v>4.636</v>
-      </c>
-      <c r="I37" s="4"/>
+        <v>4.586</v>
+      </c>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
@@ -2019,15 +2169,15 @@
         <v>78</v>
       </c>
       <c r="C38" s="2">
-        <v>4.3</v>
+        <v>3.792</v>
       </c>
       <c r="D38" s="2">
-        <v>114.283822030466</v>
+        <v>120.256446679711</v>
       </c>
       <c r="E38" s="2">
-        <v>4.641</v>
-      </c>
-      <c r="I38" s="4"/>
+        <v>4.225</v>
+      </c>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
@@ -2037,15 +2187,15 @@
         <v>80</v>
       </c>
       <c r="C39" s="2">
-        <v>3.792</v>
+        <v>3.4</v>
       </c>
       <c r="D39" s="2">
-        <v>120.094384652916</v>
+        <v>121.255611113303</v>
       </c>
       <c r="E39" s="2">
-        <v>4.28</v>
-      </c>
-      <c r="I39" s="4"/>
+        <v>4.51</v>
+      </c>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
@@ -2055,13 +2205,13 @@
         <v>82</v>
       </c>
       <c r="C40" s="2">
-        <v>2.086</v>
+        <v>3.999</v>
       </c>
       <c r="D40" s="2">
-        <v>113.978107727346</v>
+        <v>118.954900293213</v>
       </c>
       <c r="E40" s="2">
-        <v>2.255</v>
+        <v>4.436</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2072,13 +2222,13 @@
         <v>84</v>
       </c>
       <c r="C41" s="2">
-        <v>4.767</v>
+        <v>2.496</v>
       </c>
       <c r="D41" s="2">
-        <v>114.244722700767</v>
+        <v>122.386601688</v>
       </c>
       <c r="E41" s="2">
-        <v>3.047</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2089,13 +2239,13 @@
         <v>86</v>
       </c>
       <c r="C42" s="2">
-        <v>3.797</v>
+        <v>2.999</v>
       </c>
       <c r="D42" s="2">
-        <v>116.44489293139</v>
+        <v>121.249562289109</v>
       </c>
       <c r="E42" s="2">
-        <v>3.118</v>
+        <v>4.795</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2106,13 +2256,13 @@
         <v>88</v>
       </c>
       <c r="C43" s="2">
-        <v>2.17</v>
+        <v>3.797</v>
       </c>
       <c r="D43" s="2">
-        <v>115.54575529836</v>
+        <v>116.583387068428</v>
       </c>
       <c r="E43" s="2">
-        <v>2.29</v>
+        <v>3.063</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2123,13 +2273,13 @@
         <v>90</v>
       </c>
       <c r="C44" s="2">
-        <v>3.016</v>
+        <v>2.923</v>
       </c>
       <c r="D44" s="2">
-        <v>111.977713064067</v>
+        <v>124.220967788537</v>
       </c>
       <c r="E44" s="2">
-        <v>1.644</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2140,13 +2290,13 @@
         <v>92</v>
       </c>
       <c r="C45" s="2">
-        <v>4.949</v>
+        <v>2.943</v>
       </c>
       <c r="D45" s="2">
-        <v>111.888569414535</v>
+        <v>119.138612742009</v>
       </c>
       <c r="E45" s="2">
-        <v>4.652</v>
+        <v>4.696</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2157,13 +2307,13 @@
         <v>94</v>
       </c>
       <c r="C46" s="2">
-        <v>2.999</v>
+        <v>3.4</v>
       </c>
       <c r="D46" s="2">
-        <v>111.773796890189</v>
+        <v>120.937769214249</v>
       </c>
       <c r="E46" s="2">
-        <v>1.633</v>
+        <v>4.915</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2174,13 +2324,13 @@
         <v>96</v>
       </c>
       <c r="C47" s="2">
-        <v>3.199</v>
+        <v>4.189</v>
       </c>
       <c r="D47" s="2">
-        <v>113.890917093887</v>
+        <v>119.050675281673</v>
       </c>
       <c r="E47" s="2">
-        <v>2.578</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2191,13 +2341,13 @@
         <v>98</v>
       </c>
       <c r="C48" s="2">
-        <v>2.945</v>
+        <v>4.999</v>
       </c>
       <c r="D48" s="2">
-        <v>113.732399644775</v>
+        <v>120.093595805672</v>
       </c>
       <c r="E48" s="2">
-        <v>1.989</v>
+        <v>4.186</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2208,529 +2358,793 @@
         <v>100</v>
       </c>
       <c r="C49" s="2">
+        <v>3.06</v>
+      </c>
+      <c r="D49" s="2">
+        <v>119.038758481555</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2.926</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="2">
+        <v>4.993</v>
+      </c>
+      <c r="D50" s="2">
+        <v>120.170198990878</v>
+      </c>
+      <c r="E50" s="2">
+        <v>4.444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2.673</v>
+      </c>
+      <c r="D51" s="2">
+        <v>120.307112507042</v>
+      </c>
+      <c r="E51" s="2">
+        <v>4.178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="D52" s="2">
+        <v>121.294669192743</v>
+      </c>
+      <c r="E52" s="2">
+        <v>4.743</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3.977</v>
+      </c>
+      <c r="D53" s="2">
+        <v>117.373564938565</v>
+      </c>
+      <c r="E53" s="2">
+        <v>4.836</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="2">
+        <v>5</v>
+      </c>
+      <c r="D54" s="2">
+        <v>117.766735131047</v>
+      </c>
+      <c r="E54" s="2">
+        <v>4.858</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3.349</v>
+      </c>
+      <c r="D55" s="2">
+        <v>121.066671214477</v>
+      </c>
+      <c r="E55" s="2">
+        <v>4.699</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2.98</v>
+      </c>
+      <c r="D56" s="2">
+        <v>122.33536941224</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2.532</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="2">
+        <v>3.016</v>
+      </c>
+      <c r="D57" s="2">
+        <v>112.007267464518</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1.589</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4.649</v>
+      </c>
+      <c r="D58" s="2">
+        <v>120.010292278187</v>
+      </c>
+      <c r="E58" s="2">
+        <v>3.964</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="2">
+        <v>4.583</v>
+      </c>
+      <c r="D59" s="2">
+        <v>113.309914955555</v>
+      </c>
+      <c r="E59" s="2">
+        <v>2.107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="2">
+        <v>3.297</v>
+      </c>
+      <c r="D60" s="2">
+        <v>117.12573570073</v>
+      </c>
+      <c r="E60" s="2">
+        <v>4.203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="2">
+        <v>4.499</v>
+      </c>
+      <c r="D61" s="2">
+        <v>116.821166864057</v>
+      </c>
+      <c r="E61" s="2">
+        <v>4.682</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="2">
+        <v>3.008</v>
+      </c>
+      <c r="D62" s="2">
+        <v>119.20789307617</v>
+      </c>
+      <c r="E62" s="2">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2.999</v>
+      </c>
+      <c r="D63" s="2">
+        <v>111.799</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1.578</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="2">
+        <v>2.247</v>
+      </c>
+      <c r="D64" s="2">
+        <v>115.996486521172</v>
+      </c>
+      <c r="E64" s="2">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D65" s="2">
+        <v>120.582816390289</v>
+      </c>
+      <c r="E65" s="2">
+        <v>4.885</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="2">
+        <v>4.984</v>
+      </c>
+      <c r="D66" s="2">
+        <v>115.296689122954</v>
+      </c>
+      <c r="E66" s="2">
+        <v>2.926</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="2">
+        <v>2.086</v>
+      </c>
+      <c r="D67" s="2">
+        <v>113.977123431856</v>
+      </c>
+      <c r="E67" s="2">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="2">
+        <v>4.949</v>
+      </c>
+      <c r="D68" s="2">
+        <v>112.0063404349</v>
+      </c>
+      <c r="E68" s="2">
+        <v>4.597</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="2">
+        <v>3.755</v>
+      </c>
+      <c r="D69" s="2">
+        <v>116.283686012766</v>
+      </c>
+      <c r="E69" s="2">
+        <v>3.816</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="2">
         <v>3.79</v>
       </c>
-      <c r="D49" s="2">
-        <v>111.135311586902</v>
-      </c>
-      <c r="E49" s="2">
-        <v>2.282</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
+      <c r="D70" s="2">
+        <v>111.265970168352</v>
+      </c>
+      <c r="E70" s="2">
+        <v>2.227</v>
+      </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
+      <c r="A71" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" s="2">
+        <v>2.988</v>
+      </c>
+      <c r="D71" s="2">
+        <v>113.272985338456</v>
+      </c>
+      <c r="E71" s="2">
+        <v>2.159</v>
+      </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
+      <c r="A72" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="2">
+        <v>4.531</v>
+      </c>
+      <c r="D72" s="2">
+        <v>113.223428882955</v>
+      </c>
+      <c r="E72" s="2">
+        <v>2.069</v>
+      </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
+      <c r="A73" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" s="2">
+        <v>2.945</v>
+      </c>
+      <c r="D73" s="2">
+        <v>113.747043576972</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1.934</v>
+      </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="A74" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" s="2">
+        <v>4.172</v>
+      </c>
+      <c r="D74" s="2">
+        <v>113.193778289982</v>
+      </c>
+      <c r="E74" s="2">
+        <v>2.356</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="3"/>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="3"/>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1.update kgooglist for track the holdings
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>code</t>
   </si>
@@ -44,70 +44,172 @@
     <t>lastyear</t>
   </si>
   <si>
+    <t>sh113600</t>
+  </si>
+  <si>
+    <t>新星转债</t>
+  </si>
+  <si>
+    <t>sz123156</t>
+  </si>
+  <si>
+    <t>博汇转债</t>
+  </si>
+  <si>
+    <t>sh118016</t>
+  </si>
+  <si>
+    <t>京源转债</t>
+  </si>
+  <si>
+    <t>sh113665</t>
+  </si>
+  <si>
+    <t>汇通转债</t>
+  </si>
+  <si>
+    <t>sz123175</t>
+  </si>
+  <si>
+    <t>百畅转债</t>
+  </si>
+  <si>
+    <t>sz128118</t>
+  </si>
+  <si>
+    <t>瀛通转债</t>
+  </si>
+  <si>
+    <t>sz128138</t>
+  </si>
+  <si>
+    <t>侨银转债</t>
+  </si>
+  <si>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>中陆转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
+    <t>sh118018</t>
+  </si>
+  <si>
+    <t>瑞科转债</t>
+  </si>
+  <si>
+    <t>sz123189</t>
+  </si>
+  <si>
+    <t>晓鸣转债</t>
+  </si>
+  <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
+    <t>sh113565</t>
+  </si>
+  <si>
+    <t>宏辉转债</t>
+  </si>
+  <si>
+    <t>sh118007</t>
+  </si>
+  <si>
+    <t>山石转债</t>
+  </si>
+  <si>
     <t>sh113610</t>
   </si>
   <si>
     <t>灵康转债</t>
   </si>
   <si>
-    <t>sh118016</t>
-  </si>
-  <si>
-    <t>京源转债</t>
-  </si>
-  <si>
-    <t>sh113600</t>
-  </si>
-  <si>
-    <t>新星转债</t>
-  </si>
-  <si>
-    <t>sz128138</t>
-  </si>
-  <si>
-    <t>侨银转债</t>
-  </si>
-  <si>
-    <t>sz128118</t>
-  </si>
-  <si>
-    <t>瀛通转债</t>
-  </si>
-  <si>
-    <t>sz123175</t>
-  </si>
-  <si>
-    <t>百畅转债</t>
-  </si>
-  <si>
-    <t>sz123155</t>
-  </si>
-  <si>
-    <t>中陆转债</t>
-  </si>
-  <si>
-    <t>sz123156</t>
-  </si>
-  <si>
-    <t>博汇转债</t>
-  </si>
-  <si>
-    <t>sh113608</t>
-  </si>
-  <si>
-    <t>威派转债</t>
-  </si>
-  <si>
-    <t>sh113665</t>
-  </si>
-  <si>
-    <t>汇通转债</t>
-  </si>
-  <si>
-    <t>sz123153</t>
-  </si>
-  <si>
-    <t>英力转债</t>
+    <t>sz128101</t>
+  </si>
+  <si>
+    <t>联创转债</t>
+  </si>
+  <si>
+    <t>sz123166</t>
+  </si>
+  <si>
+    <t>蒙泰转债</t>
+  </si>
+  <si>
+    <t>sh110070</t>
+  </si>
+  <si>
+    <t>凌钢转债</t>
+  </si>
+  <si>
+    <t>sz123103</t>
+  </si>
+  <si>
+    <t>震安转债</t>
+  </si>
+  <si>
+    <t>sh113649</t>
+  </si>
+  <si>
+    <t>丰山转债</t>
+  </si>
+  <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
+    <t>sz123126</t>
+  </si>
+  <si>
+    <t>瑞丰转债</t>
+  </si>
+  <si>
+    <t>sz123171</t>
+  </si>
+  <si>
+    <t>共同转债</t>
+  </si>
+  <si>
+    <t>sz123157</t>
+  </si>
+  <si>
+    <t>科蓝转债</t>
+  </si>
+  <si>
+    <t>sh113624</t>
+  </si>
+  <si>
+    <t>正川转债</t>
+  </si>
+  <si>
+    <t>sz123196</t>
+  </si>
+  <si>
+    <t>正元转02</t>
+  </si>
+  <si>
+    <t>sh113593</t>
+  </si>
+  <si>
+    <t>沪工转债</t>
+  </si>
+  <si>
+    <t>sz128125</t>
+  </si>
+  <si>
+    <t>华阳转债</t>
   </si>
   <si>
     <t>sh118010</t>
@@ -116,58 +218,10 @@
     <t>洁特转债</t>
   </si>
   <si>
-    <t>sh118007</t>
-  </si>
-  <si>
-    <t>山石转债</t>
-  </si>
-  <si>
-    <t>sz123189</t>
-  </si>
-  <si>
-    <t>晓鸣转债</t>
-  </si>
-  <si>
-    <t>sz123171</t>
-  </si>
-  <si>
-    <t>共同转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
-  </si>
-  <si>
-    <t>sh118018</t>
-  </si>
-  <si>
-    <t>瑞科转债</t>
-  </si>
-  <si>
-    <t>sz123103</t>
-  </si>
-  <si>
-    <t>震安转债</t>
-  </si>
-  <si>
-    <t>sh113624</t>
-  </si>
-  <si>
-    <t>正川转债</t>
-  </si>
-  <si>
-    <t>sz123126</t>
-  </si>
-  <si>
-    <t>瑞丰转债</t>
-  </si>
-  <si>
-    <t>sz123166</t>
-  </si>
-  <si>
-    <t>蒙泰转债</t>
+    <t>sz123093</t>
+  </si>
+  <si>
+    <t>金陵转债</t>
   </si>
   <si>
     <t>sh118029</t>
@@ -176,10 +230,22 @@
     <t>富淼转债</t>
   </si>
   <si>
-    <t>sz128117</t>
-  </si>
-  <si>
-    <t>道恩转债</t>
+    <t>sh113618</t>
+  </si>
+  <si>
+    <t>美诺转债</t>
+  </si>
+  <si>
+    <t>sz128097</t>
+  </si>
+  <si>
+    <t>奥佳转债</t>
+  </si>
+  <si>
+    <t>sh113628</t>
+  </si>
+  <si>
+    <t>晨丰转债</t>
   </si>
   <si>
     <t>sz127062</t>
@@ -188,10 +254,88 @@
     <t>垒知转债</t>
   </si>
   <si>
-    <t>sz128125</t>
-  </si>
-  <si>
-    <t>华阳转债</t>
+    <t>sz123065</t>
+  </si>
+  <si>
+    <t>宝莱转债</t>
+  </si>
+  <si>
+    <t>sh113575</t>
+  </si>
+  <si>
+    <t>东时转债</t>
+  </si>
+  <si>
+    <t>sz127059</t>
+  </si>
+  <si>
+    <t>永东转2</t>
+  </si>
+  <si>
+    <t>sz123180</t>
+  </si>
+  <si>
+    <t>浙矿转债</t>
+  </si>
+  <si>
+    <t>sz123067</t>
+  </si>
+  <si>
+    <t>斯莱转债</t>
+  </si>
+  <si>
+    <t>sh113643</t>
+  </si>
+  <si>
+    <t>风语转债</t>
+  </si>
+  <si>
+    <t>sh118014</t>
+  </si>
+  <si>
+    <t>高测转债</t>
+  </si>
+  <si>
+    <t>sz123168</t>
+  </si>
+  <si>
+    <t>惠云转债</t>
+  </si>
+  <si>
+    <t>sz127087</t>
+  </si>
+  <si>
+    <t>星帅转2</t>
+  </si>
+  <si>
+    <t>sh118015</t>
+  </si>
+  <si>
+    <t>芯海转债</t>
+  </si>
+  <si>
+    <t>sz123088</t>
+  </si>
+  <si>
+    <t>威唐转债</t>
+  </si>
+  <si>
+    <t>sz123185</t>
+  </si>
+  <si>
+    <t>能辉转债</t>
+  </si>
+  <si>
+    <t>sh118035</t>
+  </si>
+  <si>
+    <t>国力转债</t>
+  </si>
+  <si>
+    <t>sh113597</t>
+  </si>
+  <si>
+    <t>佳力转债</t>
   </si>
   <si>
     <t>sh118011</t>
@@ -200,28 +344,10 @@
     <t>银微转债</t>
   </si>
   <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
-  </si>
-  <si>
-    <t>sh113593</t>
-  </si>
-  <si>
-    <t>沪工转债</t>
-  </si>
-  <si>
-    <t>sz123093</t>
-  </si>
-  <si>
-    <t>金陵转债</t>
-  </si>
-  <si>
-    <t>sz123196</t>
-  </si>
-  <si>
-    <t>正元转02</t>
+    <t>sz123059</t>
+  </si>
+  <si>
+    <t>银信转债</t>
   </si>
   <si>
     <t>sh118006</t>
@@ -230,10 +356,28 @@
     <t>阿拉转债</t>
   </si>
   <si>
-    <t>sz123180</t>
-  </si>
-  <si>
-    <t>浙矿转债</t>
+    <t>sz123163</t>
+  </si>
+  <si>
+    <t>金沃转债</t>
+  </si>
+  <si>
+    <t>sz123100</t>
+  </si>
+  <si>
+    <t>朗科转债</t>
+  </si>
+  <si>
+    <t>sh118009</t>
+  </si>
+  <si>
+    <t>XD华锐转</t>
+  </si>
+  <si>
+    <t>sz123160</t>
+  </si>
+  <si>
+    <t>泰福转债</t>
   </si>
   <si>
     <t>sz123159</t>
@@ -242,76 +386,52 @@
     <t>崧盛转债</t>
   </si>
   <si>
-    <t>sz123185</t>
-  </si>
-  <si>
-    <t>能辉转债</t>
-  </si>
-  <si>
     <t>sz123109</t>
   </si>
   <si>
     <t>昌红转债</t>
   </si>
   <si>
-    <t>sh118014</t>
-  </si>
-  <si>
-    <t>高测转债</t>
-  </si>
-  <si>
-    <t>sz123100</t>
-  </si>
-  <si>
-    <t>朗科转债</t>
-  </si>
-  <si>
-    <t>sz123065</t>
-  </si>
-  <si>
-    <t>宝莱转债</t>
-  </si>
-  <si>
-    <t>sh118015</t>
-  </si>
-  <si>
-    <t>芯海转债</t>
-  </si>
-  <si>
-    <t>sz123163</t>
-  </si>
-  <si>
-    <t>金沃转债</t>
-  </si>
-  <si>
-    <t>sz123157</t>
-  </si>
-  <si>
-    <t>科蓝转债</t>
-  </si>
-  <si>
-    <t>sz127059</t>
-  </si>
-  <si>
-    <t>永东转2</t>
-  </si>
-  <si>
-    <t>sz123089</t>
-  </si>
-  <si>
-    <t>九洲转2</t>
-  </si>
-  <si>
-    <t>sh110070</t>
-  </si>
-  <si>
-    <t>凌钢转债</t>
-  </si>
-  <si>
-    <t>sh113649</t>
-  </si>
-  <si>
-    <t>丰山转债</t>
+    <t>sz128095</t>
+  </si>
+  <si>
+    <t>恩捷转债</t>
+  </si>
+  <si>
+    <t>sz123039</t>
+  </si>
+  <si>
+    <t>开润转债</t>
+  </si>
+  <si>
+    <t>sz123061</t>
+  </si>
+  <si>
+    <t>航新转债</t>
+  </si>
+  <si>
+    <t>sz123173</t>
+  </si>
+  <si>
+    <t>恒锋转债</t>
+  </si>
+  <si>
+    <t>sz123152</t>
+  </si>
+  <si>
+    <t>润禾转债</t>
+  </si>
+  <si>
+    <t>sz128120</t>
+  </si>
+  <si>
+    <t>联诚转债</t>
+  </si>
+  <si>
+    <t>sz123141</t>
+  </si>
+  <si>
+    <t>宏丰转债</t>
   </si>
   <si>
     <t>sz127079</t>
@@ -320,82 +440,70 @@
     <t>华亚转债</t>
   </si>
   <si>
-    <t>sh113618</t>
-  </si>
-  <si>
-    <t>美诺转债</t>
-  </si>
-  <si>
-    <t>sz123160</t>
-  </si>
-  <si>
-    <t>泰福转债</t>
-  </si>
-  <si>
-    <t>sz128097</t>
-  </si>
-  <si>
-    <t>奥佳转债</t>
-  </si>
-  <si>
-    <t>sh113573</t>
-  </si>
-  <si>
-    <t>纵横转债</t>
-  </si>
-  <si>
-    <t>sh118009</t>
-  </si>
-  <si>
-    <t>华锐转债</t>
-  </si>
-  <si>
-    <t>sz123067</t>
-  </si>
-  <si>
-    <t>斯莱转债</t>
-  </si>
-  <si>
-    <t>sz123141</t>
-  </si>
-  <si>
-    <t>宏丰转债</t>
-  </si>
-  <si>
-    <t>sz123061</t>
-  </si>
-  <si>
-    <t>航新转债</t>
-  </si>
-  <si>
-    <t>sh113643</t>
-  </si>
-  <si>
-    <t>风语转债</t>
-  </si>
-  <si>
-    <t>sz123168</t>
-  </si>
-  <si>
-    <t>惠云转债</t>
-  </si>
-  <si>
-    <t>sz123152</t>
-  </si>
-  <si>
-    <t>润禾转债</t>
-  </si>
-  <si>
-    <t>sz123173</t>
-  </si>
-  <si>
-    <t>恒锋转债</t>
-  </si>
-  <si>
-    <t>sh113628</t>
-  </si>
-  <si>
-    <t>晨丰转债</t>
+    <t>sh118012</t>
+  </si>
+  <si>
+    <t>微芯转债</t>
+  </si>
+  <si>
+    <t>sz127053</t>
+  </si>
+  <si>
+    <t>豪美转债</t>
+  </si>
+  <si>
+    <t>sz123112</t>
+  </si>
+  <si>
+    <t>万讯转债</t>
+  </si>
+  <si>
+    <t>sh113660</t>
+  </si>
+  <si>
+    <t>寿22转债</t>
+  </si>
+  <si>
+    <t>sz123187</t>
+  </si>
+  <si>
+    <t>超达转债</t>
+  </si>
+  <si>
+    <t>sz123138</t>
+  </si>
+  <si>
+    <t>丝路转债</t>
+  </si>
+  <si>
+    <t>sh111003</t>
+  </si>
+  <si>
+    <t>聚合转债</t>
+  </si>
+  <si>
+    <t>sh113664</t>
+  </si>
+  <si>
+    <t>大元转债</t>
+  </si>
+  <si>
+    <t>sz123197</t>
+  </si>
+  <si>
+    <t>光力转债</t>
+  </si>
+  <si>
+    <t>sz123090</t>
+  </si>
+  <si>
+    <t>三诺转债</t>
+  </si>
+  <si>
+    <t>sz123129</t>
+  </si>
+  <si>
+    <t>锦鸡转债</t>
   </si>
   <si>
     <t>sz123044</t>
@@ -404,16 +512,10 @@
     <t>红相转债</t>
   </si>
   <si>
-    <t>sz123039</t>
-  </si>
-  <si>
-    <t>开润转债</t>
-  </si>
-  <si>
-    <t>sh113597</t>
-  </si>
-  <si>
-    <t>佳力转债</t>
+    <t>sh111012</t>
+  </si>
+  <si>
+    <t>福新转债</t>
   </si>
   <si>
     <t>sh111013</t>
@@ -422,76 +524,82 @@
     <t>新港转债</t>
   </si>
   <si>
+    <t>sz128143</t>
+  </si>
+  <si>
+    <t>锋龙转债</t>
+  </si>
+  <si>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>华体转债</t>
+  </si>
+  <si>
+    <t>sh111008</t>
+  </si>
+  <si>
+    <t>沿浦转债</t>
+  </si>
+  <si>
+    <t>sz127071</t>
+  </si>
+  <si>
+    <t>天箭转债</t>
+  </si>
+  <si>
+    <t>sz127072</t>
+  </si>
+  <si>
+    <t>博实转债</t>
+  </si>
+  <si>
+    <t>sz123050</t>
+  </si>
+  <si>
+    <t>聚飞转债</t>
+  </si>
+  <si>
+    <t>sz128090</t>
+  </si>
+  <si>
+    <t>汽模转2</t>
+  </si>
+  <si>
+    <t>sh113030</t>
+  </si>
+  <si>
+    <t>东风转债</t>
+  </si>
+  <si>
     <t>sz123130</t>
   </si>
   <si>
     <t>设研转债</t>
   </si>
   <si>
-    <t>sz123087</t>
-  </si>
-  <si>
-    <t>明电转债</t>
-  </si>
-  <si>
-    <t>sh113660</t>
-  </si>
-  <si>
-    <t>寿22转债</t>
-  </si>
-  <si>
-    <t>sh118012</t>
-  </si>
-  <si>
-    <t>微芯转债</t>
-  </si>
-  <si>
-    <t>sz128101</t>
-  </si>
-  <si>
-    <t>联创转债</t>
-  </si>
-  <si>
-    <t>sz123088</t>
-  </si>
-  <si>
-    <t>威唐转债</t>
-  </si>
-  <si>
-    <t>sh111003</t>
-  </si>
-  <si>
-    <t>聚合转债</t>
-  </si>
-  <si>
-    <t>sz123090</t>
-  </si>
-  <si>
-    <t>三诺转债</t>
-  </si>
-  <si>
-    <t>sz128095</t>
-  </si>
-  <si>
-    <t>恩捷转债</t>
-  </si>
-  <si>
-    <t>sz127071</t>
-  </si>
-  <si>
-    <t>天箭转债</t>
-  </si>
-  <si>
-    <t>sh113030</t>
-  </si>
-  <si>
-    <t>东风转债</t>
-  </si>
-  <si>
-    <t>sh113574</t>
-  </si>
-  <si>
-    <t>华体转债</t>
+    <t>sz123092</t>
+  </si>
+  <si>
+    <t>天壕转债</t>
+  </si>
+  <si>
+    <t>sz127028</t>
+  </si>
+  <si>
+    <t>英特转债</t>
+  </si>
+  <si>
+    <t>sh113039</t>
+  </si>
+  <si>
+    <t>嘉泽转债</t>
+  </si>
+  <si>
+    <t>sz123048</t>
+  </si>
+  <si>
+    <t>应急转债</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1600,7 @@
   <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E76"/>
+      <selection activeCell="A2" sqref="A2:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1533,13 +1641,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>4.579</v>
+        <v>4.529</v>
       </c>
       <c r="D2" s="2">
-        <v>119.467057560122</v>
+        <v>125.199394704625</v>
       </c>
       <c r="E2" s="2">
-        <v>2.589</v>
+        <v>2.137</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -1551,13 +1659,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>3.325</v>
+        <v>3.967</v>
       </c>
       <c r="D3" s="2">
-        <v>122.129760606272</v>
+        <v>123.491784350437</v>
       </c>
       <c r="E3" s="2">
-        <v>4.269</v>
+        <v>4.148</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -1569,13 +1677,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>4.529</v>
+        <v>3.325</v>
       </c>
       <c r="D4" s="2">
-        <v>124.376161471641</v>
+        <v>122.946785877965</v>
       </c>
       <c r="E4" s="2">
-        <v>2.288</v>
+        <v>4.118</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -1587,13 +1695,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>4.199</v>
+        <v>3.599</v>
       </c>
       <c r="D5" s="2">
-        <v>134.90902011608</v>
+        <v>121.258834636404</v>
       </c>
       <c r="E5" s="2">
-        <v>2.551</v>
+        <v>4.48</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -1605,13 +1713,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>2.995</v>
+        <v>4.2</v>
       </c>
       <c r="D6" s="2">
-        <v>120.206405567296</v>
+        <v>119.162722064161</v>
       </c>
       <c r="E6" s="2">
-        <v>2.173</v>
+        <v>4.669</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -1623,13 +1731,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>4.2</v>
+        <v>2.994</v>
       </c>
       <c r="D7" s="2">
-        <v>118.434656891323</v>
+        <v>120.567083751825</v>
       </c>
       <c r="E7" s="2">
-        <v>4.819</v>
+        <v>2.022</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -1641,13 +1749,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>3.6</v>
+        <v>4.199</v>
       </c>
       <c r="D8" s="2">
-        <v>121.819029994304</v>
+        <v>135.258944833813</v>
       </c>
       <c r="E8" s="2">
-        <v>4.288</v>
+        <v>2.4</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -1659,13 +1767,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>3.969</v>
+        <v>3.6</v>
       </c>
       <c r="D9" s="2">
-        <v>121.563898404486</v>
+        <v>122.502037050428</v>
       </c>
       <c r="E9" s="2">
-        <v>4.299</v>
+        <v>4.137</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -1677,13 +1785,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>4.2</v>
+        <v>4.993</v>
       </c>
       <c r="D10" s="2">
-        <v>119.511018522426</v>
+        <v>119.892743438118</v>
       </c>
       <c r="E10" s="2">
-        <v>2.529</v>
+        <v>2.455</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -1695,13 +1803,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>3.599</v>
+        <v>4.3</v>
       </c>
       <c r="D11" s="2">
-        <v>120.520430771148</v>
+        <v>115.066861126543</v>
       </c>
       <c r="E11" s="2">
-        <v>4.63</v>
+        <v>4.153</v>
       </c>
       <c r="I11" s="3"/>
     </row>
@@ -1713,13 +1821,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>3.4</v>
+        <v>3.29</v>
       </c>
       <c r="D12" s="2">
-        <v>121.715772621902</v>
+        <v>119.940959110932</v>
       </c>
       <c r="E12" s="2">
-        <v>4.227</v>
+        <v>4.786</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1731,13 +1839,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>4.4</v>
+        <v>4.2</v>
       </c>
       <c r="D13" s="2">
-        <v>115.275475574561</v>
+        <v>119.69825173211</v>
       </c>
       <c r="E13" s="2">
-        <v>4.164</v>
+        <v>2.378</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -1749,13 +1857,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>2.672</v>
+        <v>2.247</v>
       </c>
       <c r="D14" s="2">
-        <v>119.924963576535</v>
+        <v>114.714780282128</v>
       </c>
       <c r="E14" s="2">
-        <v>3.896</v>
+        <v>1.677</v>
       </c>
       <c r="I14" s="3"/>
     </row>
@@ -1767,13 +1875,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>3.29</v>
+        <v>2.672</v>
       </c>
       <c r="D15" s="2">
-        <v>119.372695320811</v>
+        <v>120.274367641912</v>
       </c>
       <c r="E15" s="2">
-        <v>4.937</v>
+        <v>3.745</v>
       </c>
       <c r="I15" s="3"/>
     </row>
@@ -1785,13 +1893,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>3.799</v>
+        <v>4.579</v>
       </c>
       <c r="D16" s="2">
-        <v>121.504605254238</v>
+        <v>119.440016933094</v>
       </c>
       <c r="E16" s="2">
-        <v>4.584</v>
+        <v>2.438</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -1803,13 +1911,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="2">
-        <v>4.993</v>
+        <v>2.987</v>
       </c>
       <c r="D17" s="2">
-        <v>119.550515730265</v>
+        <v>111.921599852749</v>
       </c>
       <c r="E17" s="2">
-        <v>2.606</v>
+        <v>1.726</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -1821,13 +1929,13 @@
         <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>4.3</v>
+        <v>2.999</v>
       </c>
       <c r="D18" s="2">
-        <v>114.644552877627</v>
+        <v>121.971143679641</v>
       </c>
       <c r="E18" s="2">
-        <v>4.304</v>
+        <v>4.362</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -1839,13 +1947,13 @@
         <v>40</v>
       </c>
       <c r="C19" s="2">
-        <v>2.494</v>
+        <v>2.17</v>
       </c>
       <c r="D19" s="2">
-        <v>119.262939220907</v>
+        <v>114.120663565965</v>
       </c>
       <c r="E19" s="2">
-        <v>2.866</v>
+        <v>1.803</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -1857,13 +1965,13 @@
         <v>42</v>
       </c>
       <c r="C20" s="2">
-        <v>4.049</v>
+        <v>2.494</v>
       </c>
       <c r="D20" s="2">
-        <v>119.433685489795</v>
+        <v>119.391016652016</v>
       </c>
       <c r="E20" s="2">
-        <v>2.995</v>
+        <v>2.715</v>
       </c>
       <c r="I20" s="3"/>
     </row>
@@ -1875,13 +1983,13 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>3.4</v>
+        <v>4.591</v>
       </c>
       <c r="D21" s="2">
-        <v>128.913939765725</v>
+        <v>120.75922013494</v>
       </c>
       <c r="E21" s="2">
-        <v>3.364</v>
+        <v>4.011</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -1893,13 +2001,13 @@
         <v>46</v>
       </c>
       <c r="C22" s="2">
-        <v>2.999</v>
+        <v>3.582</v>
       </c>
       <c r="D22" s="2">
-        <v>121.556256332955</v>
+        <v>121.819754153922</v>
       </c>
       <c r="E22" s="2">
-        <v>4.512</v>
+        <v>2.022</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -1911,13 +2019,13 @@
         <v>48</v>
       </c>
       <c r="C23" s="2">
-        <v>4.5</v>
+        <v>3.399</v>
       </c>
       <c r="D23" s="2">
-        <v>114.619420201385</v>
+        <v>129.212522429667</v>
       </c>
       <c r="E23" s="2">
-        <v>4.63</v>
+        <v>3.214</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -1929,13 +2037,13 @@
         <v>50</v>
       </c>
       <c r="C24" s="2">
-        <v>3.583</v>
+        <v>3.799</v>
       </c>
       <c r="D24" s="2">
-        <v>121.678177987552</v>
+        <v>121.69435727835</v>
       </c>
       <c r="E24" s="2">
-        <v>2.173</v>
+        <v>4.433</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -1947,13 +2055,13 @@
         <v>52</v>
       </c>
       <c r="C25" s="2">
-        <v>3.959</v>
+        <v>4.945</v>
       </c>
       <c r="D25" s="2">
-        <v>119.796815893399</v>
+        <v>120.549462742486</v>
       </c>
       <c r="E25" s="2">
-        <v>3.978</v>
+        <v>4.186</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -1965,13 +2073,13 @@
         <v>54</v>
       </c>
       <c r="C26" s="2">
-        <v>4.497</v>
+        <v>4.049</v>
       </c>
       <c r="D26" s="2">
-        <v>116.668130240838</v>
+        <v>119.566959136015</v>
       </c>
       <c r="E26" s="2">
-        <v>2.249</v>
+        <v>2.844</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -1983,13 +2091,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2">
-        <v>4.997</v>
+        <v>3.507</v>
       </c>
       <c r="D27" s="2">
-        <v>121.395582653618</v>
+        <v>119.811236377669</v>
       </c>
       <c r="E27" s="2">
-        <v>4.181</v>
+        <v>4.819</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2001,13 +2109,13 @@
         <v>58</v>
       </c>
       <c r="C28" s="2">
-        <v>2.247</v>
+        <v>3.996</v>
       </c>
       <c r="D28" s="2">
-        <v>114.588824710135</v>
+        <v>119.752784083348</v>
       </c>
       <c r="E28" s="2">
-        <v>1.827</v>
+        <v>2.071</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2019,13 +2127,13 @@
         <v>60</v>
       </c>
       <c r="C29" s="2">
-        <v>3.996</v>
+        <v>4.497</v>
       </c>
       <c r="D29" s="2">
-        <v>119.592429459129</v>
+        <v>116.783280896444</v>
       </c>
       <c r="E29" s="2">
-        <v>2.222</v>
+        <v>2.099</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2037,13 +2145,13 @@
         <v>62</v>
       </c>
       <c r="C30" s="2">
-        <v>2.485</v>
+        <v>4.4</v>
       </c>
       <c r="D30" s="2">
-        <v>126.798541344236</v>
+        <v>115.344662052784</v>
       </c>
       <c r="E30" s="2">
-        <v>2.723</v>
+        <v>4.014</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2055,13 +2163,13 @@
         <v>64</v>
       </c>
       <c r="C31" s="2">
-        <v>3.507</v>
+        <v>2.485</v>
       </c>
       <c r="D31" s="2">
-        <v>119.531271104535</v>
+        <v>126.978702087019</v>
       </c>
       <c r="E31" s="2">
-        <v>4.97</v>
+        <v>2.573</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2073,13 +2181,13 @@
         <v>66</v>
       </c>
       <c r="C32" s="2">
-        <v>3.87</v>
+        <v>4.5</v>
       </c>
       <c r="D32" s="2">
-        <v>120.816851324061</v>
+        <v>114.736761228227</v>
       </c>
       <c r="E32" s="2">
-        <v>3.877</v>
+        <v>4.48</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -2091,13 +2199,13 @@
         <v>68</v>
       </c>
       <c r="C33" s="2">
-        <v>3.199</v>
+        <v>4.767</v>
       </c>
       <c r="D33" s="2">
-        <v>120.172916522162</v>
+        <v>113.546468937943</v>
       </c>
       <c r="E33" s="2">
-        <v>4.86</v>
+        <v>2.559</v>
       </c>
       <c r="I33" s="3"/>
     </row>
@@ -2109,13 +2217,13 @@
         <v>70</v>
       </c>
       <c r="C34" s="2">
-        <v>2.943</v>
+        <v>4.583</v>
       </c>
       <c r="D34" s="2">
-        <v>119.298874973116</v>
+        <v>111.883314020663</v>
       </c>
       <c r="E34" s="2">
-        <v>4.414</v>
+        <v>1.674</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -2127,13 +2235,13 @@
         <v>72</v>
       </c>
       <c r="C35" s="2">
-        <v>3.479</v>
+        <v>4.149</v>
       </c>
       <c r="D35" s="2">
-        <v>117.24601650809</v>
+        <v>120.924054750445</v>
       </c>
       <c r="E35" s="2">
-        <v>4.921</v>
+        <v>3.164</v>
       </c>
       <c r="I35" s="3"/>
     </row>
@@ -2145,13 +2253,13 @@
         <v>74</v>
       </c>
       <c r="C36" s="2">
-        <v>4.595</v>
+        <v>3.959</v>
       </c>
       <c r="D36" s="2">
-        <v>119.15436584774</v>
+        <v>119.875644107386</v>
       </c>
       <c r="E36" s="2">
-        <v>2.921</v>
+        <v>3.827</v>
       </c>
       <c r="I36" s="3"/>
     </row>
@@ -2163,13 +2271,13 @@
         <v>76</v>
       </c>
       <c r="C37" s="2">
-        <v>4.832</v>
+        <v>2.188</v>
       </c>
       <c r="D37" s="2">
-        <v>114.226081399469</v>
+        <v>119.572553788613</v>
       </c>
       <c r="E37" s="2">
-        <v>4.219</v>
+        <v>2.197</v>
       </c>
       <c r="I37" s="3"/>
     </row>
@@ -2181,13 +2289,13 @@
         <v>78</v>
       </c>
       <c r="C38" s="2">
-        <v>3.797</v>
+        <v>0.981</v>
       </c>
       <c r="D38" s="2">
-        <v>115.645625219598</v>
+        <v>110.096671838305</v>
       </c>
       <c r="E38" s="2">
-        <v>2.781</v>
+        <v>1.792</v>
       </c>
       <c r="I38" s="3"/>
     </row>
@@ -2199,13 +2307,13 @@
         <v>80</v>
       </c>
       <c r="C39" s="2">
-        <v>2.188</v>
+        <v>3.792</v>
       </c>
       <c r="D39" s="2">
-        <v>119.465247876824</v>
+        <v>119.845008950242</v>
       </c>
       <c r="E39" s="2">
-        <v>2.348</v>
+        <v>3.792</v>
       </c>
       <c r="I39" s="3"/>
     </row>
@@ -2217,13 +2325,13 @@
         <v>82</v>
       </c>
       <c r="C40" s="2">
-        <v>4.1</v>
+        <v>3.199</v>
       </c>
       <c r="D40" s="2">
-        <v>121.412724469428</v>
+        <v>120.276477697728</v>
       </c>
       <c r="E40" s="2">
-        <v>4.227</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2234,13 +2342,13 @@
         <v>84</v>
       </c>
       <c r="C41" s="2">
-        <v>3.099</v>
+        <v>2.393</v>
       </c>
       <c r="D41" s="2">
-        <v>121.539605276706</v>
+        <v>119.223277642045</v>
       </c>
       <c r="E41" s="2">
-        <v>4.46</v>
+        <v>2.233</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2251,13 +2359,13 @@
         <v>86</v>
       </c>
       <c r="C42" s="2">
-        <v>4.945</v>
+        <v>4.999</v>
       </c>
       <c r="D42" s="2">
-        <v>120.233541214163</v>
+        <v>119.819942501732</v>
       </c>
       <c r="E42" s="2">
-        <v>4.337</v>
+        <v>3.753</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2268,13 +2376,13 @@
         <v>88</v>
       </c>
       <c r="C43" s="2">
-        <v>3.792</v>
+        <v>4.832</v>
       </c>
       <c r="D43" s="2">
-        <v>119.692491410521</v>
+        <v>114.302080011248</v>
       </c>
       <c r="E43" s="2">
-        <v>3.943</v>
+        <v>4.069</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2285,13 +2393,13 @@
         <v>90</v>
       </c>
       <c r="C44" s="2">
-        <v>3.06</v>
+        <v>4.899</v>
       </c>
       <c r="D44" s="2">
-        <v>119.116502145841</v>
+        <v>120.693413760147</v>
       </c>
       <c r="E44" s="2">
-        <v>2.644</v>
+        <v>4.419</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2302,13 +2410,13 @@
         <v>92</v>
       </c>
       <c r="C45" s="2">
-        <v>2.17</v>
+        <v>4.629</v>
       </c>
       <c r="D45" s="2">
-        <v>114.041741092067</v>
+        <v>120.870858163033</v>
       </c>
       <c r="E45" s="2">
-        <v>1.953</v>
+        <v>4.975</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2319,13 +2427,13 @@
         <v>94</v>
       </c>
       <c r="C46" s="2">
-        <v>4.591</v>
+        <v>4.1</v>
       </c>
       <c r="D46" s="2">
-        <v>120.320386159788</v>
+        <v>121.518066626883</v>
       </c>
       <c r="E46" s="2">
-        <v>4.162</v>
+        <v>4.077</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2336,13 +2444,13 @@
         <v>96</v>
       </c>
       <c r="C47" s="2">
-        <v>3.399</v>
+        <v>3.008</v>
       </c>
       <c r="D47" s="2">
-        <v>121.059987453644</v>
+        <v>119.402521297103</v>
       </c>
       <c r="E47" s="2">
-        <v>4.633</v>
+        <v>2.477</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2353,13 +2461,13 @@
         <v>98</v>
       </c>
       <c r="C48" s="2">
-        <v>4.767</v>
+        <v>3.479</v>
       </c>
       <c r="D48" s="2">
-        <v>113.424318575162</v>
+        <v>117.308150756297</v>
       </c>
       <c r="E48" s="2">
-        <v>2.71</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2370,13 +2478,13 @@
         <v>100</v>
       </c>
       <c r="C49" s="2">
-        <v>3.349</v>
+        <v>4.8</v>
       </c>
       <c r="D49" s="2">
-        <v>121.242189370061</v>
+        <v>120.11869865252</v>
       </c>
       <c r="E49" s="2">
-        <v>4.416</v>
+        <v>4.97</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2387,13 +2495,13 @@
         <v>102</v>
       </c>
       <c r="C50" s="2">
-        <v>4.583</v>
+        <v>2.98</v>
       </c>
       <c r="D50" s="2">
-        <v>111.829249322239</v>
+        <v>122.500470220539</v>
       </c>
       <c r="E50" s="2">
-        <v>1.825</v>
+        <v>2.099</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2404,13 +2512,13 @@
         <v>104</v>
       </c>
       <c r="C51" s="2">
-        <v>2.698</v>
+        <v>4.997</v>
       </c>
       <c r="D51" s="2">
-        <v>120.551323142979</v>
+        <v>121.393042945248</v>
       </c>
       <c r="E51" s="2">
-        <v>1.964</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2421,13 +2529,13 @@
         <v>106</v>
       </c>
       <c r="C52" s="2">
-        <v>3.999</v>
+        <v>3.907</v>
       </c>
       <c r="D52" s="2">
-        <v>118.98656338779</v>
+        <v>122.188816379074</v>
       </c>
       <c r="E52" s="2">
-        <v>4.153</v>
+        <v>2.058</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2438,13 +2546,13 @@
         <v>108</v>
       </c>
       <c r="C53" s="2">
-        <v>2.393</v>
+        <v>3.87</v>
       </c>
       <c r="D53" s="2">
-        <v>119.090407006286</v>
+        <v>120.799455321798</v>
       </c>
       <c r="E53" s="2">
-        <v>2.384</v>
+        <v>3.726</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2455,13 +2563,13 @@
         <v>110</v>
       </c>
       <c r="C54" s="2">
-        <v>3.21</v>
+        <v>3.099</v>
       </c>
       <c r="D54" s="2">
-        <v>120.625625775985</v>
+        <v>121.594396863843</v>
       </c>
       <c r="E54" s="2">
-        <v>3.877</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2472,13 +2580,13 @@
         <v>112</v>
       </c>
       <c r="C55" s="2">
-        <v>2.496</v>
+        <v>3.796</v>
       </c>
       <c r="D55" s="2">
-        <v>122.390521060885</v>
+        <v>115.664900816223</v>
       </c>
       <c r="E55" s="2">
-        <v>2.227</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2489,13 +2597,13 @@
         <v>114</v>
       </c>
       <c r="C56" s="2">
-        <v>4.999</v>
+        <v>3.999</v>
       </c>
       <c r="D56" s="2">
-        <v>119.605208797665</v>
+        <v>118.541724099802</v>
       </c>
       <c r="E56" s="2">
-        <v>3.904</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2506,13 +2614,13 @@
         <v>116</v>
       </c>
       <c r="C57" s="2">
-        <v>4.899</v>
+        <v>3.349</v>
       </c>
       <c r="D57" s="2">
-        <v>120.431566235773</v>
+        <v>121.33347117543</v>
       </c>
       <c r="E57" s="2">
-        <v>4.57</v>
+        <v>4.266</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2523,13 +2631,13 @@
         <v>118</v>
       </c>
       <c r="C58" s="2">
-        <v>2.922</v>
+        <v>2.943</v>
       </c>
       <c r="D58" s="2">
-        <v>124.214032182871</v>
+        <v>119.274416220064</v>
       </c>
       <c r="E58" s="2">
-        <v>4.227</v>
+        <v>4.263</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2540,13 +2648,13 @@
         <v>120</v>
       </c>
       <c r="C59" s="2">
-        <v>2.422</v>
+        <v>4.595</v>
       </c>
       <c r="D59" s="2">
-        <v>121.12618028064</v>
+        <v>119.169040053409</v>
       </c>
       <c r="E59" s="2">
-        <v>4.671</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2557,13 +2665,13 @@
         <v>122</v>
       </c>
       <c r="C60" s="2">
-        <v>4.149</v>
+        <v>4.53</v>
       </c>
       <c r="D60" s="2">
-        <v>120.572053341242</v>
+        <v>111.847341047428</v>
       </c>
       <c r="E60" s="2">
-        <v>3.315</v>
+        <v>1.636</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2574,13 +2682,13 @@
         <v>124</v>
       </c>
       <c r="C61" s="2">
-        <v>4.593</v>
+        <v>2.216</v>
       </c>
       <c r="D61" s="2">
-        <v>121.036583846078</v>
+        <v>117.374969634351</v>
       </c>
       <c r="E61" s="2">
-        <v>1.866</v>
+        <v>1.507</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2591,13 +2699,13 @@
         <v>126</v>
       </c>
       <c r="C62" s="2">
-        <v>2.216</v>
+        <v>2.494</v>
       </c>
       <c r="D62" s="2">
-        <v>117.320710259955</v>
+        <v>122.47587083233</v>
       </c>
       <c r="E62" s="2">
-        <v>1.658</v>
+        <v>2.077</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2608,13 +2716,13 @@
         <v>128</v>
       </c>
       <c r="C63" s="2">
-        <v>2.98</v>
+        <v>2.422</v>
       </c>
       <c r="D63" s="2">
-        <v>122.348361350437</v>
+        <v>121.314394136283</v>
       </c>
       <c r="E63" s="2">
-        <v>2.249</v>
+        <v>4.521</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2625,13 +2733,13 @@
         <v>130</v>
       </c>
       <c r="C64" s="2">
-        <v>3.687</v>
+        <v>2.922</v>
       </c>
       <c r="D64" s="2">
-        <v>120.297295853433</v>
+        <v>124.40275126066</v>
       </c>
       <c r="E64" s="2">
-        <v>4.858</v>
+        <v>4.077</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2642,13 +2750,13 @@
         <v>132</v>
       </c>
       <c r="C65" s="2">
-        <v>3.755</v>
+        <v>2.594</v>
       </c>
       <c r="D65" s="2">
-        <v>116.356835768104</v>
+        <v>116.148307836001</v>
       </c>
       <c r="E65" s="2">
-        <v>3.534</v>
+        <v>2.063</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2659,13 +2767,13 @@
         <v>134</v>
       </c>
       <c r="C66" s="2">
-        <v>4.187</v>
+        <v>3.21</v>
       </c>
       <c r="D66" s="2">
-        <v>119.046366712229</v>
+        <v>120.713612195959</v>
       </c>
       <c r="E66" s="2">
-        <v>2.627</v>
+        <v>3.726</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2676,13 +2784,13 @@
         <v>136</v>
       </c>
       <c r="C67" s="2">
-        <v>3.977</v>
+        <v>3.399</v>
       </c>
       <c r="D67" s="2">
-        <v>117.354781441167</v>
+        <v>121.0490136712</v>
       </c>
       <c r="E67" s="2">
-        <v>4.553</v>
+        <v>4.482</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2696,10 +2804,10 @@
         <v>4.999</v>
       </c>
       <c r="D68" s="2">
-        <v>121.165981400618</v>
+        <v>121.352829670366</v>
       </c>
       <c r="E68" s="2">
-        <v>4.184</v>
+        <v>4.033</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2710,13 +2818,13 @@
         <v>140</v>
       </c>
       <c r="C69" s="2">
-        <v>2.987</v>
+        <v>4.816</v>
       </c>
       <c r="D69" s="2">
-        <v>111.805469836711</v>
+        <v>123.258966989728</v>
       </c>
       <c r="E69" s="2">
-        <v>1.877</v>
+        <v>3.586</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2727,13 +2835,13 @@
         <v>142</v>
       </c>
       <c r="C70" s="2">
-        <v>3.008</v>
+        <v>2.265</v>
       </c>
       <c r="D70" s="2">
-        <v>119.234599058808</v>
+        <v>122.420177519429</v>
       </c>
       <c r="E70" s="2">
-        <v>2.627</v>
+        <v>2.789</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2744,13 +2852,13 @@
         <v>144</v>
       </c>
       <c r="C71" s="2">
-        <v>2.037</v>
+        <v>3.977</v>
       </c>
       <c r="D71" s="2">
-        <v>120.010395813362</v>
+        <v>117.462637392892</v>
       </c>
       <c r="E71" s="2">
-        <v>3.855</v>
+        <v>4.403</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2761,13 +2869,13 @@
         <v>146</v>
       </c>
       <c r="C72" s="2">
-        <v>4.984</v>
+        <v>4.527</v>
       </c>
       <c r="D72" s="2">
-        <v>115.315073205921</v>
+        <v>120.836948146898</v>
       </c>
       <c r="E72" s="2">
-        <v>2.644</v>
+        <v>4.781</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2778,13 +2886,13 @@
         <v>148</v>
       </c>
       <c r="C73" s="2">
-        <v>4.53</v>
+        <v>2.395</v>
       </c>
       <c r="D73" s="2">
-        <v>111.788778492194</v>
+        <v>120.62105654979</v>
       </c>
       <c r="E73" s="2">
-        <v>1.786</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2795,13 +2903,13 @@
         <v>150</v>
       </c>
       <c r="C74" s="2">
-        <v>4.949</v>
+        <v>2.037</v>
       </c>
       <c r="D74" s="2">
-        <v>111.93494522822</v>
+        <v>120.092621225641</v>
       </c>
       <c r="E74" s="2">
-        <v>4.315</v>
+        <v>3.704</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2812,13 +2920,13 @@
         <v>152</v>
       </c>
       <c r="C75" s="2">
-        <v>2.945</v>
+        <v>4.499</v>
       </c>
       <c r="D75" s="2">
-        <v>113.762215828285</v>
+        <v>120.712168956756</v>
       </c>
       <c r="E75" s="2">
-        <v>1.652</v>
+        <v>4.452</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2829,140 +2937,320 @@
         <v>154</v>
       </c>
       <c r="C76" s="2">
-        <v>2.082</v>
+        <v>3.996</v>
       </c>
       <c r="D76" s="2">
-        <v>112.14092636828</v>
+        <v>121.147264878616</v>
       </c>
       <c r="E76" s="2">
-        <v>1.918</v>
+        <v>4.874</v>
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
+      <c r="A77" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="2">
+        <v>4.984</v>
+      </c>
+      <c r="D77" s="2">
+        <v>115.353470683005</v>
+      </c>
+      <c r="E77" s="2">
+        <v>2.493</v>
+      </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
+      <c r="A78" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1.941</v>
+      </c>
+      <c r="D78" s="2">
+        <v>116.894841211292</v>
+      </c>
+      <c r="E78" s="2">
+        <v>3.364</v>
+      </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
+      <c r="A79" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="2">
+        <v>3.911</v>
+      </c>
+      <c r="D79" s="2">
+        <v>121.022256243338</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1.715</v>
+      </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
+      <c r="A80" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" s="2">
+        <v>2.685</v>
+      </c>
+      <c r="D80" s="2">
+        <v>121.220176857578</v>
+      </c>
+      <c r="E80" s="2">
+        <v>4.534</v>
+      </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
+      <c r="A81" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="2">
+        <v>3.686</v>
+      </c>
+      <c r="D81" s="2">
+        <v>120.254492054178</v>
+      </c>
+      <c r="E81" s="2">
+        <v>4.707</v>
+      </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
+      <c r="A82" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" s="2">
+        <v>1.731</v>
+      </c>
+      <c r="D82" s="2">
+        <v>119.341438445334</v>
+      </c>
+      <c r="E82" s="2">
+        <v>2.543</v>
+      </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
+      <c r="A83" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="2">
+        <v>2.081</v>
+      </c>
+      <c r="D83" s="2">
+        <v>112.198127177337</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1.767</v>
+      </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
+      <c r="A84" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="2">
+        <v>3.838</v>
+      </c>
+      <c r="D84" s="2">
+        <v>118.98674840318</v>
+      </c>
+      <c r="E84" s="2">
+        <v>4.362</v>
+      </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
+      <c r="A85" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="2">
+        <v>4.949</v>
+      </c>
+      <c r="D85" s="2">
+        <v>111.977018618211</v>
+      </c>
+      <c r="E85" s="2">
+        <v>4.164</v>
+      </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
+      <c r="A86" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="2">
+        <v>4.499</v>
+      </c>
+      <c r="D86" s="2">
+        <v>116.796426809137</v>
+      </c>
+      <c r="E86" s="2">
+        <v>4.249</v>
+      </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
+      <c r="A87" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="2">
+        <v>3.745</v>
+      </c>
+      <c r="D87" s="2">
+        <v>120.493308889341</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1.806</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
+      <c r="A88" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="2">
+        <v>3.081</v>
+      </c>
+      <c r="D88" s="2">
+        <v>111.801435792332</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1.51</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
+      <c r="A89" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="2">
+        <v>2.945</v>
+      </c>
+      <c r="D89" s="2">
+        <v>113.784831738325</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1.501</v>
+      </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
+      <c r="A90" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C90" s="2">
+        <v>3.754</v>
+      </c>
+      <c r="D90" s="2">
+        <v>116.26195726766</v>
+      </c>
+      <c r="E90" s="2">
+        <v>3.384</v>
+      </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
+      <c r="A91" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="2">
+        <v>3.987</v>
+      </c>
+      <c r="D91" s="2">
+        <v>119.165121482338</v>
+      </c>
+      <c r="E91" s="2">
+        <v>2.501</v>
+      </c>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
+      <c r="A92" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" s="2">
+        <v>4.063</v>
+      </c>
+      <c r="D92" s="2">
+        <v>111.181583674691</v>
+      </c>
+      <c r="E92" s="2">
+        <v>2.534</v>
+      </c>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
+      <c r="A93" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2.877</v>
+      </c>
+      <c r="D93" s="2">
+        <v>111.183954320036</v>
+      </c>
+      <c r="E93" s="2">
+        <v>2.167</v>
+      </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
+      <c r="A94" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C94" s="2">
+        <v>3.79</v>
+      </c>
+      <c r="D94" s="2">
+        <v>109.731572214406</v>
+      </c>
+      <c r="E94" s="2">
+        <v>1.795</v>
+      </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="4"/>

</xml_diff>

<commit_message>
1.give options for select bond (allbond or optbond)
</commit_message>
<xml_diff>
--- a/selected.xlsx
+++ b/selected.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
   <si>
     <t>code</t>
   </si>
@@ -44,118 +44,328 @@
     <t>lastyear</t>
   </si>
   <si>
+    <t>sz123156</t>
+  </si>
+  <si>
+    <t>博汇转债</t>
+  </si>
+  <si>
+    <t>sz128138</t>
+  </si>
+  <si>
+    <t>侨银转债</t>
+  </si>
+  <si>
+    <t>sh118016</t>
+  </si>
+  <si>
+    <t>京源转债</t>
+  </si>
+  <si>
+    <t>sz123175</t>
+  </si>
+  <si>
+    <t>百畅转债</t>
+  </si>
+  <si>
+    <t>sh113608</t>
+  </si>
+  <si>
+    <t>威派转债</t>
+  </si>
+  <si>
+    <t>sh113610</t>
+  </si>
+  <si>
+    <t>灵康转债</t>
+  </si>
+  <si>
+    <t>sh113665</t>
+  </si>
+  <si>
+    <t>汇通转债</t>
+  </si>
+  <si>
+    <t>sz123171</t>
+  </si>
+  <si>
+    <t>共同转债</t>
+  </si>
+  <si>
+    <t>sz123155</t>
+  </si>
+  <si>
+    <t>中陆转债</t>
+  </si>
+  <si>
+    <t>sz127062</t>
+  </si>
+  <si>
+    <t>垒知转债</t>
+  </si>
+  <si>
+    <t>sh113649</t>
+  </si>
+  <si>
+    <t>丰山转债</t>
+  </si>
+  <si>
+    <t>sz123126</t>
+  </si>
+  <si>
+    <t>瑞丰转债</t>
+  </si>
+  <si>
+    <t>sz123157</t>
+  </si>
+  <si>
+    <t>科蓝转债</t>
+  </si>
+  <si>
+    <t>sz123189</t>
+  </si>
+  <si>
+    <t>晓鸣转债</t>
+  </si>
+  <si>
+    <t>sz123168</t>
+  </si>
+  <si>
+    <t>惠云转债</t>
+  </si>
+  <si>
+    <t>sh118007</t>
+  </si>
+  <si>
+    <t>山石转债</t>
+  </si>
+  <si>
+    <t>sh118040</t>
+  </si>
+  <si>
+    <t>宏微转债</t>
+  </si>
+  <si>
+    <t>sh118015</t>
+  </si>
+  <si>
+    <t>芯海转债</t>
+  </si>
+  <si>
+    <t>sh118018</t>
+  </si>
+  <si>
+    <t>瑞科转债</t>
+  </si>
+  <si>
+    <t>sh118029</t>
+  </si>
+  <si>
+    <t>富淼转债</t>
+  </si>
+  <si>
+    <t>sz123196</t>
+  </si>
+  <si>
+    <t>正元转02</t>
+  </si>
+  <si>
+    <t>sz123163</t>
+  </si>
+  <si>
+    <t>金沃转债</t>
+  </si>
+  <si>
+    <t>sz123200</t>
+  </si>
+  <si>
+    <t>海泰转债</t>
+  </si>
+  <si>
+    <t>sz123082</t>
+  </si>
+  <si>
+    <t>北陆转债</t>
+  </si>
+  <si>
+    <t>sz123166</t>
+  </si>
+  <si>
+    <t>蒙泰转债</t>
+  </si>
+  <si>
+    <t>sh113628</t>
+  </si>
+  <si>
+    <t>晨丰转债</t>
+  </si>
+  <si>
+    <t>sz127059</t>
+  </si>
+  <si>
+    <t>永东转2</t>
+  </si>
+  <si>
     <t>sh113600</t>
   </si>
   <si>
     <t>新星转债</t>
   </si>
   <si>
-    <t>sz123156</t>
-  </si>
-  <si>
-    <t>博汇转债</t>
-  </si>
-  <si>
-    <t>sh118016</t>
-  </si>
-  <si>
-    <t>京源转债</t>
-  </si>
-  <si>
-    <t>sh113665</t>
-  </si>
-  <si>
-    <t>汇通转债</t>
-  </si>
-  <si>
-    <t>sz123175</t>
-  </si>
-  <si>
-    <t>百畅转债</t>
-  </si>
-  <si>
-    <t>sz128138</t>
-  </si>
-  <si>
-    <t>侨银转债</t>
-  </si>
-  <si>
-    <t>sh113610</t>
-  </si>
-  <si>
-    <t>灵康转债</t>
-  </si>
-  <si>
-    <t>sz123155</t>
-  </si>
-  <si>
-    <t>中陆转债</t>
-  </si>
-  <si>
-    <t>sh113608</t>
-  </si>
-  <si>
-    <t>威派转债</t>
-  </si>
-  <si>
-    <t>sh118018</t>
-  </si>
-  <si>
-    <t>瑞科转债</t>
-  </si>
-  <si>
-    <t>sz123157</t>
-  </si>
-  <si>
-    <t>科蓝转债</t>
-  </si>
-  <si>
-    <t>sz123171</t>
-  </si>
-  <si>
-    <t>共同转债</t>
-  </si>
-  <si>
-    <t>sh118007</t>
-  </si>
-  <si>
-    <t>山石转债</t>
-  </si>
-  <si>
-    <t>sz123126</t>
-  </si>
-  <si>
-    <t>瑞丰转债</t>
-  </si>
-  <si>
-    <t>sz123166</t>
-  </si>
-  <si>
-    <t>蒙泰转债</t>
-  </si>
-  <si>
-    <t>sz123082</t>
-  </si>
-  <si>
-    <t>北陆转债</t>
-  </si>
-  <si>
-    <t>sz123189</t>
-  </si>
-  <si>
-    <t>晓鸣转债</t>
-  </si>
-  <si>
-    <t>sh118040</t>
-  </si>
-  <si>
-    <t>XD宏微转</t>
-  </si>
-  <si>
-    <t>sz123196</t>
-  </si>
-  <si>
-    <t>正元转02</t>
+    <t>sh113643</t>
+  </si>
+  <si>
+    <t>风语转债</t>
+  </si>
+  <si>
+    <t>sz123180</t>
+  </si>
+  <si>
+    <t>浙矿转债</t>
+  </si>
+  <si>
+    <t>sz123160</t>
+  </si>
+  <si>
+    <t>泰福转债</t>
+  </si>
+  <si>
+    <t>sh118012</t>
+  </si>
+  <si>
+    <t>微芯转债</t>
+  </si>
+  <si>
+    <t>sh118014</t>
+  </si>
+  <si>
+    <t>高测转债</t>
+  </si>
+  <si>
+    <t>sz127053</t>
+  </si>
+  <si>
+    <t>豪美转债</t>
+  </si>
+  <si>
+    <t>sh113593</t>
+  </si>
+  <si>
+    <t>沪工转债</t>
+  </si>
+  <si>
+    <t>sz123220</t>
+  </si>
+  <si>
+    <t>易瑞转债</t>
+  </si>
+  <si>
+    <t>sh118035</t>
+  </si>
+  <si>
+    <t>国力转债</t>
+  </si>
+  <si>
+    <t>sz128117</t>
+  </si>
+  <si>
+    <t>道恩转债</t>
+  </si>
+  <si>
+    <t>sh113624</t>
+  </si>
+  <si>
+    <t>正川转债</t>
+  </si>
+  <si>
+    <t>sh118009</t>
+  </si>
+  <si>
+    <t>华锐转债</t>
+  </si>
+  <si>
+    <t>sh118011</t>
+  </si>
+  <si>
+    <t>银微转债</t>
+  </si>
+  <si>
+    <t>sz123141</t>
+  </si>
+  <si>
+    <t>宏丰转债</t>
+  </si>
+  <si>
+    <t>sz123185</t>
+  </si>
+  <si>
+    <t>能辉转债</t>
+  </si>
+  <si>
+    <t>sh113618</t>
+  </si>
+  <si>
+    <t>美诺转债</t>
+  </si>
+  <si>
+    <t>sz128120</t>
+  </si>
+  <si>
+    <t>联诚转债</t>
+  </si>
+  <si>
+    <t>sz123207</t>
+  </si>
+  <si>
+    <t>冠中转债</t>
+  </si>
+  <si>
+    <t>sz123214</t>
+  </si>
+  <si>
+    <t>东宝转债</t>
+  </si>
+  <si>
+    <t>sz123109</t>
+  </si>
+  <si>
+    <t>昌红转债</t>
+  </si>
+  <si>
+    <t>sh118010</t>
+  </si>
+  <si>
+    <t>洁特转债</t>
+  </si>
+  <si>
+    <t>sh118006</t>
+  </si>
+  <si>
+    <t>阿拉转债</t>
+  </si>
+  <si>
+    <t>sz123088</t>
+  </si>
+  <si>
+    <t>威唐转债</t>
+  </si>
+  <si>
+    <t>sz123093</t>
+  </si>
+  <si>
+    <t>金陵转债</t>
+  </si>
+  <si>
+    <t>sh118036</t>
+  </si>
+  <si>
+    <t>力合转债</t>
+  </si>
+  <si>
+    <t>sh113597</t>
+  </si>
+  <si>
+    <t>佳力转债</t>
   </si>
   <si>
     <t>sh110070</t>
@@ -164,40 +374,40 @@
     <t>凌钢转债</t>
   </si>
   <si>
-    <t>sh113628</t>
-  </si>
-  <si>
-    <t>晨丰转债</t>
-  </si>
-  <si>
-    <t>sh113649</t>
-  </si>
-  <si>
-    <t>丰山转债</t>
-  </si>
-  <si>
-    <t>sz123168</t>
-  </si>
-  <si>
-    <t>惠云转债</t>
-  </si>
-  <si>
-    <t>sh113624</t>
-  </si>
-  <si>
-    <t>正川转债</t>
-  </si>
-  <si>
-    <t>sh118015</t>
-  </si>
-  <si>
-    <t>芯海转债</t>
-  </si>
-  <si>
-    <t>sh113565</t>
-  </si>
-  <si>
-    <t>宏辉转债</t>
+    <t>sz123065</t>
+  </si>
+  <si>
+    <t>宝莱转债</t>
+  </si>
+  <si>
+    <t>sz123201</t>
+  </si>
+  <si>
+    <t>纽泰转债</t>
+  </si>
+  <si>
+    <t>sz123159</t>
+  </si>
+  <si>
+    <t>崧盛转债</t>
+  </si>
+  <si>
+    <t>sz123218</t>
+  </si>
+  <si>
+    <t>宏昌转债</t>
+  </si>
+  <si>
+    <t>sh118039</t>
+  </si>
+  <si>
+    <t>煜邦转债</t>
+  </si>
+  <si>
+    <t>sz123092</t>
+  </si>
+  <si>
+    <t>天壕转债</t>
   </si>
   <si>
     <t>sz128125</t>
@@ -206,76 +416,22 @@
     <t>华阳转债</t>
   </si>
   <si>
-    <t>sh118029</t>
-  </si>
-  <si>
-    <t>富淼转债</t>
-  </si>
-  <si>
-    <t>sz128117</t>
-  </si>
-  <si>
-    <t>道恩转债</t>
-  </si>
-  <si>
-    <t>sz123207</t>
-  </si>
-  <si>
-    <t>冠中转债</t>
-  </si>
-  <si>
-    <t>sz128101</t>
-  </si>
-  <si>
-    <t>联创转债</t>
-  </si>
-  <si>
-    <t>sh113618</t>
-  </si>
-  <si>
-    <t>美诺转债</t>
-  </si>
-  <si>
-    <t>sz123160</t>
-  </si>
-  <si>
-    <t>泰福转债</t>
-  </si>
-  <si>
-    <t>sz123163</t>
-  </si>
-  <si>
-    <t>金沃转债</t>
-  </si>
-  <si>
-    <t>sh118039</t>
-  </si>
-  <si>
-    <t>煜邦转债</t>
-  </si>
-  <si>
-    <t>sh118010</t>
-  </si>
-  <si>
-    <t>洁特转债</t>
-  </si>
-  <si>
-    <t>sz127059</t>
-  </si>
-  <si>
-    <t>永东转2</t>
-  </si>
-  <si>
-    <t>sz123200</t>
-  </si>
-  <si>
-    <t>海泰转债</t>
-  </si>
-  <si>
-    <t>sz123141</t>
-  </si>
-  <si>
-    <t>宏丰转债</t>
+    <t>sz123061</t>
+  </si>
+  <si>
+    <t>航新转债</t>
+  </si>
+  <si>
+    <t>sz123197</t>
+  </si>
+  <si>
+    <t>光力转债</t>
+  </si>
+  <si>
+    <t>sz123130</t>
+  </si>
+  <si>
+    <t>设研转债</t>
   </si>
   <si>
     <t>sz123100</t>
@@ -284,172 +440,148 @@
     <t>朗科转债</t>
   </si>
   <si>
+    <t>sz123152</t>
+  </si>
+  <si>
+    <t>润禾转债</t>
+  </si>
+  <si>
+    <t>sh113660</t>
+  </si>
+  <si>
+    <t>寿22转债</t>
+  </si>
+  <si>
+    <t>sh118044</t>
+  </si>
+  <si>
+    <t>赛特转债</t>
+  </si>
+  <si>
+    <t>sz123187</t>
+  </si>
+  <si>
+    <t>超达转债</t>
+  </si>
+  <si>
+    <t>sz123067</t>
+  </si>
+  <si>
+    <t>斯莱转债</t>
+  </si>
+  <si>
+    <t>sz127079</t>
+  </si>
+  <si>
+    <t>华亚转债</t>
+  </si>
+  <si>
+    <t>sz123173</t>
+  </si>
+  <si>
+    <t>恒锋转债</t>
+  </si>
+  <si>
+    <t>sz123202</t>
+  </si>
+  <si>
+    <t>祥源转债</t>
+  </si>
+  <si>
+    <t>sz123138</t>
+  </si>
+  <si>
+    <t>丝路转债</t>
+  </si>
+  <si>
+    <t>sh113671</t>
+  </si>
+  <si>
+    <t>武进转债</t>
+  </si>
+  <si>
+    <t>sz123112</t>
+  </si>
+  <si>
+    <t>万讯转债</t>
+  </si>
+  <si>
+    <t>sz123087</t>
+  </si>
+  <si>
+    <t>明电转债</t>
+  </si>
+  <si>
+    <t>sz127090</t>
+  </si>
+  <si>
+    <t>兴瑞转债</t>
+  </si>
+  <si>
+    <t>sh118004</t>
+  </si>
+  <si>
+    <t>博瑞转债</t>
+  </si>
+  <si>
+    <t>sz127087</t>
+  </si>
+  <si>
+    <t>星帅转2</t>
+  </si>
+  <si>
+    <t>sh111013</t>
+  </si>
+  <si>
+    <t>新港转债</t>
+  </si>
+  <si>
+    <t>sh111003</t>
+  </si>
+  <si>
+    <t>聚合转债</t>
+  </si>
+  <si>
+    <t>sz123129</t>
+  </si>
+  <si>
+    <t>锦鸡转债</t>
+  </si>
+  <si>
+    <t>sh111012</t>
+  </si>
+  <si>
+    <t>福新转债</t>
+  </si>
+  <si>
+    <t>sz123059</t>
+  </si>
+  <si>
+    <t>银信转债</t>
+  </si>
+  <si>
+    <t>sh118045</t>
+  </si>
+  <si>
+    <t>盟升转债</t>
+  </si>
+  <si>
+    <t>sz123089</t>
+  </si>
+  <si>
+    <t>九洲转2</t>
+  </si>
+  <si>
     <t>sz123103</t>
   </si>
   <si>
     <t>震安转债</t>
   </si>
   <si>
-    <t>sz123180</t>
-  </si>
-  <si>
-    <t>浙矿转债</t>
-  </si>
-  <si>
-    <t>sh113643</t>
-  </si>
-  <si>
-    <t>风语转债</t>
-  </si>
-  <si>
-    <t>sz123088</t>
-  </si>
-  <si>
-    <t>威唐转债</t>
-  </si>
-  <si>
-    <t>sh118014</t>
-  </si>
-  <si>
-    <t>高测转债</t>
-  </si>
-  <si>
-    <t>sh113593</t>
-  </si>
-  <si>
-    <t>沪工转债</t>
-  </si>
-  <si>
-    <t>sh118009</t>
-  </si>
-  <si>
-    <t>华锐转债</t>
-  </si>
-  <si>
-    <t>sz123093</t>
-  </si>
-  <si>
-    <t>金陵转债</t>
-  </si>
-  <si>
-    <t>sz128097</t>
-  </si>
-  <si>
-    <t>奥佳转债</t>
-  </si>
-  <si>
-    <t>sz127062</t>
-  </si>
-  <si>
-    <t>垒知转债</t>
-  </si>
-  <si>
-    <t>sz123067</t>
-  </si>
-  <si>
-    <t>斯莱转债</t>
-  </si>
-  <si>
-    <t>sh118011</t>
-  </si>
-  <si>
-    <t>银微转债</t>
-  </si>
-  <si>
-    <t>sz123159</t>
-  </si>
-  <si>
-    <t>崧盛转债</t>
-  </si>
-  <si>
-    <t>sh118035</t>
-  </si>
-  <si>
-    <t>国力转债</t>
-  </si>
-  <si>
-    <t>sz123061</t>
-  </si>
-  <si>
-    <t>航新转债</t>
-  </si>
-  <si>
-    <t>sz123059</t>
-  </si>
-  <si>
-    <t>银信转债</t>
-  </si>
-  <si>
-    <t>sz123109</t>
-  </si>
-  <si>
-    <t>昌红转债</t>
-  </si>
-  <si>
-    <t>sz127079</t>
-  </si>
-  <si>
-    <t>华亚转债</t>
-  </si>
-  <si>
-    <t>sh113597</t>
-  </si>
-  <si>
-    <t>佳力转债</t>
-  </si>
-  <si>
-    <t>sz123202</t>
-  </si>
-  <si>
-    <t>祥源转债</t>
-  </si>
-  <si>
-    <t>sz123185</t>
-  </si>
-  <si>
-    <t>能辉转债</t>
-  </si>
-  <si>
-    <t>sz128095</t>
-  </si>
-  <si>
-    <t>恩捷转债</t>
-  </si>
-  <si>
-    <t>sh118006</t>
-  </si>
-  <si>
-    <t>阿拉转债</t>
-  </si>
-  <si>
-    <t>sh118012</t>
-  </si>
-  <si>
-    <t>微芯转债</t>
-  </si>
-  <si>
-    <t>sz127053</t>
-  </si>
-  <si>
-    <t>豪美转债</t>
-  </si>
-  <si>
-    <t>sz128120</t>
-  </si>
-  <si>
-    <t>联诚转债</t>
-  </si>
-  <si>
-    <t>sz123197</t>
-  </si>
-  <si>
-    <t>光力转债</t>
-  </si>
-  <si>
-    <t>sz123065</t>
-  </si>
-  <si>
-    <t>宝莱转债</t>
+    <t>sh113674</t>
+  </si>
+  <si>
+    <t>华设转债</t>
   </si>
   <si>
     <t>sh111008</t>
@@ -458,82 +590,58 @@
     <t>沿浦转债</t>
   </si>
   <si>
-    <t>sz123152</t>
-  </si>
-  <si>
-    <t>润禾转债</t>
-  </si>
-  <si>
-    <t>sh118036</t>
-  </si>
-  <si>
-    <t>力合转债</t>
-  </si>
-  <si>
-    <t>sz123044</t>
-  </si>
-  <si>
-    <t>红相转债</t>
-  </si>
-  <si>
-    <t>sh113660</t>
-  </si>
-  <si>
-    <t>寿22转债</t>
-  </si>
-  <si>
-    <t>sz123112</t>
-  </si>
-  <si>
-    <t>万讯转债</t>
-  </si>
-  <si>
-    <t>sh111003</t>
-  </si>
-  <si>
-    <t>聚合转债</t>
-  </si>
-  <si>
-    <t>sz123138</t>
-  </si>
-  <si>
-    <t>丝路转债</t>
-  </si>
-  <si>
-    <t>sz123173</t>
-  </si>
-  <si>
-    <t>恒锋转债</t>
-  </si>
-  <si>
-    <t>sz123089</t>
-  </si>
-  <si>
-    <t>九洲转2</t>
-  </si>
-  <si>
-    <t>sh113598</t>
-  </si>
-  <si>
-    <t>法兰转债</t>
-  </si>
-  <si>
-    <t>sz127090</t>
-  </si>
-  <si>
-    <t>兴瑞转债</t>
-  </si>
-  <si>
-    <t>sz123129</t>
-  </si>
-  <si>
-    <t>锦鸡转债</t>
-  </si>
-  <si>
-    <t>sh111013</t>
-  </si>
-  <si>
-    <t>新港转债</t>
+    <t>sh113664</t>
+  </si>
+  <si>
+    <t>大元转债</t>
+  </si>
+  <si>
+    <t>sh113039</t>
+  </si>
+  <si>
+    <t>嘉泽转债</t>
+  </si>
+  <si>
+    <t>sz123203</t>
+  </si>
+  <si>
+    <t>明电转02</t>
+  </si>
+  <si>
+    <t>sz127081</t>
+  </si>
+  <si>
+    <t>中旗转债</t>
+  </si>
+  <si>
+    <t>sz127072</t>
+  </si>
+  <si>
+    <t>博实转债</t>
+  </si>
+  <si>
+    <t>sz123090</t>
+  </si>
+  <si>
+    <t>三诺转债</t>
+  </si>
+  <si>
+    <t>sz123199</t>
+  </si>
+  <si>
+    <t>山河转债</t>
+  </si>
+  <si>
+    <t>sz123206</t>
+  </si>
+  <si>
+    <t>开能转债</t>
+  </si>
+  <si>
+    <t>sh113573</t>
+  </si>
+  <si>
+    <t>纵横转债</t>
   </si>
   <si>
     <t>sz123050</t>
@@ -542,16 +650,70 @@
     <t>聚飞转债</t>
   </si>
   <si>
-    <t>sz123206</t>
-  </si>
-  <si>
-    <t>开能转债</t>
-  </si>
-  <si>
-    <t>sz127072</t>
-  </si>
-  <si>
-    <t>博实转债</t>
+    <t>sz123221</t>
+  </si>
+  <si>
+    <t>力诺转债</t>
+  </si>
+  <si>
+    <t>sz128143</t>
+  </si>
+  <si>
+    <t>锋龙转债</t>
+  </si>
+  <si>
+    <t>sz127071</t>
+  </si>
+  <si>
+    <t>天箭转债</t>
+  </si>
+  <si>
+    <t>sh113662</t>
+  </si>
+  <si>
+    <t>豪能转债</t>
+  </si>
+  <si>
+    <t>sz123177</t>
+  </si>
+  <si>
+    <t>测绘转债</t>
+  </si>
+  <si>
+    <t>sh111011</t>
+  </si>
+  <si>
+    <t>冠盛转债</t>
+  </si>
+  <si>
+    <t>sz123209</t>
+  </si>
+  <si>
+    <t>聚隆转债</t>
+  </si>
+  <si>
+    <t>sz127080</t>
+  </si>
+  <si>
+    <t>声迅转债</t>
+  </si>
+  <si>
+    <t>sh118021</t>
+  </si>
+  <si>
+    <t>新致转债</t>
+  </si>
+  <si>
+    <t>sz123222</t>
+  </si>
+  <si>
+    <t>博俊转债</t>
+  </si>
+  <si>
+    <t>sz127028</t>
+  </si>
+  <si>
+    <t>英特转债</t>
   </si>
   <si>
     <t>sz128118</t>
@@ -560,154 +722,28 @@
     <t>瀛通转债</t>
   </si>
   <si>
-    <t>sz127087</t>
-  </si>
-  <si>
-    <t>星帅转2</t>
-  </si>
-  <si>
-    <t>sz123130</t>
-  </si>
-  <si>
-    <t>设研转债</t>
-  </si>
-  <si>
-    <t>sh111012</t>
-  </si>
-  <si>
-    <t>福新转债</t>
-  </si>
-  <si>
-    <t>sz128143</t>
-  </si>
-  <si>
-    <t>锋龙转债</t>
-  </si>
-  <si>
-    <t>sh113664</t>
-  </si>
-  <si>
-    <t>大元转债</t>
-  </si>
-  <si>
-    <t>sh113662</t>
-  </si>
-  <si>
-    <t>豪能转债</t>
-  </si>
-  <si>
-    <t>sz123177</t>
-  </si>
-  <si>
-    <t>测绘转债</t>
-  </si>
-  <si>
-    <t>sz123187</t>
-  </si>
-  <si>
-    <t>超达转债</t>
-  </si>
-  <si>
-    <t>sz123203</t>
-  </si>
-  <si>
-    <t>明电转02</t>
-  </si>
-  <si>
-    <t>sz123199</t>
-  </si>
-  <si>
-    <t>山河转债</t>
-  </si>
-  <si>
-    <t>sh113671</t>
-  </si>
-  <si>
-    <t>武进转债</t>
-  </si>
-  <si>
-    <t>sz123201</t>
-  </si>
-  <si>
-    <t>纽泰转债</t>
-  </si>
-  <si>
-    <t>sz127071</t>
-  </si>
-  <si>
-    <t>天箭转债</t>
-  </si>
-  <si>
-    <t>sh118004</t>
-  </si>
-  <si>
-    <t>博瑞转债</t>
-  </si>
-  <si>
-    <t>sh113573</t>
-  </si>
-  <si>
-    <t>纵横转债</t>
-  </si>
-  <si>
-    <t>sz123087</t>
-  </si>
-  <si>
-    <t>明电转债</t>
-  </si>
-  <si>
-    <t>sz123090</t>
-  </si>
-  <si>
-    <t>三诺转债</t>
-  </si>
-  <si>
-    <t>sz123092</t>
-  </si>
-  <si>
-    <t>天壕转债</t>
-  </si>
-  <si>
-    <t>sh111011</t>
-  </si>
-  <si>
-    <t>冠盛转债</t>
-  </si>
-  <si>
-    <t>sh113674</t>
-  </si>
-  <si>
-    <t>华设转债</t>
+    <t>sh113582</t>
+  </si>
+  <si>
+    <t>火炬转债</t>
+  </si>
+  <si>
+    <t>sh113577</t>
+  </si>
+  <si>
+    <t>春秋转债</t>
+  </si>
+  <si>
+    <t>sh113574</t>
+  </si>
+  <si>
+    <t>华体转债</t>
   </si>
   <si>
     <t>sz123048</t>
   </si>
   <si>
     <t>应急转债</t>
-  </si>
-  <si>
-    <t>sh113039</t>
-  </si>
-  <si>
-    <t>嘉泽转债</t>
-  </si>
-  <si>
-    <t>sh113574</t>
-  </si>
-  <si>
-    <t>华体转债</t>
-  </si>
-  <si>
-    <t>sz127028</t>
-  </si>
-  <si>
-    <t>英特转债</t>
-  </si>
-  <si>
-    <t>sh113577</t>
-  </si>
-  <si>
-    <t>春秋转债</t>
   </si>
   <si>
     <t>sh113588</t>
@@ -1713,8 +1749,8 @@
   <sheetPr/>
   <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E113"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1755,13 +1791,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>4.529</v>
+        <v>3.967</v>
       </c>
       <c r="D2" s="2">
-        <v>125.120392366036</v>
+        <v>121.645992940336</v>
       </c>
       <c r="E2" s="2">
-        <v>2.052</v>
+        <v>3.912</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -1773,13 +1809,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>3.967</v>
+        <v>4.199</v>
       </c>
       <c r="D3" s="2">
-        <v>122.834884929795</v>
+        <v>135.327419786399</v>
       </c>
       <c r="E3" s="2">
-        <v>4.063</v>
+        <v>2.164</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -1794,10 +1830,10 @@
         <v>3.325</v>
       </c>
       <c r="D4" s="2">
-        <v>122.935423765177</v>
+        <v>121.757611783817</v>
       </c>
       <c r="E4" s="2">
-        <v>4.033</v>
+        <v>3.882</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -1809,13 +1845,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>3.599</v>
+        <v>4.2</v>
       </c>
       <c r="D5" s="2">
-        <v>121.1871999645</v>
+        <v>119.101928896841</v>
       </c>
       <c r="E5" s="2">
-        <v>4.395</v>
+        <v>4.433</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -1830,10 +1866,10 @@
         <v>4.2</v>
       </c>
       <c r="D6" s="2">
-        <v>119.055449781856</v>
+        <v>119.764752346285</v>
       </c>
       <c r="E6" s="2">
-        <v>4.584</v>
+        <v>2.143</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -1845,13 +1881,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>4.199</v>
+        <v>2.53</v>
       </c>
       <c r="D7" s="2">
-        <v>135.149909353297</v>
+        <v>119.507521245164</v>
       </c>
       <c r="E7" s="2">
-        <v>2.315</v>
+        <v>2.203</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -1863,13 +1899,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>2.53</v>
+        <v>3.599</v>
       </c>
       <c r="D8" s="2">
-        <v>119.548912451216</v>
+        <v>120.950728545103</v>
       </c>
       <c r="E8" s="2">
-        <v>2.353</v>
+        <v>4.244</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -1881,13 +1917,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>3.6</v>
+        <v>3.799</v>
       </c>
       <c r="D9" s="2">
-        <v>122.318518254244</v>
+        <v>122.095680355139</v>
       </c>
       <c r="E9" s="2">
-        <v>4.052</v>
+        <v>4.197</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -1899,13 +1935,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="D10" s="2">
-        <v>119.728953565724</v>
+        <v>121.379067667326</v>
       </c>
       <c r="E10" s="2">
-        <v>2.293</v>
+        <v>3.901</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -1917,13 +1953,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>4.3</v>
+        <v>3.959</v>
       </c>
       <c r="D11" s="2">
-        <v>115.065868101577</v>
+        <v>120.204129246416</v>
       </c>
       <c r="E11" s="2">
-        <v>4.069</v>
+        <v>3.592</v>
       </c>
       <c r="I11" s="3"/>
     </row>
@@ -1935,13 +1971,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>4.945</v>
+        <v>4.591</v>
       </c>
       <c r="D12" s="2">
-        <v>120.836708973986</v>
+        <v>120.207659280069</v>
       </c>
       <c r="E12" s="2">
-        <v>4.101</v>
+        <v>3.775</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1953,13 +1989,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>3.799</v>
+        <v>3.399</v>
       </c>
       <c r="D13" s="2">
-        <v>122.051591879413</v>
+        <v>127.3250548441</v>
       </c>
       <c r="E13" s="2">
-        <v>4.348</v>
+        <v>2.978</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -1971,13 +2007,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="2">
-        <v>2.672</v>
+        <v>4.945</v>
       </c>
       <c r="D14" s="2">
-        <v>120.323334974573</v>
+        <v>120.27011574861</v>
       </c>
       <c r="E14" s="2">
-        <v>3.66</v>
+        <v>3.951</v>
       </c>
       <c r="I14" s="3"/>
     </row>
@@ -1989,13 +2025,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="2">
-        <v>3.399</v>
+        <v>3.29</v>
       </c>
       <c r="D15" s="2">
-        <v>129.494669638849</v>
+        <v>119.895100521348</v>
       </c>
       <c r="E15" s="2">
-        <v>3.129</v>
+        <v>4.551</v>
       </c>
       <c r="I15" s="3"/>
     </row>
@@ -2007,13 +2043,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>2.999</v>
+        <v>4.899</v>
       </c>
       <c r="D16" s="2">
-        <v>122.097294021327</v>
+        <v>121.192847705911</v>
       </c>
       <c r="E16" s="2">
-        <v>4.277</v>
+        <v>4.184</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -2025,13 +2061,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="2">
-        <v>4.993</v>
+        <v>2.672</v>
       </c>
       <c r="D17" s="2">
-        <v>119.749230762007</v>
+        <v>120.321154604544</v>
       </c>
       <c r="E17" s="2">
-        <v>2.37</v>
+        <v>3.51</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -2043,13 +2079,13 @@
         <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>3.29</v>
+        <v>4.3</v>
       </c>
       <c r="D18" s="2">
-        <v>119.771456338761</v>
+        <v>121.977679136096</v>
       </c>
       <c r="E18" s="2">
-        <v>4.701</v>
+        <v>4.852</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -2061,13 +2097,13 @@
         <v>40</v>
       </c>
       <c r="C19" s="2">
-        <v>4.3</v>
+        <v>4.1</v>
       </c>
       <c r="D19" s="2">
-        <v>121.8394367178</v>
+        <v>121.148780746945</v>
       </c>
       <c r="E19" s="2">
-        <v>5</v>
+        <v>3.841</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -2079,13 +2115,13 @@
         <v>42</v>
       </c>
       <c r="C20" s="2">
-        <v>3.507</v>
+        <v>4.3</v>
       </c>
       <c r="D20" s="2">
-        <v>119.917963365958</v>
+        <v>114.430820200204</v>
       </c>
       <c r="E20" s="2">
-        <v>4.734</v>
+        <v>3.918</v>
       </c>
       <c r="I20" s="3"/>
     </row>
@@ -2097,13 +2133,13 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>2.17</v>
+        <v>4.5</v>
       </c>
       <c r="D21" s="2">
-        <v>114.135946458522</v>
+        <v>114.963672193515</v>
       </c>
       <c r="E21" s="2">
-        <v>1.718</v>
+        <v>4.244</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -2115,13 +2151,13 @@
         <v>46</v>
       </c>
       <c r="C22" s="2">
-        <v>4.149</v>
+        <v>3.507</v>
       </c>
       <c r="D22" s="2">
-        <v>121.12454630176</v>
+        <v>119.928993481049</v>
       </c>
       <c r="E22" s="2">
-        <v>3.08</v>
+        <v>4.584</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -2133,13 +2169,13 @@
         <v>48</v>
       </c>
       <c r="C23" s="2">
-        <v>4.591</v>
+        <v>3.099</v>
       </c>
       <c r="D23" s="2">
-        <v>120.044201053491</v>
+        <v>122.141319859624</v>
       </c>
       <c r="E23" s="2">
-        <v>3.926</v>
+        <v>4.074</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -2151,13 +2187,13 @@
         <v>50</v>
       </c>
       <c r="C24" s="2">
-        <v>4.899</v>
+        <v>3.701</v>
       </c>
       <c r="D24" s="2">
-        <v>121.038086984881</v>
+        <v>124.903441773054</v>
       </c>
       <c r="E24" s="2">
-        <v>4.334</v>
+        <v>4.775</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -2169,13 +2205,13 @@
         <v>52</v>
       </c>
       <c r="C25" s="2">
-        <v>4.049</v>
+        <v>4.993</v>
       </c>
       <c r="D25" s="2">
-        <v>119.611430967615</v>
+        <v>119.721845433189</v>
       </c>
       <c r="E25" s="2">
-        <v>2.759</v>
+        <v>2.219</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -2187,13 +2223,13 @@
         <v>54</v>
       </c>
       <c r="C26" s="2">
-        <v>4.1</v>
+        <v>2.999</v>
       </c>
       <c r="D26" s="2">
-        <v>121.03043206305</v>
+        <v>121.977388029218</v>
       </c>
       <c r="E26" s="2">
-        <v>3.992</v>
+        <v>4.126</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2205,13 +2241,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2">
-        <v>2.247</v>
+        <v>4.149</v>
       </c>
       <c r="D27" s="2">
-        <v>114.678310091921</v>
+        <v>119.947562512896</v>
       </c>
       <c r="E27" s="2">
-        <v>1.592</v>
+        <v>2.929</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2223,13 +2259,13 @@
         <v>58</v>
       </c>
       <c r="C28" s="2">
-        <v>4.497</v>
+        <v>3.792</v>
       </c>
       <c r="D28" s="2">
-        <v>116.823585301732</v>
+        <v>120.098735316757</v>
       </c>
       <c r="E28" s="2">
-        <v>2.014</v>
+        <v>3.556</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2241,13 +2277,13 @@
         <v>60</v>
       </c>
       <c r="C29" s="2">
-        <v>4.5</v>
+        <v>3.87</v>
       </c>
       <c r="D29" s="2">
-        <v>114.813624076948</v>
+        <v>122.695485137155</v>
       </c>
       <c r="E29" s="2">
-        <v>4.395</v>
+        <v>1.901</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2259,13 +2295,13 @@
         <v>62</v>
       </c>
       <c r="C30" s="2">
-        <v>3.582</v>
+        <v>4.999</v>
       </c>
       <c r="D30" s="2">
-        <v>120.133446429684</v>
+        <v>120.071721507572</v>
       </c>
       <c r="E30" s="2">
-        <v>1.937</v>
+        <v>3.518</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2277,13 +2313,13 @@
         <v>64</v>
       </c>
       <c r="C31" s="2">
-        <v>3.998</v>
+        <v>3.199</v>
       </c>
       <c r="D31" s="2">
-        <v>121.396489871612</v>
+        <v>120.575553032139</v>
       </c>
       <c r="E31" s="2">
-        <v>4.992</v>
+        <v>4.474</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2295,13 +2331,13 @@
         <v>66</v>
       </c>
       <c r="C32" s="2">
-        <v>2.987</v>
+        <v>3.349</v>
       </c>
       <c r="D32" s="2">
-        <v>111.909144227555</v>
+        <v>121.839549389525</v>
       </c>
       <c r="E32" s="2">
-        <v>1.641</v>
+        <v>4.03</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -2313,13 +2349,13 @@
         <v>68</v>
       </c>
       <c r="C33" s="2">
-        <v>4.766</v>
+        <v>4.999</v>
       </c>
       <c r="D33" s="2">
-        <v>113.586294575664</v>
+        <v>121.161914449629</v>
       </c>
       <c r="E33" s="2">
-        <v>2.474</v>
+        <v>3.797</v>
       </c>
       <c r="I33" s="3"/>
     </row>
@@ -2331,13 +2367,13 @@
         <v>70</v>
       </c>
       <c r="C34" s="2">
-        <v>3.349</v>
+        <v>4.832</v>
       </c>
       <c r="D34" s="2">
-        <v>121.707780489039</v>
+        <v>114.030713389815</v>
       </c>
       <c r="E34" s="2">
-        <v>4.181</v>
+        <v>3.833</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -2349,13 +2385,13 @@
         <v>72</v>
       </c>
       <c r="C35" s="2">
-        <v>3.099</v>
+        <v>4.816</v>
       </c>
       <c r="D35" s="2">
-        <v>121.872589594197</v>
+        <v>123.673960726705</v>
       </c>
       <c r="E35" s="2">
-        <v>4.225</v>
+        <v>3.351</v>
       </c>
       <c r="I35" s="3"/>
     </row>
@@ -2367,13 +2403,13 @@
         <v>74</v>
       </c>
       <c r="C36" s="2">
-        <v>4.108</v>
+        <v>3.996</v>
       </c>
       <c r="D36" s="2">
-        <v>119.127875078096</v>
+        <v>117.557892537642</v>
       </c>
       <c r="E36" s="2">
-        <v>4.989</v>
+        <v>1.836</v>
       </c>
       <c r="I36" s="3"/>
     </row>
@@ -2385,13 +2421,13 @@
         <v>76</v>
       </c>
       <c r="C37" s="2">
-        <v>4.4</v>
+        <v>3.28</v>
       </c>
       <c r="D37" s="2">
-        <v>114.747335178202</v>
+        <v>119.802658367722</v>
       </c>
       <c r="E37" s="2">
-        <v>3.929</v>
+        <v>4.918</v>
       </c>
       <c r="I37" s="3"/>
     </row>
@@ -2403,13 +2439,13 @@
         <v>78</v>
       </c>
       <c r="C38" s="2">
-        <v>3.792</v>
+        <v>4.8</v>
       </c>
       <c r="D38" s="2">
-        <v>119.92667603852</v>
+        <v>120.421736968986</v>
       </c>
       <c r="E38" s="2">
-        <v>3.707</v>
+        <v>4.734</v>
       </c>
       <c r="I38" s="3"/>
     </row>
@@ -2421,13 +2457,13 @@
         <v>80</v>
       </c>
       <c r="C39" s="2">
-        <v>3.702</v>
+        <v>3.582</v>
       </c>
       <c r="D39" s="2">
-        <v>124.656617458662</v>
+        <v>120.136274739134</v>
       </c>
       <c r="E39" s="2">
-        <v>4.926</v>
+        <v>1.786</v>
       </c>
       <c r="I39" s="3"/>
     </row>
@@ -2439,13 +2475,13 @@
         <v>82</v>
       </c>
       <c r="C40" s="2">
-        <v>3.206</v>
+        <v>4.049</v>
       </c>
       <c r="D40" s="2">
-        <v>120.994691857841</v>
+        <v>119.585275320747</v>
       </c>
       <c r="E40" s="2">
-        <v>3.641</v>
+        <v>2.608</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2456,13 +2492,13 @@
         <v>84</v>
       </c>
       <c r="C41" s="2">
-        <v>3.796</v>
+        <v>3.999</v>
       </c>
       <c r="D41" s="2">
-        <v>115.770386408473</v>
+        <v>118.862294772648</v>
       </c>
       <c r="E41" s="2">
-        <v>2.545</v>
+        <v>3.767</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2473,13 +2509,13 @@
         <v>86</v>
       </c>
       <c r="C42" s="2">
-        <v>2.494</v>
+        <v>4.997</v>
       </c>
       <c r="D42" s="2">
-        <v>119.301157800161</v>
+        <v>121.015193060988</v>
       </c>
       <c r="E42" s="2">
-        <v>2.63</v>
+        <v>3.795</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2490,13 +2526,13 @@
         <v>88</v>
       </c>
       <c r="C43" s="2">
-        <v>3.199</v>
+        <v>3.206</v>
       </c>
       <c r="D43" s="2">
-        <v>120.410194893312</v>
+        <v>121.0878111331</v>
       </c>
       <c r="E43" s="2">
-        <v>4.625</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2507,13 +2543,13 @@
         <v>90</v>
       </c>
       <c r="C44" s="2">
-        <v>4.999</v>
+        <v>3.479</v>
       </c>
       <c r="D44" s="2">
-        <v>119.914573240918</v>
+        <v>117.582911023669</v>
       </c>
       <c r="E44" s="2">
-        <v>3.669</v>
+        <v>4.534</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2524,13 +2560,13 @@
         <v>92</v>
       </c>
       <c r="C45" s="2">
-        <v>3.008</v>
+        <v>4.766</v>
       </c>
       <c r="D45" s="2">
-        <v>119.500412639553</v>
+        <v>113.576966152539</v>
       </c>
       <c r="E45" s="2">
-        <v>2.392</v>
+        <v>2.323</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2541,13 +2577,13 @@
         <v>94</v>
       </c>
       <c r="C46" s="2">
-        <v>4.832</v>
+        <v>2.594</v>
       </c>
       <c r="D46" s="2">
-        <v>113.950588538005</v>
+        <v>114.339099738894</v>
       </c>
       <c r="E46" s="2">
-        <v>3.984</v>
+        <v>1.827</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2558,13 +2594,13 @@
         <v>96</v>
       </c>
       <c r="C47" s="2">
-        <v>3.996</v>
+        <v>3.998</v>
       </c>
       <c r="D47" s="2">
-        <v>117.516597398666</v>
+        <v>121.308203140594</v>
       </c>
       <c r="E47" s="2">
-        <v>1.986</v>
+        <v>4.841</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2575,13 +2611,13 @@
         <v>98</v>
       </c>
       <c r="C48" s="2">
-        <v>3.999</v>
+        <v>4.55</v>
       </c>
       <c r="D48" s="2">
-        <v>118.753398185329</v>
+        <v>118.539174980061</v>
       </c>
       <c r="E48" s="2">
-        <v>3.918</v>
+        <v>4.869</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2592,13 +2628,13 @@
         <v>100</v>
       </c>
       <c r="C49" s="2">
-        <v>2.485</v>
+        <v>4.595</v>
       </c>
       <c r="D49" s="2">
-        <v>126.953252870585</v>
+        <v>119.308251239962</v>
       </c>
       <c r="E49" s="2">
-        <v>2.488</v>
+        <v>2.534</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2609,13 +2645,13 @@
         <v>102</v>
       </c>
       <c r="C50" s="2">
-        <v>4.583</v>
+        <v>4.4</v>
       </c>
       <c r="D50" s="2">
-        <v>111.882224438656</v>
+        <v>114.724305538494</v>
       </c>
       <c r="E50" s="2">
-        <v>1.589</v>
+        <v>3.778</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2626,13 +2662,13 @@
         <v>104</v>
       </c>
       <c r="C51" s="2">
-        <v>3.959</v>
+        <v>3.87</v>
       </c>
       <c r="D51" s="2">
-        <v>119.881408313058</v>
+        <v>121.016176556364</v>
       </c>
       <c r="E51" s="2">
-        <v>3.743</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2643,13 +2679,13 @@
         <v>106</v>
       </c>
       <c r="C52" s="2">
-        <v>2.393</v>
+        <v>3.008</v>
       </c>
       <c r="D52" s="2">
-        <v>119.242482416096</v>
+        <v>119.533948097199</v>
       </c>
       <c r="E52" s="2">
-        <v>2.148</v>
+        <v>2.241</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2660,13 +2696,13 @@
         <v>108</v>
       </c>
       <c r="C53" s="2">
-        <v>4.997</v>
+        <v>2.485</v>
       </c>
       <c r="D53" s="2">
-        <v>120.839359148641</v>
+        <v>127.005382064305</v>
       </c>
       <c r="E53" s="2">
-        <v>3.945</v>
+        <v>2.337</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2677,13 +2713,13 @@
         <v>110</v>
       </c>
       <c r="C54" s="2">
-        <v>2.943</v>
+        <v>3.8</v>
       </c>
       <c r="D54" s="2">
-        <v>119.437683345423</v>
+        <v>120.289832656383</v>
       </c>
       <c r="E54" s="2">
-        <v>4.178</v>
+        <v>4.778</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2694,13 +2730,13 @@
         <v>112</v>
       </c>
       <c r="C55" s="2">
-        <v>4.8</v>
+        <v>2.979</v>
       </c>
       <c r="D55" s="2">
-        <v>120.211664461952</v>
+        <v>120.632104328997</v>
       </c>
       <c r="E55" s="2">
-        <v>4.885</v>
+        <v>1.863</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2711,13 +2747,13 @@
         <v>114</v>
       </c>
       <c r="C56" s="2">
-        <v>2.494</v>
+        <v>2.17</v>
       </c>
       <c r="D56" s="2">
-        <v>120.607254119345</v>
+        <v>114.096365664895</v>
       </c>
       <c r="E56" s="2">
-        <v>1.992</v>
+        <v>1.567</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2728,13 +2764,13 @@
         <v>116</v>
       </c>
       <c r="C57" s="2">
-        <v>3.907</v>
+        <v>2.188</v>
       </c>
       <c r="D57" s="2">
-        <v>120.597598214028</v>
+        <v>117.635014303159</v>
       </c>
       <c r="E57" s="2">
-        <v>1.973</v>
+        <v>1.962</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2745,13 +2781,13 @@
         <v>118</v>
       </c>
       <c r="C58" s="2">
-        <v>4.595</v>
+        <v>3.493</v>
       </c>
       <c r="D58" s="2">
-        <v>119.225267349452</v>
+        <v>121.597559196743</v>
       </c>
       <c r="E58" s="2">
-        <v>2.685</v>
+        <v>4.775</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2762,13 +2798,13 @@
         <v>120</v>
       </c>
       <c r="C59" s="2">
-        <v>3.399</v>
+        <v>2.943</v>
       </c>
       <c r="D59" s="2">
-        <v>121.246044988638</v>
+        <v>119.493960573303</v>
       </c>
       <c r="E59" s="2">
-        <v>4.397</v>
+        <v>4.027</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2779,13 +2815,13 @@
         <v>122</v>
       </c>
       <c r="C60" s="2">
-        <v>2.98</v>
+        <v>3.796</v>
       </c>
       <c r="D60" s="2">
-        <v>122.514382635828</v>
+        <v>121.298455309072</v>
       </c>
       <c r="E60" s="2">
-        <v>2.014</v>
+        <v>4.896</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2796,13 +2832,13 @@
         <v>124</v>
       </c>
       <c r="C61" s="2">
-        <v>4.599</v>
+        <v>4.108</v>
       </c>
       <c r="D61" s="2">
-        <v>120.270744355804</v>
+        <v>119.012829695811</v>
       </c>
       <c r="E61" s="2">
-        <v>4.943</v>
+        <v>4.838</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2813,13 +2849,13 @@
         <v>126</v>
       </c>
       <c r="C62" s="2">
-        <v>3.479</v>
+        <v>3.987</v>
       </c>
       <c r="D62" s="2">
-        <v>117.317964714839</v>
+        <v>119.472423627537</v>
       </c>
       <c r="E62" s="2">
-        <v>4.685</v>
+        <v>2.266</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2830,13 +2866,13 @@
         <v>128</v>
       </c>
       <c r="C63" s="2">
-        <v>4.53</v>
+        <v>4.497</v>
       </c>
       <c r="D63" s="2">
-        <v>111.860117290198</v>
+        <v>115.097615129435</v>
       </c>
       <c r="E63" s="2">
-        <v>1.551</v>
+        <v>1.863</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2847,13 +2883,13 @@
         <v>130</v>
       </c>
       <c r="C64" s="2">
-        <v>3.87</v>
+        <v>2.493</v>
       </c>
       <c r="D64" s="2">
-        <v>120.836165732451</v>
+        <v>120.614959401426</v>
       </c>
       <c r="E64" s="2">
-        <v>3.641</v>
+        <v>1.841</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2864,13 +2900,13 @@
         <v>132</v>
       </c>
       <c r="C65" s="2">
-        <v>4.999</v>
+        <v>3.996</v>
       </c>
       <c r="D65" s="2">
-        <v>120.845119251914</v>
+        <v>121.543136064874</v>
       </c>
       <c r="E65" s="2">
-        <v>3.948</v>
+        <v>4.638</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2881,13 +2917,13 @@
         <v>134</v>
       </c>
       <c r="C66" s="2">
-        <v>4.816</v>
+        <v>3.754</v>
       </c>
       <c r="D66" s="2">
-        <v>123.401601873188</v>
+        <v>116.628954345567</v>
       </c>
       <c r="E66" s="2">
-        <v>3.501</v>
+        <v>3.148</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2898,13 +2934,13 @@
         <v>136</v>
       </c>
       <c r="C67" s="2">
-        <v>2.594</v>
+        <v>3.796</v>
       </c>
       <c r="D67" s="2">
-        <v>114.276278218371</v>
+        <v>115.722571804392</v>
       </c>
       <c r="E67" s="2">
-        <v>1.978</v>
+        <v>2.395</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2915,13 +2951,13 @@
         <v>138</v>
       </c>
       <c r="C68" s="2">
-        <v>3.996</v>
+        <v>2.922</v>
       </c>
       <c r="D68" s="2">
-        <v>121.376231463858</v>
+        <v>123.929111269627</v>
       </c>
       <c r="E68" s="2">
-        <v>4.789</v>
+        <v>3.841</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2932,13 +2968,13 @@
         <v>140</v>
       </c>
       <c r="C69" s="2">
-        <v>2.188</v>
+        <v>3.977</v>
       </c>
       <c r="D69" s="2">
-        <v>119.511478905221</v>
+        <v>117.765668316562</v>
       </c>
       <c r="E69" s="2">
-        <v>2.112</v>
+        <v>4.167</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2949,13 +2985,13 @@
         <v>142</v>
       </c>
       <c r="C70" s="2">
-        <v>3.838</v>
+        <v>4.42</v>
       </c>
       <c r="D70" s="2">
-        <v>119.386047643886</v>
+        <v>118.086261212321</v>
       </c>
       <c r="E70" s="2">
-        <v>4.277</v>
+        <v>4.984</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2966,13 +3002,13 @@
         <v>144</v>
       </c>
       <c r="C71" s="2">
-        <v>2.922</v>
+        <v>4.526</v>
       </c>
       <c r="D71" s="2">
-        <v>123.777935487733</v>
+        <v>121.159168522177</v>
       </c>
       <c r="E71" s="2">
-        <v>3.992</v>
+        <v>4.545</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2983,13 +3019,13 @@
         <v>146</v>
       </c>
       <c r="C72" s="2">
-        <v>3.8</v>
+        <v>2.393</v>
       </c>
       <c r="D72" s="2">
-        <v>120.090583673904</v>
+        <v>117.609748859284</v>
       </c>
       <c r="E72" s="2">
-        <v>4.929</v>
+        <v>1.997</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3000,13 +3036,13 @@
         <v>148</v>
       </c>
       <c r="C73" s="2">
-        <v>3.875</v>
+        <v>3.399</v>
       </c>
       <c r="D73" s="2">
-        <v>121.089713427463</v>
+        <v>121.241500027048</v>
       </c>
       <c r="E73" s="2">
-        <v>1.63</v>
+        <v>4.247</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3017,13 +3053,13 @@
         <v>150</v>
       </c>
       <c r="C74" s="2">
-        <v>3.977</v>
+        <v>2.422</v>
       </c>
       <c r="D74" s="2">
-        <v>117.617693839993</v>
+        <v>121.413665958494</v>
       </c>
       <c r="E74" s="2">
-        <v>4.318</v>
+        <v>4.285</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3034,13 +3070,13 @@
         <v>152</v>
       </c>
       <c r="C75" s="2">
-        <v>2.265</v>
+        <v>4.599</v>
       </c>
       <c r="D75" s="2">
-        <v>122.459410441503</v>
+        <v>120.246130347484</v>
       </c>
       <c r="E75" s="2">
-        <v>2.704</v>
+        <v>4.792</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3051,13 +3087,13 @@
         <v>154</v>
       </c>
       <c r="C76" s="2">
-        <v>2.037</v>
+        <v>2.395</v>
       </c>
       <c r="D76" s="2">
-        <v>120.200477322264</v>
+        <v>120.829927621097</v>
       </c>
       <c r="E76" s="2">
-        <v>3.619</v>
+        <v>3.455</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3068,13 +3104,13 @@
         <v>156</v>
       </c>
       <c r="C77" s="2">
-        <v>2.395</v>
+        <v>3.1</v>
       </c>
       <c r="D77" s="2">
-        <v>120.731920614589</v>
+        <v>115.117734168219</v>
       </c>
       <c r="E77" s="2">
-        <v>3.606</v>
+        <v>4.811</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3085,13 +3121,13 @@
         <v>158</v>
       </c>
       <c r="C78" s="2">
-        <v>2.422</v>
+        <v>2.265</v>
       </c>
       <c r="D78" s="2">
-        <v>121.286027529783</v>
+        <v>122.492791946295</v>
       </c>
       <c r="E78" s="2">
-        <v>4.436</v>
+        <v>2.553</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3102,13 +3138,13 @@
         <v>160</v>
       </c>
       <c r="C79" s="2">
-        <v>3.057</v>
+        <v>3.587</v>
       </c>
       <c r="D79" s="2">
-        <v>119.121469453199</v>
+        <v>119.189483467087</v>
       </c>
       <c r="E79" s="2">
-        <v>2.408</v>
+        <v>2.241</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3119,13 +3155,13 @@
         <v>162</v>
       </c>
       <c r="C80" s="2">
-        <v>2.752</v>
+        <v>4.617</v>
       </c>
       <c r="D80" s="2">
-        <v>119.121431073247</v>
+        <v>119.022156967572</v>
       </c>
       <c r="E80" s="2">
-        <v>2.016</v>
+        <v>4.849</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3136,13 +3172,13 @@
         <v>164</v>
       </c>
       <c r="C81" s="2">
-        <v>4.617</v>
+        <v>4.649</v>
       </c>
       <c r="D81" s="2">
-        <v>118.92205167884</v>
+        <v>120.287565229992</v>
       </c>
       <c r="E81" s="2">
-        <v>5</v>
+        <v>3.296</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3153,13 +3189,13 @@
         <v>166</v>
       </c>
       <c r="C82" s="2">
-        <v>1.941</v>
+        <v>4.629</v>
       </c>
       <c r="D82" s="2">
-        <v>116.997323943873</v>
+        <v>120.857488984724</v>
       </c>
       <c r="E82" s="2">
-        <v>3.28</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3173,10 +3209,10 @@
         <v>3.686</v>
       </c>
       <c r="D83" s="2">
-        <v>120.408616149615</v>
+        <v>120.507018057831</v>
       </c>
       <c r="E83" s="2">
-        <v>4.622</v>
+        <v>4.471</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3187,13 +3223,13 @@
         <v>170</v>
       </c>
       <c r="C84" s="2">
-        <v>3.745</v>
+        <v>2.037</v>
       </c>
       <c r="D84" s="2">
-        <v>120.550865351382</v>
+        <v>120.253460904419</v>
       </c>
       <c r="E84" s="2">
-        <v>1.721</v>
+        <v>3.469</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3204,13 +3240,13 @@
         <v>172</v>
       </c>
       <c r="C85" s="2">
-        <v>2.497</v>
+        <v>1.941</v>
       </c>
       <c r="D85" s="2">
-        <v>121.022824540719</v>
+        <v>117.056607456549</v>
       </c>
       <c r="E85" s="2">
-        <v>4.989</v>
+        <v>3.129</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -3221,13 +3257,13 @@
         <v>174</v>
       </c>
       <c r="C86" s="2">
-        <v>4.499</v>
+        <v>2.685</v>
       </c>
       <c r="D86" s="2">
-        <v>116.982269258806</v>
+        <v>121.472654138577</v>
       </c>
       <c r="E86" s="2">
-        <v>4.164</v>
+        <v>4.299</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -3238,13 +3274,13 @@
         <v>176</v>
       </c>
       <c r="C87" s="2">
-        <v>2.993</v>
+        <v>3.907</v>
       </c>
       <c r="D87" s="2">
-        <v>118.061805113147</v>
+        <v>120.573959406638</v>
       </c>
       <c r="E87" s="2">
-        <v>1.937</v>
+        <v>1.822</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3255,13 +3291,13 @@
         <v>178</v>
       </c>
       <c r="C88" s="2">
-        <v>4.629</v>
+        <v>3</v>
       </c>
       <c r="D88" s="2">
-        <v>120.688558835438</v>
+        <v>116.569567145003</v>
       </c>
       <c r="E88" s="2">
-        <v>4.89</v>
+        <v>4.986</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -3272,13 +3308,13 @@
         <v>180</v>
       </c>
       <c r="C89" s="2">
-        <v>3.754</v>
+        <v>3.056</v>
       </c>
       <c r="D89" s="2">
-        <v>116.450598285732</v>
+        <v>119.164916156829</v>
       </c>
       <c r="E89" s="2">
-        <v>3.299</v>
+        <v>2.258</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -3289,13 +3325,13 @@
         <v>182</v>
       </c>
       <c r="C90" s="2">
-        <v>2.685</v>
+        <v>2.493</v>
       </c>
       <c r="D90" s="2">
-        <v>121.312541031374</v>
+        <v>119.17329951534</v>
       </c>
       <c r="E90" s="2">
-        <v>4.449</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -3306,13 +3342,13 @@
         <v>184</v>
       </c>
       <c r="C91" s="2">
-        <v>1.731</v>
+        <v>3.999</v>
       </c>
       <c r="D91" s="2">
-        <v>119.408567729162</v>
+        <v>117.083424336633</v>
       </c>
       <c r="E91" s="2">
-        <v>2.458</v>
+        <v>4.841</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -3323,13 +3359,13 @@
         <v>186</v>
       </c>
       <c r="C92" s="2">
-        <v>4.499</v>
+        <v>3.838</v>
       </c>
       <c r="D92" s="2">
-        <v>120.781919860934</v>
+        <v>119.293046463697</v>
       </c>
       <c r="E92" s="2">
-        <v>4.367</v>
+        <v>4.126</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -3340,13 +3376,13 @@
         <v>188</v>
       </c>
       <c r="C93" s="2">
-        <v>4.999</v>
+        <v>4.499</v>
       </c>
       <c r="D93" s="2">
-        <v>117.862505660231</v>
+        <v>120.873071827628</v>
       </c>
       <c r="E93" s="2">
-        <v>4.34</v>
+        <v>4.216</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3357,13 +3393,13 @@
         <v>190</v>
       </c>
       <c r="C94" s="2">
-        <v>2.435</v>
+        <v>2.877</v>
       </c>
       <c r="D94" s="2">
-        <v>120.023454529324</v>
+        <v>109.840257690136</v>
       </c>
       <c r="E94" s="2">
-        <v>4.606</v>
+        <v>1.932</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3374,13 +3410,13 @@
         <v>192</v>
       </c>
       <c r="C95" s="2">
-        <v>4.526</v>
+        <v>4.121</v>
       </c>
       <c r="D95" s="2">
-        <v>120.861778472075</v>
+        <v>123.239918045712</v>
       </c>
       <c r="E95" s="2">
-        <v>4.696</v>
+        <v>4.792</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3391,13 +3427,13 @@
         <v>194</v>
       </c>
       <c r="C96" s="2">
-        <v>4.121</v>
+        <v>4.732</v>
       </c>
       <c r="D96" s="2">
-        <v>123.147162260782</v>
+        <v>116.322392680284</v>
       </c>
       <c r="E96" s="2">
-        <v>4.943</v>
+        <v>4.458</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -3408,13 +3444,13 @@
         <v>196</v>
       </c>
       <c r="C97" s="2">
-        <v>3.199</v>
+        <v>4.499</v>
       </c>
       <c r="D97" s="2">
-        <v>113.113607465955</v>
+        <v>117.008003456406</v>
       </c>
       <c r="E97" s="2">
-        <v>4.885</v>
+        <v>4.014</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -3425,13 +3461,13 @@
         <v>198</v>
       </c>
       <c r="C98" s="2">
-        <v>3.1</v>
+        <v>4.984</v>
       </c>
       <c r="D98" s="2">
-        <v>114.895735571827</v>
+        <v>115.413230509748</v>
       </c>
       <c r="E98" s="2">
-        <v>4.962</v>
+        <v>2.258</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -3442,13 +3478,13 @@
         <v>200</v>
       </c>
       <c r="C99" s="2">
-        <v>3.493</v>
+        <v>3.198</v>
       </c>
       <c r="D99" s="2">
-        <v>121.109808605122</v>
+        <v>113.22572045815</v>
       </c>
       <c r="E99" s="2">
-        <v>4.926</v>
+        <v>4.734</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -3459,13 +3495,13 @@
         <v>202</v>
       </c>
       <c r="C100" s="2">
-        <v>4.949</v>
+        <v>2.497</v>
       </c>
       <c r="D100" s="2">
-        <v>112.065988700128</v>
+        <v>121.017100596646</v>
       </c>
       <c r="E100" s="2">
-        <v>4.08</v>
+        <v>4.838</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3476,13 +3512,13 @@
         <v>204</v>
       </c>
       <c r="C101" s="2">
-        <v>4.649</v>
+        <v>2.698</v>
       </c>
       <c r="D101" s="2">
-        <v>120.077828881287</v>
+        <v>120.555776440934</v>
       </c>
       <c r="E101" s="2">
-        <v>3.447</v>
+        <v>1.578</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -3493,13 +3529,13 @@
         <v>206</v>
       </c>
       <c r="C102" s="2">
-        <v>2.698</v>
+        <v>3.745</v>
       </c>
       <c r="D102" s="2">
-        <v>120.520616336272</v>
+        <v>120.538491444256</v>
       </c>
       <c r="E102" s="2">
-        <v>1.729</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -3510,13 +3546,13 @@
         <v>208</v>
       </c>
       <c r="C103" s="2">
-        <v>3.587</v>
+        <v>4.994</v>
       </c>
       <c r="D103" s="2">
-        <v>119.058553600342</v>
+        <v>112.964851271359</v>
       </c>
       <c r="E103" s="2">
-        <v>2.392</v>
+        <v>4.932</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -3527,13 +3563,13 @@
         <v>210</v>
       </c>
       <c r="C104" s="2">
-        <v>4.984</v>
+        <v>1.731</v>
       </c>
       <c r="D104" s="2">
-        <v>115.335764843196</v>
+        <v>119.399214169586</v>
       </c>
       <c r="E104" s="2">
-        <v>2.408</v>
+        <v>2.307</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -3544,13 +3580,13 @@
         <v>212</v>
       </c>
       <c r="C105" s="2">
-        <v>3.987</v>
+        <v>4.949</v>
       </c>
       <c r="D105" s="2">
-        <v>119.234298993093</v>
+        <v>111.788393058267</v>
       </c>
       <c r="E105" s="2">
-        <v>2.416</v>
+        <v>3.929</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -3561,13 +3597,13 @@
         <v>214</v>
       </c>
       <c r="C106" s="2">
-        <v>4.033</v>
+        <v>4.999</v>
       </c>
       <c r="D106" s="2">
-        <v>119.681658010405</v>
+        <v>117.833473695684</v>
       </c>
       <c r="E106" s="2">
-        <v>4.447</v>
+        <v>4.189</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -3578,13 +3614,13 @@
         <v>216</v>
       </c>
       <c r="C107" s="2">
-        <v>3.999</v>
+        <v>2.434</v>
       </c>
       <c r="D107" s="2">
-        <v>116.734230290772</v>
+        <v>120.00052843636</v>
       </c>
       <c r="E107" s="2">
-        <v>4.992</v>
+        <v>4.455</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -3595,13 +3631,13 @@
         <v>218</v>
       </c>
       <c r="C108" s="2">
-        <v>3.789</v>
+        <v>4.033</v>
       </c>
       <c r="D108" s="2">
-        <v>109.765950710178</v>
+        <v>119.799709227071</v>
       </c>
       <c r="E108" s="2">
-        <v>1.71</v>
+        <v>4.296</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -3612,13 +3648,13 @@
         <v>220</v>
       </c>
       <c r="C109" s="2">
-        <v>2.877</v>
+        <v>2.15</v>
       </c>
       <c r="D109" s="2">
-        <v>111.216503636193</v>
+        <v>118.554611017439</v>
       </c>
       <c r="E109" s="2">
-        <v>2.082</v>
+        <v>4.855</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -3629,13 +3665,13 @@
         <v>222</v>
       </c>
       <c r="C110" s="2">
-        <v>2.081</v>
+        <v>2.796</v>
       </c>
       <c r="D110" s="2">
-        <v>112.148288444422</v>
+        <v>120.739732347392</v>
       </c>
       <c r="E110" s="2">
-        <v>1.682</v>
+        <v>4.285</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -3646,13 +3682,13 @@
         <v>224</v>
       </c>
       <c r="C111" s="2">
-        <v>4.063</v>
+        <v>2.497</v>
       </c>
       <c r="D111" s="2">
-        <v>111.19715142832</v>
+        <v>117.717166233772</v>
       </c>
       <c r="E111" s="2">
-        <v>2.449</v>
+        <v>4.027</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -3663,13 +3699,13 @@
         <v>226</v>
       </c>
       <c r="C112" s="2">
-        <v>1.777</v>
+        <v>4.998</v>
       </c>
       <c r="D112" s="2">
-        <v>114.425758726076</v>
+        <v>119.758486957905</v>
       </c>
       <c r="E112" s="2">
-        <v>1.721</v>
+        <v>4.975</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -3680,50 +3716,116 @@
         <v>228</v>
       </c>
       <c r="C113" s="2">
-        <v>2.968</v>
+        <v>4.063</v>
       </c>
       <c r="D113" s="2">
-        <v>110.708685930883</v>
+        <v>111.279221508725</v>
       </c>
       <c r="E113" s="2">
-        <v>1.896</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="4"/>
-      <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
+        <v>2.299</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C114" s="2">
+        <v>2.987</v>
+      </c>
+      <c r="D114" s="2">
+        <v>117.975612619989</v>
+      </c>
+      <c r="E114" s="2">
+        <v>1.786</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C115" s="2">
+        <v>4.172</v>
+      </c>
+      <c r="D115" s="2">
+        <v>111.782178377749</v>
+      </c>
+      <c r="E115" s="2">
+        <v>1.688</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C116" s="2">
+        <v>1.777</v>
+      </c>
+      <c r="D116" s="2">
+        <v>114.449218846686</v>
+      </c>
+      <c r="E116" s="2">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C117" s="2">
+        <v>2.081</v>
+      </c>
+      <c r="D117" s="2">
+        <v>112.148205085326</v>
+      </c>
+      <c r="E117" s="2">
+        <v>1.532</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C118" s="2">
+        <v>3.789</v>
+      </c>
+      <c r="D118" s="2">
+        <v>109.72019903934</v>
+      </c>
+      <c r="E118" s="2">
+        <v>1.559</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C119" s="2">
+        <v>2.966</v>
+      </c>
+      <c r="D119" s="2">
+        <v>110.711996964702</v>
+      </c>
+      <c r="E119" s="2">
+        <v>1.745</v>
+      </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4"/>

</xml_diff>